<commit_message>
Change Host Tmp Failure bits to binary conversion and change text a bit
</commit_message>
<xml_diff>
--- a/genSpacecraft/DownlinkSpecLTM.xlsx
+++ b/genSpacecraft/DownlinkSpecLTM.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1394" uniqueCount="514">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1394" uniqueCount="515">
   <si>
     <t xml:space="preserve">//</t>
   </si>
@@ -851,12 +851,18 @@
     <t xml:space="preserve">Number of software commands since last reset</t>
   </si>
   <si>
-    <t xml:space="preserve">I2c Fail Host Temp</t>
+    <t xml:space="preserve">Host Tmp Fail</t>
   </si>
   <si>
     <t xml:space="preserve">I2CfailureHostTemp</t>
   </si>
   <si>
+    <t xml:space="preserve">BIN5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bits</t>
+  </si>
+  <si>
     <t xml:space="preserve">Bits Indicate Host Temp Sensor Failure</t>
   </si>
   <si>
@@ -1533,9 +1539,6 @@
   </si>
   <si>
     <t xml:space="preserve">Total Bytes per Frame</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bits</t>
   </si>
   <si>
     <t xml:space="preserve">Time to Downlink</t>
@@ -1940,8 +1943,8 @@
   </sheetPr>
   <dimension ref="A1:Q263"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A106" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G123" activeCellId="0" sqref="G123"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A88" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B104" activeCellId="0" sqref="B104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6538,13 +6541,13 @@
       </c>
       <c r="F104" s="23"/>
       <c r="G104" s="23" t="s">
-        <v>133</v>
+        <v>278</v>
       </c>
       <c r="H104" s="22" t="s">
-        <v>27</v>
+        <v>279</v>
       </c>
       <c r="I104" s="23" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="J104" s="29" t="n">
         <f aca="false">J103+D103</f>
@@ -6577,10 +6580,10 @@
     </row>
     <row r="105" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B105" s="31" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="C105" s="32" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="D105" s="32" t="n">
         <v>1</v>
@@ -6590,13 +6593,13 @@
       </c>
       <c r="F105" s="23"/>
       <c r="G105" s="22" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="H105" s="22" t="s">
         <v>27</v>
       </c>
       <c r="I105" s="32" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="J105" s="29" t="n">
         <f aca="false">J104+D104</f>
@@ -6629,10 +6632,10 @@
     </row>
     <row r="106" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B106" s="31" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="C106" s="32" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="D106" s="32" t="n">
         <v>1</v>
@@ -6642,7 +6645,7 @@
       </c>
       <c r="F106" s="23"/>
       <c r="G106" s="22" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="H106" s="22" t="s">
         <v>27</v>
@@ -6679,10 +6682,10 @@
     </row>
     <row r="107" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B107" s="31" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="C107" s="32" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="D107" s="32" t="n">
         <v>1</v>
@@ -6692,7 +6695,7 @@
       </c>
       <c r="F107" s="23"/>
       <c r="G107" s="22" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="H107" s="22" t="s">
         <v>27</v>
@@ -6729,10 +6732,10 @@
     </row>
     <row r="108" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B108" s="31" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="C108" s="32" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="D108" s="32" t="n">
         <v>1</v>
@@ -6742,7 +6745,7 @@
       </c>
       <c r="F108" s="23"/>
       <c r="G108" s="22" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="H108" s="22" t="s">
         <v>27</v>
@@ -6779,10 +6782,10 @@
     </row>
     <row r="109" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B109" s="31" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="C109" s="32" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="D109" s="32" t="n">
         <v>1</v>
@@ -6792,7 +6795,7 @@
       </c>
       <c r="F109" s="23"/>
       <c r="G109" s="22" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="H109" s="22" t="s">
         <v>27</v>
@@ -6815,7 +6818,7 @@
         <v>17.125</v>
       </c>
       <c r="N109" s="1" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="O109" s="24" t="n">
         <v>9</v>
@@ -6829,10 +6832,10 @@
     </row>
     <row r="110" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B110" s="31" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="C110" s="32" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="D110" s="32" t="n">
         <v>1</v>
@@ -6842,7 +6845,7 @@
       </c>
       <c r="F110" s="23"/>
       <c r="G110" s="22" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="H110" s="22" t="s">
         <v>27</v>
@@ -6865,7 +6868,7 @@
         <v>17.15625</v>
       </c>
       <c r="N110" s="1" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="O110" s="24" t="n">
         <v>9</v>
@@ -6879,10 +6882,10 @@
     </row>
     <row r="111" customFormat="false" ht="25.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B111" s="31" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="C111" s="32" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="D111" s="32" t="n">
         <v>1</v>
@@ -6892,7 +6895,7 @@
       </c>
       <c r="F111" s="23"/>
       <c r="G111" s="22" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="H111" s="22" t="s">
         <v>27</v>
@@ -6915,7 +6918,7 @@
         <v>17.1875</v>
       </c>
       <c r="N111" s="1" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="O111" s="24" t="n">
         <v>9</v>
@@ -6929,10 +6932,10 @@
     </row>
     <row r="112" customFormat="false" ht="25.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B112" s="31" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="C112" s="32" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="D112" s="32" t="n">
         <v>1</v>
@@ -6942,7 +6945,7 @@
       </c>
       <c r="F112" s="23"/>
       <c r="G112" s="22" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="H112" s="22" t="s">
         <v>27</v>
@@ -6965,7 +6968,7 @@
         <v>17.21875</v>
       </c>
       <c r="N112" s="1" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="O112" s="24" t="n">
         <v>9</v>
@@ -6979,10 +6982,10 @@
     </row>
     <row r="113" customFormat="false" ht="25.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B113" s="31" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="C113" s="32" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="D113" s="32" t="n">
         <v>1</v>
@@ -6992,13 +6995,13 @@
       </c>
       <c r="F113" s="23"/>
       <c r="G113" s="22" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="H113" s="22" t="s">
         <v>27</v>
       </c>
       <c r="I113" s="32" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="J113" s="29" t="n">
         <f aca="false">J112+D112</f>
@@ -7017,7 +7020,7 @@
         <v>17.25</v>
       </c>
       <c r="N113" s="1" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="O113" s="24" t="n">
         <v>9</v>
@@ -7031,10 +7034,10 @@
     </row>
     <row r="114" customFormat="false" ht="25.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B114" s="31" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="C114" s="32" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="D114" s="32" t="n">
         <v>1</v>
@@ -7044,7 +7047,7 @@
       </c>
       <c r="F114" s="23"/>
       <c r="G114" s="22" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="H114" s="22" t="s">
         <v>27</v>
@@ -7067,7 +7070,7 @@
         <v>17.28125</v>
       </c>
       <c r="N114" s="1" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="O114" s="24" t="n">
         <v>9</v>
@@ -7081,10 +7084,10 @@
     </row>
     <row r="115" customFormat="false" ht="25.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B115" s="31" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="C115" s="32" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="D115" s="32" t="n">
         <v>1</v>
@@ -7094,7 +7097,7 @@
       </c>
       <c r="F115" s="23"/>
       <c r="G115" s="22" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="H115" s="22" t="s">
         <v>27</v>
@@ -7117,7 +7120,7 @@
         <v>17.3125</v>
       </c>
       <c r="N115" s="1" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="O115" s="24" t="n">
         <v>9</v>
@@ -7131,10 +7134,10 @@
     </row>
     <row r="116" customFormat="false" ht="25.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B116" s="31" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="C116" s="32" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="D116" s="32" t="n">
         <v>1</v>
@@ -7144,7 +7147,7 @@
       </c>
       <c r="F116" s="23"/>
       <c r="G116" s="22" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="H116" s="22" t="s">
         <v>27</v>
@@ -7167,7 +7170,7 @@
         <v>17.34375</v>
       </c>
       <c r="N116" s="1" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="O116" s="24" t="n">
         <v>9</v>
@@ -7181,10 +7184,10 @@
     </row>
     <row r="117" customFormat="false" ht="25.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B117" s="31" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="C117" s="32" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="D117" s="32" t="n">
         <v>1</v>
@@ -7194,7 +7197,7 @@
       </c>
       <c r="F117" s="23"/>
       <c r="G117" s="22" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="H117" s="22" t="s">
         <v>27</v>
@@ -7217,7 +7220,7 @@
         <v>17.375</v>
       </c>
       <c r="N117" s="1" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="O117" s="24" t="n">
         <v>9</v>
@@ -7231,10 +7234,10 @@
     </row>
     <row r="118" customFormat="false" ht="25.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B118" s="31" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="C118" s="32" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="D118" s="32" t="n">
         <v>1</v>
@@ -7244,7 +7247,7 @@
       </c>
       <c r="F118" s="23"/>
       <c r="G118" s="22" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="H118" s="22" t="s">
         <v>27</v>
@@ -7267,7 +7270,7 @@
         <v>17.40625</v>
       </c>
       <c r="N118" s="1" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="O118" s="24" t="n">
         <v>9</v>
@@ -7281,10 +7284,10 @@
     </row>
     <row r="119" customFormat="false" ht="25.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B119" s="31" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="C119" s="32" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="D119" s="32" t="n">
         <v>1</v>
@@ -7294,7 +7297,7 @@
       </c>
       <c r="F119" s="23"/>
       <c r="G119" s="22" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="H119" s="22" t="s">
         <v>27</v>
@@ -7317,7 +7320,7 @@
         <v>17.4375</v>
       </c>
       <c r="N119" s="1" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="O119" s="24" t="n">
         <v>9</v>
@@ -7331,10 +7334,10 @@
     </row>
     <row r="120" customFormat="false" ht="25.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B120" s="31" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="C120" s="32" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="D120" s="32" t="n">
         <v>1</v>
@@ -7344,7 +7347,7 @@
       </c>
       <c r="F120" s="23"/>
       <c r="G120" s="22" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="H120" s="22" t="s">
         <v>27</v>
@@ -7367,7 +7370,7 @@
         <v>17.46875</v>
       </c>
       <c r="N120" s="1" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="O120" s="24" t="n">
         <v>9</v>
@@ -7381,10 +7384,10 @@
     </row>
     <row r="121" customFormat="false" ht="25.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B121" s="31" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="C121" s="32" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="D121" s="32" t="n">
         <v>1</v>
@@ -7394,13 +7397,13 @@
       </c>
       <c r="F121" s="23"/>
       <c r="G121" s="22" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="H121" s="22" t="s">
         <v>27</v>
       </c>
       <c r="I121" s="32" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="J121" s="29" t="n">
         <f aca="false">J120+D120</f>
@@ -7419,7 +7422,7 @@
         <v>17.5</v>
       </c>
       <c r="N121" s="1" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="O121" s="24" t="n">
         <v>9</v>
@@ -7433,10 +7436,10 @@
     </row>
     <row r="122" customFormat="false" ht="25.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B122" s="31" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="C122" s="32" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="D122" s="32" t="n">
         <v>1</v>
@@ -7446,7 +7449,7 @@
       </c>
       <c r="F122" s="23"/>
       <c r="G122" s="22" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="H122" s="22" t="s">
         <v>27</v>
@@ -7469,7 +7472,7 @@
         <v>17.53125</v>
       </c>
       <c r="N122" s="1" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="O122" s="24" t="n">
         <v>9</v>
@@ -7483,10 +7486,10 @@
     </row>
     <row r="123" customFormat="false" ht="25.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B123" s="31" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="C123" s="32" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="D123" s="32" t="n">
         <v>1</v>
@@ -7496,7 +7499,7 @@
       </c>
       <c r="F123" s="23"/>
       <c r="G123" s="22" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="H123" s="22" t="s">
         <v>27</v>
@@ -7519,7 +7522,7 @@
         <v>17.5625</v>
       </c>
       <c r="N123" s="1" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="O123" s="24" t="n">
         <v>9</v>
@@ -7533,10 +7536,10 @@
     </row>
     <row r="124" customFormat="false" ht="25.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B124" s="31" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="C124" s="32" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="D124" s="32" t="n">
         <v>1</v>
@@ -7546,7 +7549,7 @@
       </c>
       <c r="F124" s="23"/>
       <c r="G124" s="22" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="H124" s="22" t="s">
         <v>27</v>
@@ -7569,7 +7572,7 @@
         <v>17.59375</v>
       </c>
       <c r="N124" s="1" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="O124" s="24" t="n">
         <v>9</v>
@@ -7583,10 +7586,10 @@
     </row>
     <row r="125" customFormat="false" ht="25.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B125" s="31" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="C125" s="32" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="D125" s="32" t="n">
         <v>1</v>
@@ -7596,7 +7599,7 @@
       </c>
       <c r="F125" s="23"/>
       <c r="G125" s="22" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="H125" s="22" t="s">
         <v>27</v>
@@ -7619,7 +7622,7 @@
         <v>17.625</v>
       </c>
       <c r="N125" s="1" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="O125" s="24" t="n">
         <v>9</v>
@@ -7633,10 +7636,10 @@
     </row>
     <row r="126" customFormat="false" ht="25.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B126" s="31" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="C126" s="32" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="D126" s="32" t="n">
         <v>1</v>
@@ -7646,7 +7649,7 @@
       </c>
       <c r="F126" s="23"/>
       <c r="G126" s="22" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="H126" s="22" t="s">
         <v>27</v>
@@ -7669,7 +7672,7 @@
         <v>17.65625</v>
       </c>
       <c r="N126" s="1" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="O126" s="24" t="n">
         <v>9</v>
@@ -7683,10 +7686,10 @@
     </row>
     <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B127" s="31" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="C127" s="32" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="D127" s="32" t="n">
         <v>2</v>
@@ -7733,10 +7736,10 @@
     </row>
     <row r="128" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B128" s="31" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="C128" s="32" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="D128" s="32" t="n">
         <v>1</v>
@@ -7746,7 +7749,7 @@
       </c>
       <c r="F128" s="23"/>
       <c r="G128" s="22" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="H128" s="22" t="s">
         <v>27</v>
@@ -7783,10 +7786,10 @@
     </row>
     <row r="129" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B129" s="31" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="C129" s="32" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="D129" s="32" t="n">
         <v>1</v>
@@ -7796,7 +7799,7 @@
       </c>
       <c r="F129" s="23"/>
       <c r="G129" s="22" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="H129" s="22" t="s">
         <v>27</v>
@@ -7833,10 +7836,10 @@
     </row>
     <row r="130" customFormat="false" ht="25.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B130" s="31" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="C130" s="32" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="D130" s="32" t="n">
         <v>1</v>
@@ -7846,7 +7849,7 @@
       </c>
       <c r="F130" s="23"/>
       <c r="G130" s="22" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="H130" s="22" t="s">
         <v>27</v>
@@ -7883,10 +7886,10 @@
     </row>
     <row r="131" customFormat="false" ht="25.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B131" s="31" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="C131" s="32" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="D131" s="32" t="n">
         <v>1</v>
@@ -7896,7 +7899,7 @@
       </c>
       <c r="F131" s="23"/>
       <c r="G131" s="22" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="H131" s="22" t="s">
         <v>27</v>
@@ -7933,10 +7936,10 @@
     </row>
     <row r="132" customFormat="false" ht="25.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B132" s="31" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="C132" s="32" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="D132" s="32" t="n">
         <v>1</v>
@@ -7946,7 +7949,7 @@
       </c>
       <c r="F132" s="23"/>
       <c r="G132" s="22" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="H132" s="22"/>
       <c r="I132" s="32"/>
@@ -7967,7 +7970,7 @@
         <v>17.875</v>
       </c>
       <c r="N132" s="1" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="O132" s="24" t="n">
         <v>9</v>
@@ -7981,10 +7984,10 @@
     </row>
     <row r="133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B133" s="31" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="C133" s="32" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="D133" s="32" t="n">
         <v>3</v>
@@ -8031,10 +8034,10 @@
     </row>
     <row r="134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B134" s="31" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="C134" s="32" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="D134" s="32" t="n">
         <v>8</v>
@@ -8083,10 +8086,10 @@
     </row>
     <row r="135" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B135" s="31" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="C135" s="32" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="D135" s="32" t="n">
         <v>8</v>
@@ -8102,7 +8105,7 @@
         <v>27</v>
       </c>
       <c r="I135" s="23" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="J135" s="29" t="n">
         <f aca="false">J134+D134</f>
@@ -8135,10 +8138,10 @@
     </row>
     <row r="136" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B136" s="31" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="C136" s="32" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="D136" s="32" t="n">
         <v>8</v>
@@ -8154,7 +8157,7 @@
         <v>27</v>
       </c>
       <c r="I136" s="23" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="J136" s="29" t="n">
         <f aca="false">J135+D135</f>
@@ -8187,10 +8190,10 @@
     </row>
     <row r="137" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B137" s="31" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="C137" s="32" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="D137" s="32" t="n">
         <v>8</v>
@@ -8206,7 +8209,7 @@
         <v>27</v>
       </c>
       <c r="I137" s="23" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="J137" s="29" t="n">
         <f aca="false">J136+D136</f>
@@ -8239,10 +8242,10 @@
     </row>
     <row r="138" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B138" s="31" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="C138" s="32" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="D138" s="32" t="n">
         <v>8</v>
@@ -8258,7 +8261,7 @@
         <v>27</v>
       </c>
       <c r="I138" s="23" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="J138" s="29" t="n">
         <f aca="false">J137+D137</f>
@@ -8291,10 +8294,10 @@
     </row>
     <row r="139" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B139" s="31" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="C139" s="32" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="D139" s="32" t="n">
         <v>8</v>
@@ -8341,10 +8344,10 @@
     </row>
     <row r="140" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B140" s="31" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="C140" s="32" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="D140" s="32" t="n">
         <v>8</v>
@@ -8391,10 +8394,10 @@
     </row>
     <row r="141" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B141" s="31" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="C141" s="32" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="D141" s="32" t="n">
         <v>8</v>
@@ -8441,10 +8444,10 @@
     </row>
     <row r="142" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B142" s="31" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="C142" s="32" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="D142" s="32" t="n">
         <v>8</v>
@@ -8491,10 +8494,10 @@
     </row>
     <row r="143" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B143" s="31" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="C143" s="32" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="D143" s="32" t="n">
         <v>8</v>
@@ -8541,10 +8544,10 @@
     </row>
     <row r="144" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B144" s="31" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="C144" s="32" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="D144" s="32" t="n">
         <v>8</v>
@@ -8613,10 +8616,10 @@
     </row>
     <row r="146" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B146" s="31" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="C146" s="32" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="D146" s="32" t="n">
         <v>1</v>
@@ -8662,10 +8665,10 @@
     </row>
     <row r="147" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B147" s="31" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="C147" s="32" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="D147" s="32" t="n">
         <v>1</v>
@@ -8681,7 +8684,7 @@
         <v>27</v>
       </c>
       <c r="I147" s="23" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="J147" s="29" t="n">
         <f aca="false">J146+D146</f>
@@ -8714,10 +8717,10 @@
     </row>
     <row r="148" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B148" s="31" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="C148" s="32" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="D148" s="32" t="n">
         <v>3</v>
@@ -8727,7 +8730,7 @@
       </c>
       <c r="F148" s="23"/>
       <c r="G148" s="23" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="H148" s="22" t="s">
         <v>27</v>
@@ -8764,10 +8767,10 @@
     </row>
     <row r="149" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B149" s="31" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="C149" s="32" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="D149" s="32" t="n">
         <v>1</v>
@@ -8814,10 +8817,10 @@
     </row>
     <row r="150" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B150" s="31" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="C150" s="32" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="D150" s="32" t="n">
         <v>1</v>
@@ -8833,7 +8836,7 @@
         <v>27</v>
       </c>
       <c r="I150" s="23" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="J150" s="29" t="n">
         <f aca="false">J149+D149</f>
@@ -8866,10 +8869,10 @@
     </row>
     <row r="151" customFormat="false" ht="25.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B151" s="31" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="C151" s="32" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="D151" s="32" t="n">
         <v>1</v>
@@ -8885,7 +8888,7 @@
         <v>27</v>
       </c>
       <c r="I151" s="23" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="J151" s="29" t="n">
         <f aca="false">J150+D150</f>
@@ -8938,10 +8941,10 @@
     </row>
     <row r="153" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B153" s="31" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="C153" s="32" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="D153" s="32" t="n">
         <v>8</v>
@@ -8988,10 +8991,10 @@
     </row>
     <row r="154" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B154" s="31" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="C154" s="32" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="D154" s="32" t="n">
         <v>8</v>
@@ -9038,10 +9041,10 @@
     </row>
     <row r="155" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B155" s="31" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="C155" s="32" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="D155" s="32" t="n">
         <v>8</v>
@@ -9088,10 +9091,10 @@
     </row>
     <row r="156" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B156" s="31" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="C156" s="32" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="D156" s="32" t="n">
         <v>8</v>
@@ -9148,7 +9151,7 @@
       <c r="G157" s="36"/>
       <c r="H157" s="35"/>
       <c r="I157" s="36" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="J157" s="29" t="n">
         <f aca="false">J156+D156</f>
@@ -9175,7 +9178,7 @@
     </row>
     <row r="160" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="1" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="B160" s="31"/>
       <c r="C160" s="32"/>
@@ -9195,7 +9198,7 @@
         <v>57</v>
       </c>
       <c r="C161" s="32" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="D161" s="32" t="n">
         <v>32</v>
@@ -9253,7 +9256,7 @@
       <c r="G162" s="36"/>
       <c r="H162" s="35"/>
       <c r="I162" s="36" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="J162" s="29" t="n">
         <f aca="false">J161+D161</f>
@@ -9290,31 +9293,31 @@
     </row>
     <row r="164" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="1" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B165" s="31" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="C165" s="32" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="D165" s="27" t="n">
         <v>32</v>
       </c>
       <c r="E165" s="38" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="F165" s="23"/>
       <c r="G165" s="39" t="n">
         <v>1</v>
       </c>
       <c r="H165" s="3" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="I165" s="28" t="s">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="J165" s="29" t="n">
         <f aca="false">J83</f>
@@ -9333,7 +9336,7 @@
         <v>14</v>
       </c>
       <c r="N165" s="1" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="O165" s="3" t="n">
         <v>5</v>
@@ -9347,10 +9350,10 @@
     </row>
     <row r="166" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B166" s="31" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="C166" s="32" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="D166" s="27" t="n">
         <v>16</v>
@@ -9363,10 +9366,10 @@
         <v>1</v>
       </c>
       <c r="H166" s="3" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="I166" s="28" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="J166" s="29" t="n">
         <f aca="false">J165+D165</f>
@@ -9385,7 +9388,7 @@
         <v>15</v>
       </c>
       <c r="N166" s="1" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="O166" s="3" t="n">
         <v>5</v>
@@ -9399,16 +9402,16 @@
     </row>
     <row r="167" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B167" s="31" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="C167" s="32" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="D167" s="27" t="n">
         <v>8</v>
       </c>
       <c r="E167" s="38" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="F167" s="23"/>
       <c r="G167" s="22" t="n">
@@ -9418,7 +9421,7 @@
         <v>27</v>
       </c>
       <c r="I167" s="28" t="s">
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="J167" s="29" t="n">
         <f aca="false">J166+D166</f>
@@ -9437,7 +9440,7 @@
         <v>15.5</v>
       </c>
       <c r="N167" s="1" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="O167" s="3" t="n">
         <v>5</v>
@@ -9451,10 +9454,10 @@
     </row>
     <row r="168" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B168" s="31" t="s">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c r="C168" s="32" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="D168" s="27" t="n">
         <v>8</v>
@@ -9468,7 +9471,7 @@
         <v>27</v>
       </c>
       <c r="I168" s="28" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="J168" s="29" t="n">
         <f aca="false">J167+D167</f>
@@ -9510,7 +9513,7 @@
       <c r="G169" s="36"/>
       <c r="H169" s="35"/>
       <c r="I169" s="36" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="J169" s="29" t="n">
         <f aca="false">J168+D168</f>
@@ -9531,15 +9534,15 @@
     </row>
     <row r="172" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="1" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B173" s="31" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="C173" s="32" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="D173" s="27" t="n">
         <v>32</v>
@@ -9550,10 +9553,10 @@
         <v>1</v>
       </c>
       <c r="H173" s="3" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="I173" s="28" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="J173" s="29" t="n">
         <f aca="false">J83</f>
@@ -9572,7 +9575,7 @@
         <v>14</v>
       </c>
       <c r="N173" s="1" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="O173" s="3" t="n">
         <v>5</v>
@@ -9586,10 +9589,10 @@
     </row>
     <row r="174" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B174" s="31" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="C174" s="32" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="D174" s="27" t="n">
         <v>16</v>
@@ -9602,10 +9605,10 @@
         <v>1</v>
       </c>
       <c r="H174" s="3" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="I174" s="28" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="J174" s="29" t="n">
         <f aca="false">J173+D173</f>
@@ -9624,7 +9627,7 @@
         <v>15</v>
       </c>
       <c r="N174" s="1" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="O174" s="3" t="n">
         <v>5</v>
@@ -9638,10 +9641,10 @@
     </row>
     <row r="175" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B175" s="31" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="C175" s="32" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
       <c r="D175" s="27" t="n">
         <v>16</v>
@@ -9652,7 +9655,7 @@
         <v>1</v>
       </c>
       <c r="I175" s="28" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="J175" s="29" t="n">
         <f aca="false">J174+D174</f>
@@ -9671,7 +9674,7 @@
         <v>15.5</v>
       </c>
       <c r="N175" s="1" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="O175" s="3" t="n">
         <v>5</v>
@@ -9685,10 +9688,10 @@
     </row>
     <row r="176" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B176" s="31" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="C176" s="32" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="D176" s="27" t="n">
         <v>32</v>
@@ -9699,7 +9702,7 @@
         <v>1</v>
       </c>
       <c r="I176" s="28" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="J176" s="29" t="n">
         <f aca="false">J175+D175</f>
@@ -9718,7 +9721,7 @@
         <v>16</v>
       </c>
       <c r="N176" s="1" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="O176" s="3" t="n">
         <v>5</v>
@@ -9732,16 +9735,16 @@
     </row>
     <row r="177" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B177" s="31" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="C177" s="32" t="s">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="D177" s="27" t="n">
         <v>8</v>
       </c>
       <c r="E177" s="38" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="F177" s="23"/>
       <c r="G177" s="22" t="n">
@@ -9751,7 +9754,7 @@
         <v>27</v>
       </c>
       <c r="I177" s="28" t="s">
-        <v>407</v>
+        <v>409</v>
       </c>
       <c r="J177" s="29" t="n">
         <f aca="false">J176+D176</f>
@@ -9770,7 +9773,7 @@
         <v>17</v>
       </c>
       <c r="N177" s="1" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="O177" s="3" t="n">
         <v>5</v>
@@ -9784,10 +9787,10 @@
     </row>
     <row r="178" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B178" s="31" t="s">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c r="C178" s="32" t="s">
-        <v>408</v>
+        <v>410</v>
       </c>
       <c r="D178" s="27" t="n">
         <v>24</v>
@@ -9844,7 +9847,7 @@
       <c r="G179" s="36"/>
       <c r="H179" s="35"/>
       <c r="I179" s="36" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="J179" s="29" t="n">
         <f aca="false">J178+D178</f>
@@ -9870,15 +9873,15 @@
     </row>
     <row r="183" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="1" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B184" s="31" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="C184" s="32" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
       <c r="D184" s="27" t="n">
         <v>32</v>
@@ -9891,10 +9894,10 @@
         <v>1</v>
       </c>
       <c r="H184" s="39" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="I184" s="28" t="s">
-        <v>412</v>
+        <v>414</v>
       </c>
       <c r="J184" s="29" t="n">
         <f aca="false">J157</f>
@@ -9913,7 +9916,7 @@
         <v>22</v>
       </c>
       <c r="N184" s="1" t="s">
-        <v>413</v>
+        <v>415</v>
       </c>
       <c r="O184" s="3" t="n">
         <v>10</v>
@@ -9927,10 +9930,10 @@
     </row>
     <row r="185" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B185" s="31" t="s">
-        <v>414</v>
+        <v>416</v>
       </c>
       <c r="C185" s="32" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c r="D185" s="27" t="n">
         <v>16</v>
@@ -9946,7 +9949,7 @@
         <v>27</v>
       </c>
       <c r="I185" s="28" t="s">
-        <v>412</v>
+        <v>414</v>
       </c>
       <c r="J185" s="29" t="n">
         <f aca="false">J184+D184</f>
@@ -9965,7 +9968,7 @@
         <v>23</v>
       </c>
       <c r="N185" s="1" t="s">
-        <v>413</v>
+        <v>415</v>
       </c>
       <c r="O185" s="3" t="n">
         <v>10</v>
@@ -9979,10 +9982,10 @@
     </row>
     <row r="186" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B186" s="31" t="s">
-        <v>416</v>
+        <v>418</v>
       </c>
       <c r="C186" s="32" t="s">
-        <v>417</v>
+        <v>419</v>
       </c>
       <c r="D186" s="27" t="n">
         <v>8</v>
@@ -9998,7 +10001,7 @@
         <v>27</v>
       </c>
       <c r="I186" s="28" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="J186" s="29" t="n">
         <f aca="false">J185+D185</f>
@@ -10017,7 +10020,7 @@
         <v>23.5</v>
       </c>
       <c r="N186" s="5" t="s">
-        <v>413</v>
+        <v>415</v>
       </c>
       <c r="O186" s="24" t="n">
         <v>10</v>
@@ -10296,7 +10299,7 @@
     </row>
     <row r="194" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="40" t="s">
-        <v>419</v>
+        <v>421</v>
       </c>
       <c r="B194" s="11"/>
       <c r="C194" s="41"/>
@@ -10362,10 +10365,10 @@
     </row>
     <row r="196" customFormat="false" ht="37.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B196" s="31" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="C196" s="22" t="s">
-        <v>421</v>
+        <v>423</v>
       </c>
       <c r="D196" s="22" t="n">
         <v>5248</v>
@@ -10383,7 +10386,7 @@
         <v>27</v>
       </c>
       <c r="I196" s="23" t="s">
-        <v>422</v>
+        <v>424</v>
       </c>
       <c r="J196" s="4" t="n">
         <v>0</v>
@@ -10415,10 +10418,10 @@
     </row>
     <row r="197" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B197" s="31" t="s">
-        <v>423</v>
+        <v>425</v>
       </c>
       <c r="C197" s="22" t="s">
-        <v>424</v>
+        <v>426</v>
       </c>
       <c r="D197" s="22" t="n">
         <v>7</v>
@@ -10455,10 +10458,10 @@
     </row>
     <row r="198" customFormat="false" ht="25.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B198" s="31" t="s">
-        <v>425</v>
+        <v>427</v>
       </c>
       <c r="C198" s="22" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="D198" s="22" t="n">
         <v>1</v>
@@ -10472,7 +10475,7 @@
       </c>
       <c r="H198" s="22"/>
       <c r="I198" s="23" t="s">
-        <v>427</v>
+        <v>429</v>
       </c>
       <c r="J198" s="4" t="n">
         <f aca="false">J197+D197</f>
@@ -10536,7 +10539,7 @@
     </row>
     <row r="201" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="42" t="s">
-        <v>428</v>
+        <v>430</v>
       </c>
       <c r="B201" s="11"/>
       <c r="C201" s="41"/>
@@ -10602,10 +10605,10 @@
     </row>
     <row r="203" customFormat="false" ht="37.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B203" s="31" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="C203" s="22" t="s">
-        <v>421</v>
+        <v>423</v>
       </c>
       <c r="D203" s="22" t="n">
         <v>664</v>
@@ -10623,7 +10626,7 @@
         <v>27</v>
       </c>
       <c r="I203" s="23" t="s">
-        <v>422</v>
+        <v>424</v>
       </c>
       <c r="J203" s="4" t="n">
         <v>0</v>
@@ -10655,10 +10658,10 @@
     </row>
     <row r="204" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B204" s="31" t="s">
-        <v>423</v>
+        <v>425</v>
       </c>
       <c r="C204" s="22" t="s">
-        <v>424</v>
+        <v>426</v>
       </c>
       <c r="D204" s="22" t="n">
         <v>7</v>
@@ -10707,10 +10710,10 @@
     </row>
     <row r="205" customFormat="false" ht="25.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B205" s="31" t="s">
-        <v>425</v>
+        <v>427</v>
       </c>
       <c r="C205" s="22" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="D205" s="22" t="n">
         <v>1</v>
@@ -10724,7 +10727,7 @@
       </c>
       <c r="H205" s="22"/>
       <c r="I205" s="23" t="s">
-        <v>427</v>
+        <v>429</v>
       </c>
       <c r="J205" s="4" t="n">
         <f aca="false">J204+D204</f>
@@ -10781,7 +10784,7 @@
     </row>
     <row r="210" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A210" s="42" t="s">
-        <v>429</v>
+        <v>431</v>
       </c>
       <c r="B210" s="11"/>
       <c r="C210" s="41"/>
@@ -10847,10 +10850,10 @@
     </row>
     <row r="212" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B212" s="31" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="C212" s="32" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
       <c r="D212" s="27" t="n">
         <v>32</v>
@@ -10863,10 +10866,10 @@
         <v>1</v>
       </c>
       <c r="H212" s="39" t="s">
-        <v>430</v>
+        <v>432</v>
       </c>
       <c r="I212" s="28" t="s">
-        <v>412</v>
+        <v>414</v>
       </c>
       <c r="J212" s="4" t="n">
         <f aca="false">J206</f>
@@ -10885,7 +10888,7 @@
         <v>21</v>
       </c>
       <c r="N212" s="1" t="s">
-        <v>413</v>
+        <v>415</v>
       </c>
       <c r="O212" s="3" t="n">
         <v>8</v>
@@ -10899,10 +10902,10 @@
     </row>
     <row r="213" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B213" s="31" t="s">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c r="C213" s="32" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c r="D213" s="27" t="n">
         <v>16</v>
@@ -10911,7 +10914,7 @@
         <v>26</v>
       </c>
       <c r="F213" s="23" t="s">
-        <v>432</v>
+        <v>434</v>
       </c>
       <c r="G213" s="39" t="n">
         <v>1</v>
@@ -10920,7 +10923,7 @@
         <v>27</v>
       </c>
       <c r="I213" s="28" t="s">
-        <v>412</v>
+        <v>414</v>
       </c>
       <c r="J213" s="4" t="n">
         <f aca="false">J212+D212</f>
@@ -10939,7 +10942,7 @@
         <v>22</v>
       </c>
       <c r="N213" s="1" t="s">
-        <v>413</v>
+        <v>415</v>
       </c>
       <c r="O213" s="3" t="n">
         <v>8</v>
@@ -10956,7 +10959,7 @@
         <v>28</v>
       </c>
       <c r="C214" s="32" t="s">
-        <v>417</v>
+        <v>419</v>
       </c>
       <c r="D214" s="27" t="n">
         <v>8</v>
@@ -10970,7 +10973,7 @@
         <v>27</v>
       </c>
       <c r="I214" s="28" t="s">
-        <v>433</v>
+        <v>435</v>
       </c>
       <c r="J214" s="4" t="n">
         <f aca="false">J213+D213</f>
@@ -10989,7 +10992,7 @@
         <v>22.5</v>
       </c>
       <c r="N214" s="5" t="s">
-        <v>413</v>
+        <v>415</v>
       </c>
       <c r="O214" s="24" t="n">
         <v>8</v>
@@ -11006,7 +11009,7 @@
         <v>28</v>
       </c>
       <c r="C215" s="32" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="D215" s="27" t="n">
         <v>8</v>
@@ -11089,7 +11092,7 @@
     </row>
     <row r="218" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A218" s="42" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
     </row>
     <row r="219" s="14" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11147,10 +11150,10 @@
     </row>
     <row r="220" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B220" s="43" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="C220" s="38" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="D220" s="38" t="n">
         <v>32</v>
@@ -11163,10 +11166,10 @@
         <v>133</v>
       </c>
       <c r="H220" s="38" t="s">
-        <v>435</v>
+        <v>437</v>
       </c>
       <c r="I220" s="38" t="s">
-        <v>436</v>
+        <v>438</v>
       </c>
       <c r="J220" s="44" t="n">
         <v>0</v>
@@ -11184,7 +11187,7 @@
         <v>0</v>
       </c>
       <c r="N220" s="1" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="O220" s="3" t="n">
         <v>1</v>
@@ -11198,7 +11201,7 @@
     </row>
     <row r="221" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A221" s="1" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="B221" s="43"/>
       <c r="C221" s="38"/>
@@ -11215,10 +11218,10 @@
     </row>
     <row r="222" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B222" s="43" t="s">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="C222" s="38" t="s">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="D222" s="38" t="n">
         <v>1</v>
@@ -11228,13 +11231,13 @@
       </c>
       <c r="F222" s="38"/>
       <c r="G222" s="38" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
       <c r="H222" s="38" t="s">
         <v>27</v>
       </c>
       <c r="I222" s="38" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="J222" s="44" t="n">
         <f aca="false">J220+D220</f>
@@ -11253,7 +11256,7 @@
         <v>1</v>
       </c>
       <c r="N222" s="1" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="O222" s="3" t="n">
         <v>1</v>
@@ -11267,10 +11270,10 @@
     </row>
     <row r="223" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B223" s="43" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="C223" s="38" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="D223" s="38" t="n">
         <v>5</v>
@@ -11284,7 +11287,7 @@
       </c>
       <c r="H223" s="38"/>
       <c r="I223" s="38" t="s">
-        <v>443</v>
+        <v>445</v>
       </c>
       <c r="J223" s="44" t="n">
         <f aca="false">J222+D222</f>
@@ -11303,7 +11306,7 @@
         <v>1.03125</v>
       </c>
       <c r="N223" s="1" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="O223" s="3" t="n">
         <v>1</v>
@@ -11317,10 +11320,10 @@
     </row>
     <row r="224" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B224" s="43" t="s">
-        <v>444</v>
+        <v>446</v>
       </c>
       <c r="C224" s="38" t="s">
-        <v>444</v>
+        <v>446</v>
       </c>
       <c r="D224" s="38" t="n">
         <v>4</v>
@@ -11336,7 +11339,7 @@
         <v>27</v>
       </c>
       <c r="I224" s="38" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="J224" s="44" t="n">
         <f aca="false">J223+D223</f>
@@ -11355,7 +11358,7 @@
         <v>1.1875</v>
       </c>
       <c r="N224" s="1" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="O224" s="3" t="n">
         <v>1</v>
@@ -11369,10 +11372,10 @@
     </row>
     <row r="225" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B225" s="43" t="s">
-        <v>445</v>
+        <v>447</v>
       </c>
       <c r="C225" s="38" t="s">
-        <v>445</v>
+        <v>447</v>
       </c>
       <c r="D225" s="38" t="n">
         <v>5</v>
@@ -11388,7 +11391,7 @@
         <v>27</v>
       </c>
       <c r="I225" s="38" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="J225" s="44" t="n">
         <f aca="false">J224+D224</f>
@@ -11407,7 +11410,7 @@
         <v>1.3125</v>
       </c>
       <c r="N225" s="1" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="O225" s="3" t="n">
         <v>1</v>
@@ -11421,10 +11424,10 @@
     </row>
     <row r="226" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B226" s="43" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="C226" s="38" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="D226" s="38" t="n">
         <v>6</v>
@@ -11440,7 +11443,7 @@
         <v>27</v>
       </c>
       <c r="I226" s="38" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="J226" s="44" t="n">
         <f aca="false">J225+D225</f>
@@ -11459,7 +11462,7 @@
         <v>1.46875</v>
       </c>
       <c r="N226" s="1" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="O226" s="3" t="n">
         <v>1</v>
@@ -11473,10 +11476,10 @@
     </row>
     <row r="227" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B227" s="43" t="s">
-        <v>447</v>
+        <v>449</v>
       </c>
       <c r="C227" s="38" t="s">
-        <v>447</v>
+        <v>449</v>
       </c>
       <c r="D227" s="38" t="n">
         <v>6</v>
@@ -11492,7 +11495,7 @@
         <v>27</v>
       </c>
       <c r="I227" s="38" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="J227" s="44" t="n">
         <f aca="false">J226+D226</f>
@@ -11511,7 +11514,7 @@
         <v>1.65625</v>
       </c>
       <c r="N227" s="1" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="O227" s="3" t="n">
         <v>1</v>
@@ -11525,10 +11528,10 @@
     </row>
     <row r="228" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B228" s="43" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="C228" s="38" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="D228" s="38" t="n">
         <v>5</v>
@@ -11544,7 +11547,7 @@
         <v>27</v>
       </c>
       <c r="I228" s="38" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="J228" s="44" t="n">
         <f aca="false">J227+D227</f>
@@ -11563,7 +11566,7 @@
         <v>1.84375</v>
       </c>
       <c r="N228" s="1" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="O228" s="3" t="n">
         <v>1</v>
@@ -11577,7 +11580,7 @@
     </row>
     <row r="229" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A229" s="1" t="s">
-        <v>449</v>
+        <v>451</v>
       </c>
       <c r="B229" s="43"/>
       <c r="C229" s="38"/>
@@ -11594,10 +11597,10 @@
     </row>
     <row r="230" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B230" s="43" t="s">
-        <v>450</v>
+        <v>452</v>
       </c>
       <c r="C230" s="38" t="s">
-        <v>450</v>
+        <v>452</v>
       </c>
       <c r="D230" s="38" t="n">
         <v>8</v>
@@ -11613,7 +11616,7 @@
         <v>71</v>
       </c>
       <c r="I230" s="38" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="J230" s="44" t="n">
         <f aca="false">J228+D228</f>
@@ -11632,7 +11635,7 @@
         <v>2</v>
       </c>
       <c r="N230" s="1" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="O230" s="3" t="n">
         <v>1</v>
@@ -11646,10 +11649,10 @@
     </row>
     <row r="231" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B231" s="43" t="s">
-        <v>451</v>
+        <v>453</v>
       </c>
       <c r="C231" s="38" t="s">
-        <v>451</v>
+        <v>453</v>
       </c>
       <c r="D231" s="38" t="n">
         <v>8</v>
@@ -11665,7 +11668,7 @@
         <v>71</v>
       </c>
       <c r="I231" s="38" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="J231" s="44" t="n">
         <f aca="false">J230+D230</f>
@@ -11684,7 +11687,7 @@
         <v>2.25</v>
       </c>
       <c r="N231" s="1" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="O231" s="3" t="n">
         <v>1</v>
@@ -11698,10 +11701,10 @@
     </row>
     <row r="232" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B232" s="43" t="s">
-        <v>452</v>
+        <v>454</v>
       </c>
       <c r="C232" s="38" t="s">
-        <v>453</v>
+        <v>455</v>
       </c>
       <c r="D232" s="38" t="n">
         <v>16</v>
@@ -11717,7 +11720,7 @@
         <v>27</v>
       </c>
       <c r="I232" s="38" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="J232" s="44" t="n">
         <f aca="false">J231+D231</f>
@@ -11780,7 +11783,7 @@
     </row>
     <row r="234" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A234" s="42" t="s">
-        <v>454</v>
+        <v>456</v>
       </c>
       <c r="F234" s="38"/>
       <c r="G234" s="38"/>
@@ -11864,10 +11867,10 @@
     </row>
     <row r="237" s="47" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B237" s="21" t="s">
-        <v>455</v>
+        <v>457</v>
       </c>
       <c r="C237" s="45" t="s">
-        <v>456</v>
+        <v>458</v>
       </c>
       <c r="D237" s="1" t="n">
         <v>5</v>
@@ -11883,7 +11886,7 @@
         <v>27</v>
       </c>
       <c r="I237" s="38" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="J237" s="44" t="n">
         <f aca="false">J233</f>
@@ -11916,10 +11919,10 @@
     </row>
     <row r="238" s="47" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B238" s="21" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
       <c r="C238" s="45" t="s">
-        <v>458</v>
+        <v>460</v>
       </c>
       <c r="D238" s="1" t="n">
         <v>1</v>
@@ -11929,13 +11932,13 @@
       </c>
       <c r="F238" s="46"/>
       <c r="G238" s="38" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
       <c r="H238" s="38" t="s">
         <v>27</v>
       </c>
       <c r="I238" s="38" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="J238" s="44" t="n">
         <f aca="false">J237+D237</f>
@@ -11954,7 +11957,7 @@
         <v>3.15625</v>
       </c>
       <c r="N238" s="1" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="O238" s="3" t="n">
         <v>1</v>
@@ -11968,10 +11971,10 @@
     </row>
     <row r="239" s="47" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B239" s="21" t="s">
-        <v>459</v>
+        <v>461</v>
       </c>
       <c r="C239" s="45" t="s">
-        <v>460</v>
+        <v>462</v>
       </c>
       <c r="D239" s="1" t="n">
         <v>1</v>
@@ -11981,13 +11984,13 @@
       </c>
       <c r="F239" s="46"/>
       <c r="G239" s="38" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
       <c r="H239" s="38" t="s">
         <v>27</v>
       </c>
       <c r="I239" s="38" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="J239" s="44" t="n">
         <f aca="false">J238+D238</f>
@@ -12006,7 +12009,7 @@
         <v>3.1875</v>
       </c>
       <c r="N239" s="1" t="s">
-        <v>461</v>
+        <v>463</v>
       </c>
       <c r="O239" s="3" t="n">
         <v>2</v>
@@ -12020,10 +12023,10 @@
     </row>
     <row r="240" s="47" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B240" s="21" t="s">
-        <v>462</v>
+        <v>464</v>
       </c>
       <c r="C240" s="45" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="D240" s="1" t="n">
         <v>3</v>
@@ -12039,7 +12042,7 @@
         <v>27</v>
       </c>
       <c r="I240" s="38" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="J240" s="44" t="n">
         <f aca="false">J239+D239</f>
@@ -12058,7 +12061,7 @@
         <v>3.21875</v>
       </c>
       <c r="N240" s="1" t="s">
-        <v>461</v>
+        <v>463</v>
       </c>
       <c r="O240" s="3" t="n">
         <v>2</v>
@@ -12072,10 +12075,10 @@
     </row>
     <row r="241" s="47" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B241" s="21" t="s">
-        <v>464</v>
+        <v>466</v>
       </c>
       <c r="C241" s="45" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="D241" s="1" t="n">
         <v>4</v>
@@ -12085,13 +12088,13 @@
       </c>
       <c r="F241" s="46"/>
       <c r="G241" s="38" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="H241" s="38" t="s">
         <v>27</v>
       </c>
       <c r="I241" s="38" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="J241" s="44" t="n">
         <f aca="false">J240+D240</f>
@@ -12110,7 +12113,7 @@
         <v>3.3125</v>
       </c>
       <c r="N241" s="1" t="s">
-        <v>461</v>
+        <v>463</v>
       </c>
       <c r="O241" s="3" t="n">
         <v>2</v>
@@ -12124,10 +12127,10 @@
     </row>
     <row r="242" s="47" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B242" s="21" t="s">
-        <v>467</v>
+        <v>469</v>
       </c>
       <c r="C242" s="45" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="D242" s="1" t="n">
         <v>4</v>
@@ -12137,13 +12140,13 @@
       </c>
       <c r="F242" s="46"/>
       <c r="G242" s="38" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="H242" s="38" t="s">
         <v>27</v>
       </c>
       <c r="I242" s="38" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="J242" s="44" t="n">
         <f aca="false">J241+D241</f>
@@ -12162,7 +12165,7 @@
         <v>3.4375</v>
       </c>
       <c r="N242" s="1" t="s">
-        <v>461</v>
+        <v>463</v>
       </c>
       <c r="O242" s="3" t="n">
         <v>2</v>
@@ -12176,10 +12179,10 @@
     </row>
     <row r="243" s="47" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B243" s="21" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="C243" s="45" t="s">
-        <v>470</v>
+        <v>472</v>
       </c>
       <c r="D243" s="1" t="n">
         <v>5</v>
@@ -12189,13 +12192,13 @@
       </c>
       <c r="F243" s="46"/>
       <c r="G243" s="38" t="s">
-        <v>471</v>
+        <v>473</v>
       </c>
       <c r="H243" s="38" t="s">
         <v>27</v>
       </c>
       <c r="I243" s="38" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="J243" s="44" t="n">
         <f aca="false">J242+D242</f>
@@ -12214,7 +12217,7 @@
         <v>3.5625</v>
       </c>
       <c r="N243" s="1" t="s">
-        <v>461</v>
+        <v>463</v>
       </c>
       <c r="O243" s="3" t="n">
         <v>2</v>
@@ -12228,10 +12231,10 @@
     </row>
     <row r="244" s="47" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B244" s="21" t="s">
-        <v>472</v>
+        <v>474</v>
       </c>
       <c r="C244" s="45" t="s">
-        <v>473</v>
+        <v>475</v>
       </c>
       <c r="D244" s="1" t="n">
         <v>9</v>
@@ -12247,7 +12250,7 @@
         <v>27</v>
       </c>
       <c r="I244" s="38" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="J244" s="44" t="n">
         <f aca="false">J243+D243</f>
@@ -12266,7 +12269,7 @@
         <v>3.71875</v>
       </c>
       <c r="N244" s="1" t="s">
-        <v>461</v>
+        <v>463</v>
       </c>
       <c r="O244" s="3" t="n">
         <v>2</v>
@@ -12299,10 +12302,10 @@
     </row>
     <row r="246" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B246" s="47" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="C246" s="3" t="s">
-        <v>475</v>
+        <v>477</v>
       </c>
       <c r="D246" s="1" t="n">
         <v>8</v>
@@ -12318,7 +12321,7 @@
         <v>27</v>
       </c>
       <c r="I246" s="38" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="J246" s="44" t="n">
         <f aca="false">J244+D244</f>
@@ -12337,7 +12340,7 @@
         <v>4</v>
       </c>
       <c r="N246" s="1" t="s">
-        <v>476</v>
+        <v>478</v>
       </c>
       <c r="O246" s="3" t="n">
         <v>3</v>
@@ -12351,10 +12354,10 @@
     </row>
     <row r="247" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B247" s="47" t="s">
-        <v>477</v>
+        <v>479</v>
       </c>
       <c r="C247" s="3" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="D247" s="1" t="n">
         <v>8</v>
@@ -12370,7 +12373,7 @@
         <v>27</v>
       </c>
       <c r="I247" s="38" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="J247" s="44" t="n">
         <f aca="false">J246+D246</f>
@@ -12389,7 +12392,7 @@
         <v>4.25</v>
       </c>
       <c r="N247" s="1" t="s">
-        <v>476</v>
+        <v>478</v>
       </c>
       <c r="O247" s="3" t="n">
         <v>3</v>
@@ -12403,10 +12406,10 @@
     </row>
     <row r="248" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B248" s="47" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="C248" s="3" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="D248" s="1" t="n">
         <v>8</v>
@@ -12422,7 +12425,7 @@
         <v>27</v>
       </c>
       <c r="I248" s="38" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="J248" s="44" t="n">
         <f aca="false">J247+D247</f>
@@ -12441,7 +12444,7 @@
         <v>4.5</v>
       </c>
       <c r="N248" s="1" t="s">
-        <v>476</v>
+        <v>478</v>
       </c>
       <c r="O248" s="3" t="n">
         <v>3</v>
@@ -12455,10 +12458,10 @@
     </row>
     <row r="249" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B249" s="47" t="s">
-        <v>481</v>
+        <v>483</v>
       </c>
       <c r="C249" s="3" t="s">
-        <v>482</v>
+        <v>484</v>
       </c>
       <c r="D249" s="1" t="n">
         <v>8</v>
@@ -12474,7 +12477,7 @@
         <v>27</v>
       </c>
       <c r="I249" s="38" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="J249" s="44" t="n">
         <f aca="false">J248+D248</f>
@@ -12493,7 +12496,7 @@
         <v>4.75</v>
       </c>
       <c r="N249" s="1" t="s">
-        <v>476</v>
+        <v>478</v>
       </c>
       <c r="O249" s="3" t="n">
         <v>3</v>
@@ -12507,10 +12510,10 @@
     </row>
     <row r="250" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B250" s="47" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="C250" s="3" t="s">
-        <v>484</v>
+        <v>486</v>
       </c>
       <c r="D250" s="1" t="n">
         <v>8</v>
@@ -12526,7 +12529,7 @@
         <v>27</v>
       </c>
       <c r="I250" s="38" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="J250" s="44" t="n">
         <f aca="false">J249+D249</f>
@@ -12545,7 +12548,7 @@
         <v>5</v>
       </c>
       <c r="N250" s="1" t="s">
-        <v>476</v>
+        <v>478</v>
       </c>
       <c r="O250" s="3" t="n">
         <v>3</v>
@@ -12559,10 +12562,10 @@
     </row>
     <row r="251" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B251" s="47" t="s">
-        <v>485</v>
+        <v>487</v>
       </c>
       <c r="C251" s="3" t="s">
-        <v>486</v>
+        <v>488</v>
       </c>
       <c r="D251" s="1" t="n">
         <v>8</v>
@@ -12578,7 +12581,7 @@
         <v>27</v>
       </c>
       <c r="I251" s="38" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="J251" s="44" t="n">
         <f aca="false">J250+D250</f>
@@ -12597,7 +12600,7 @@
         <v>5.25</v>
       </c>
       <c r="N251" s="1" t="s">
-        <v>476</v>
+        <v>478</v>
       </c>
       <c r="O251" s="3" t="n">
         <v>3</v>
@@ -12611,10 +12614,10 @@
     </row>
     <row r="252" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B252" s="47" t="s">
-        <v>487</v>
+        <v>489</v>
       </c>
       <c r="C252" s="3" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="D252" s="1" t="n">
         <v>8</v>
@@ -12630,7 +12633,7 @@
         <v>27</v>
       </c>
       <c r="I252" s="38" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="J252" s="44" t="n">
         <f aca="false">J251+D251</f>
@@ -12649,7 +12652,7 @@
         <v>5.5</v>
       </c>
       <c r="N252" s="1" t="s">
-        <v>476</v>
+        <v>478</v>
       </c>
       <c r="O252" s="3" t="n">
         <v>3</v>
@@ -12663,10 +12666,10 @@
     </row>
     <row r="253" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B253" s="47" t="s">
-        <v>489</v>
+        <v>491</v>
       </c>
       <c r="C253" s="3" t="s">
-        <v>490</v>
+        <v>492</v>
       </c>
       <c r="D253" s="1" t="n">
         <v>8</v>
@@ -12682,7 +12685,7 @@
         <v>27</v>
       </c>
       <c r="I253" s="38" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="J253" s="44" t="n">
         <f aca="false">J252+D252</f>
@@ -12701,7 +12704,7 @@
         <v>5.75</v>
       </c>
       <c r="N253" s="1" t="s">
-        <v>476</v>
+        <v>478</v>
       </c>
       <c r="O253" s="3" t="n">
         <v>3</v>
@@ -12715,10 +12718,10 @@
     </row>
     <row r="254" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B254" s="47" t="s">
-        <v>491</v>
+        <v>493</v>
       </c>
       <c r="C254" s="3" t="s">
-        <v>491</v>
+        <v>493</v>
       </c>
       <c r="D254" s="1" t="n">
         <v>8</v>
@@ -12734,7 +12737,7 @@
         <v>27</v>
       </c>
       <c r="I254" s="38" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="J254" s="44" t="n">
         <f aca="false">J253+D253</f>
@@ -12753,7 +12756,7 @@
         <v>6</v>
       </c>
       <c r="N254" s="1" t="s">
-        <v>476</v>
+        <v>478</v>
       </c>
       <c r="O254" s="3" t="n">
         <v>3</v>
@@ -12767,10 +12770,10 @@
     </row>
     <row r="255" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B255" s="47" t="s">
-        <v>492</v>
+        <v>494</v>
       </c>
       <c r="C255" s="3" t="s">
-        <v>492</v>
+        <v>494</v>
       </c>
       <c r="D255" s="1" t="n">
         <v>8</v>
@@ -12786,7 +12789,7 @@
         <v>27</v>
       </c>
       <c r="I255" s="38" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="J255" s="44" t="n">
         <f aca="false">J254+D254</f>
@@ -12805,7 +12808,7 @@
         <v>6.25</v>
       </c>
       <c r="N255" s="1" t="s">
-        <v>476</v>
+        <v>478</v>
       </c>
       <c r="O255" s="3" t="n">
         <v>3</v>
@@ -12819,10 +12822,10 @@
     </row>
     <row r="256" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B256" s="47" t="s">
-        <v>493</v>
+        <v>495</v>
       </c>
       <c r="C256" s="3" t="s">
-        <v>493</v>
+        <v>495</v>
       </c>
       <c r="D256" s="1" t="n">
         <v>8</v>
@@ -12838,7 +12841,7 @@
         <v>27</v>
       </c>
       <c r="I256" s="38" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="J256" s="44" t="n">
         <f aca="false">J255+D255</f>
@@ -12857,7 +12860,7 @@
         <v>6.5</v>
       </c>
       <c r="N256" s="1" t="s">
-        <v>476</v>
+        <v>478</v>
       </c>
       <c r="O256" s="3" t="n">
         <v>3</v>
@@ -12871,10 +12874,10 @@
     </row>
     <row r="257" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B257" s="47" t="s">
-        <v>494</v>
+        <v>496</v>
       </c>
       <c r="C257" s="3" t="s">
-        <v>494</v>
+        <v>496</v>
       </c>
       <c r="D257" s="1" t="n">
         <v>8</v>
@@ -12890,7 +12893,7 @@
         <v>27</v>
       </c>
       <c r="I257" s="38" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="J257" s="44" t="n">
         <f aca="false">J256+D256</f>
@@ -12909,7 +12912,7 @@
         <v>6.75</v>
       </c>
       <c r="N257" s="1" t="s">
-        <v>476</v>
+        <v>478</v>
       </c>
       <c r="O257" s="3" t="n">
         <v>3</v>
@@ -12923,10 +12926,10 @@
     </row>
     <row r="258" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B258" s="47" t="s">
-        <v>495</v>
+        <v>497</v>
       </c>
       <c r="C258" s="3" t="s">
-        <v>495</v>
+        <v>497</v>
       </c>
       <c r="D258" s="1" t="n">
         <v>8</v>
@@ -12942,7 +12945,7 @@
         <v>27</v>
       </c>
       <c r="I258" s="38" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="J258" s="44" t="n">
         <f aca="false">J257+D257</f>
@@ -12961,7 +12964,7 @@
         <v>7</v>
       </c>
       <c r="N258" s="1" t="s">
-        <v>476</v>
+        <v>478</v>
       </c>
       <c r="O258" s="3" t="n">
         <v>3</v>
@@ -12975,10 +12978,10 @@
     </row>
     <row r="259" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B259" s="47" t="s">
-        <v>496</v>
+        <v>498</v>
       </c>
       <c r="C259" s="3" t="s">
-        <v>497</v>
+        <v>499</v>
       </c>
       <c r="D259" s="1" t="n">
         <v>16</v>
@@ -12996,7 +12999,7 @@
         <v>27</v>
       </c>
       <c r="I259" s="38" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="J259" s="44" t="n">
         <f aca="false">J258+D258</f>
@@ -13015,7 +13018,7 @@
         <v>7.25</v>
       </c>
       <c r="N259" s="1" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="O259" s="3" t="n">
         <v>1</v>
@@ -13029,10 +13032,10 @@
     </row>
     <row r="260" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B260" s="47" t="s">
-        <v>498</v>
+        <v>500</v>
       </c>
       <c r="C260" s="3" t="s">
-        <v>499</v>
+        <v>501</v>
       </c>
       <c r="D260" s="1" t="n">
         <v>8</v>
@@ -13048,7 +13051,7 @@
         <v>27</v>
       </c>
       <c r="I260" s="38" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="J260" s="44" t="n">
         <f aca="false">J259+D259</f>
@@ -13067,7 +13070,7 @@
         <v>7.75</v>
       </c>
       <c r="N260" s="1" t="s">
-        <v>461</v>
+        <v>463</v>
       </c>
       <c r="O260" s="3" t="n">
         <v>2</v>
@@ -13155,7 +13158,7 @@
   <dimension ref="B6:Q1031"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C33" activeCellId="1" sqref="G123 C33"/>
+      <selection pane="topLeft" activeCell="C33" activeCellId="0" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.0390625" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13169,22 +13172,22 @@
     <row r="6" s="49" customFormat="true" ht="34.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B6" s="50"/>
       <c r="C6" s="50" t="s">
-        <v>500</v>
+        <v>502</v>
       </c>
       <c r="D6" s="50" t="s">
-        <v>501</v>
+        <v>503</v>
       </c>
       <c r="E6" s="50" t="s">
-        <v>502</v>
+        <v>504</v>
       </c>
       <c r="F6" s="50" t="s">
-        <v>503</v>
+        <v>505</v>
       </c>
       <c r="G6" s="50" t="s">
-        <v>504</v>
+        <v>279</v>
       </c>
       <c r="H6" s="50" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="I6" s="50"/>
     </row>
@@ -13554,10 +13557,10 @@
     </row>
     <row r="26" s="1" customFormat="true" ht="37.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="32" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="C26" s="32" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="D26" s="27" t="n">
         <v>16</v>
@@ -13570,10 +13573,10 @@
         <v>1</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="I26" s="28" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="J26" s="29" t="n">
         <f aca="false">DownlinkSpecLTM!J166+DownlinkSpecLTM!D166</f>
@@ -13592,7 +13595,7 @@
         <v>15.5</v>
       </c>
       <c r="N26" s="1" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="O26" s="3" t="n">
         <v>6</v>
@@ -13606,10 +13609,10 @@
     </row>
     <row r="27" s="1" customFormat="true" ht="37.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="32" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="C27" s="32" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="D27" s="27" t="n">
         <v>32</v>
@@ -13620,10 +13623,10 @@
         <v>1</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="I27" s="28" t="s">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="J27" s="29" t="n">
         <f aca="false">J26+D26</f>
@@ -13642,7 +13645,7 @@
         <v>16</v>
       </c>
       <c r="N27" s="1" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="O27" s="3" t="n">
         <v>6</v>
@@ -13656,16 +13659,16 @@
     </row>
     <row r="30" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="52" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="C30" s="52" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="D30" s="52" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="E30" s="52" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="F30" s="52"/>
     </row>

</xml_diff>

<commit_message>
Tweak the antenna status info
(Deployable sense and Deploy sense ok under Spacecraft Status)
</commit_message>
<xml_diff>
--- a/genSpacecraft/DownlinkSpecLTM.xlsx
+++ b/genSpacecraft/DownlinkSpecLTM.xlsx
@@ -731,22 +731,22 @@
     <t xml:space="preserve">Structure: commonRtWodPayload_t,file:common2Downlink.h</t>
   </si>
   <si>
-    <t xml:space="preserve">Deploy Sense via CAN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DeploySenseCan</t>
+    <t xml:space="preserve">Deployable Sense</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DeploySense</t>
   </si>
   <si>
     <t xml:space="preserve">DeployableStatus_t</t>
   </si>
   <si>
+    <t xml:space="preserve">BIN8</t>
+  </si>
+  <si>
     <t xml:space="preserve">TBD</t>
   </si>
   <si>
-    <t xml:space="preserve">Deploy Sense via I2c</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DeploySenseI2c</t>
+    <t xml:space="preserve">spare28</t>
   </si>
   <si>
     <t xml:space="preserve">de</t>
@@ -794,16 +794,19 @@
     <t xml:space="preserve">I2CfailureICR</t>
   </si>
   <si>
-    <t xml:space="preserve">Antenna is not communicating over bus 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I2c Deploy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I2CFailureDeploy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Antenna is not communicating over bus 1</t>
+    <t xml:space="preserve">ICR I2c ADC Not Working</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deploy Sense Ok</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DeploySenseOK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STATUS_1_EQ_OK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Antenna sensor is ok</t>
   </si>
   <si>
     <t xml:space="preserve">Min/Max Resets</t>
@@ -975,9 +978,6 @@
   </si>
   <si>
     <t xml:space="preserve">hostBits19</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STATUS_1_EQ_OK</t>
   </si>
   <si>
     <t xml:space="preserve">Detumble</t>
@@ -1943,8 +1943,8 @@
   </sheetPr>
   <dimension ref="A1:Q263"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A88" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B104" activeCellId="0" sqref="B104"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A82" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G97" activeCellId="0" sqref="G97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5705,7 +5705,7 @@
       <c r="L86" s="28"/>
       <c r="M86" s="28"/>
     </row>
-    <row r="87" customFormat="false" ht="25.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B87" s="31" t="s">
         <v>236</v>
       </c>
@@ -5721,14 +5721,14 @@
       <c r="F87" s="23" t="s">
         <v>238</v>
       </c>
-      <c r="G87" s="22" t="n">
-        <v>16</v>
+      <c r="G87" s="22" t="s">
+        <v>239</v>
       </c>
       <c r="H87" s="22" t="s">
         <v>27</v>
       </c>
       <c r="I87" s="23" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="J87" s="29" t="n">
         <f aca="false">J83</f>
@@ -5759,9 +5759,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" customFormat="false" ht="25.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B88" s="31" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C88" s="32" t="s">
         <v>241</v>
@@ -5772,17 +5772,13 @@
       <c r="E88" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="F88" s="23" t="s">
-        <v>238</v>
-      </c>
+      <c r="F88" s="23"/>
       <c r="G88" s="22" t="n">
-        <v>16</v>
-      </c>
-      <c r="H88" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="I88" s="23" t="s">
-        <v>239</v>
+        <v>0</v>
+      </c>
+      <c r="H88" s="22"/>
+      <c r="I88" s="32" t="s">
+        <v>230</v>
       </c>
       <c r="J88" s="29" t="n">
         <f aca="false">J87+D87</f>
@@ -5800,14 +5796,14 @@
         <f aca="false">J88/32</f>
         <v>14.25</v>
       </c>
-      <c r="N88" s="5" t="s">
-        <v>185</v>
+      <c r="N88" s="1" t="s">
+        <v>28</v>
       </c>
       <c r="O88" s="24" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P88" s="1" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="Q88" s="1" t="n">
         <v>0</v>
@@ -5928,7 +5924,7 @@
         <v>2</v>
       </c>
       <c r="P91" s="1" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Q91" s="1" t="n">
         <v>0</v>
@@ -5980,7 +5976,7 @@
         <v>2</v>
       </c>
       <c r="P92" s="1" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="Q92" s="1" t="n">
         <v>0</v>
@@ -6140,7 +6136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" customFormat="false" ht="37.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="96" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B96" s="33" t="s">
         <v>255</v>
       </c>
@@ -6192,7 +6188,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" customFormat="false" ht="37.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="97" customFormat="false" ht="25.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B97" s="33" t="s">
         <v>258</v>
       </c>
@@ -6206,14 +6202,14 @@
         <v>26</v>
       </c>
       <c r="F97" s="23"/>
-      <c r="G97" s="23" t="n">
-        <v>17</v>
+      <c r="G97" s="22" t="s">
+        <v>260</v>
       </c>
       <c r="H97" s="22" t="s">
         <v>27</v>
       </c>
       <c r="I97" s="23" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="J97" s="29" t="n">
         <f aca="false">J96+D96</f>
@@ -6238,7 +6234,7 @@
         <v>2</v>
       </c>
       <c r="P97" s="1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="Q97" s="1" t="n">
         <v>0</v>
@@ -6266,10 +6262,10 @@
     </row>
     <row r="99" customFormat="false" ht="50.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B99" s="31" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="C99" s="32" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="D99" s="32" t="n">
         <v>8</v>
@@ -6285,7 +6281,7 @@
         <v>27</v>
       </c>
       <c r="I99" s="23" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="J99" s="29" t="n">
         <f aca="false">J97+D97</f>
@@ -6310,7 +6306,7 @@
         <v>2</v>
       </c>
       <c r="P99" s="1" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="Q99" s="1" t="n">
         <v>0</v>
@@ -6318,10 +6314,10 @@
     </row>
     <row r="100" customFormat="false" ht="75.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B100" s="31" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="C100" s="32" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="D100" s="32" t="n">
         <v>8</v>
@@ -6337,7 +6333,7 @@
         <v>27</v>
       </c>
       <c r="I100" s="23" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="J100" s="29" t="n">
         <f aca="false">J99+D99</f>
@@ -6362,7 +6358,7 @@
         <v>2</v>
       </c>
       <c r="P100" s="1" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="Q100" s="1" t="n">
         <v>0</v>
@@ -6370,10 +6366,10 @@
     </row>
     <row r="101" customFormat="false" ht="25.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B101" s="31" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="C101" s="32" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="D101" s="32" t="n">
         <v>32</v>
@@ -6391,7 +6387,7 @@
         <v>27</v>
       </c>
       <c r="I101" s="23" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="J101" s="29" t="n">
         <f aca="false">J100+D100</f>
@@ -6424,10 +6420,10 @@
     </row>
     <row r="102" customFormat="false" ht="50.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B102" s="31" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="C102" s="32" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="D102" s="32" t="n">
         <v>8</v>
@@ -6443,7 +6439,7 @@
         <v>27</v>
       </c>
       <c r="I102" s="23" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="J102" s="29" t="n">
         <f aca="false">J101+D101</f>
@@ -6476,10 +6472,10 @@
     </row>
     <row r="103" customFormat="false" ht="50.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B103" s="31" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="C103" s="32" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="D103" s="32" t="n">
         <v>8</v>
@@ -6495,7 +6491,7 @@
         <v>27</v>
       </c>
       <c r="I103" s="23" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="J103" s="29" t="n">
         <f aca="false">J102+D102</f>
@@ -6528,10 +6524,10 @@
     </row>
     <row r="104" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B104" s="31" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C104" s="32" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="D104" s="32" t="n">
         <v>8</v>
@@ -6541,13 +6537,13 @@
       </c>
       <c r="F104" s="23"/>
       <c r="G104" s="23" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="H104" s="22" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="I104" s="23" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="J104" s="29" t="n">
         <f aca="false">J103+D103</f>
@@ -6580,10 +6576,10 @@
     </row>
     <row r="105" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B105" s="31" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="C105" s="32" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="D105" s="32" t="n">
         <v>1</v>
@@ -6593,13 +6589,13 @@
       </c>
       <c r="F105" s="23"/>
       <c r="G105" s="22" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="H105" s="22" t="s">
         <v>27</v>
       </c>
       <c r="I105" s="32" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="J105" s="29" t="n">
         <f aca="false">J104+D104</f>
@@ -6632,10 +6628,10 @@
     </row>
     <row r="106" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B106" s="31" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C106" s="32" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="D106" s="32" t="n">
         <v>1</v>
@@ -6645,7 +6641,7 @@
       </c>
       <c r="F106" s="23"/>
       <c r="G106" s="22" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="H106" s="22" t="s">
         <v>27</v>
@@ -6682,10 +6678,10 @@
     </row>
     <row r="107" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B107" s="31" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="C107" s="32" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="D107" s="32" t="n">
         <v>1</v>
@@ -6695,7 +6691,7 @@
       </c>
       <c r="F107" s="23"/>
       <c r="G107" s="22" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="H107" s="22" t="s">
         <v>27</v>
@@ -6732,10 +6728,10 @@
     </row>
     <row r="108" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B108" s="31" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="C108" s="32" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="D108" s="32" t="n">
         <v>1</v>
@@ -6745,7 +6741,7 @@
       </c>
       <c r="F108" s="23"/>
       <c r="G108" s="22" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="H108" s="22" t="s">
         <v>27</v>
@@ -6782,10 +6778,10 @@
     </row>
     <row r="109" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B109" s="31" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C109" s="32" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="D109" s="32" t="n">
         <v>1</v>
@@ -6795,7 +6791,7 @@
       </c>
       <c r="F109" s="23"/>
       <c r="G109" s="22" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="H109" s="22" t="s">
         <v>27</v>
@@ -6818,7 +6814,7 @@
         <v>17.125</v>
       </c>
       <c r="N109" s="1" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="O109" s="24" t="n">
         <v>9</v>
@@ -6832,10 +6828,10 @@
     </row>
     <row r="110" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B110" s="31" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C110" s="32" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="D110" s="32" t="n">
         <v>1</v>
@@ -6845,7 +6841,7 @@
       </c>
       <c r="F110" s="23"/>
       <c r="G110" s="22" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="H110" s="22" t="s">
         <v>27</v>
@@ -6868,7 +6864,7 @@
         <v>17.15625</v>
       </c>
       <c r="N110" s="1" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="O110" s="24" t="n">
         <v>9</v>
@@ -6882,10 +6878,10 @@
     </row>
     <row r="111" customFormat="false" ht="25.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B111" s="31" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="C111" s="32" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="D111" s="32" t="n">
         <v>1</v>
@@ -6895,7 +6891,7 @@
       </c>
       <c r="F111" s="23"/>
       <c r="G111" s="22" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="H111" s="22" t="s">
         <v>27</v>
@@ -6918,7 +6914,7 @@
         <v>17.1875</v>
       </c>
       <c r="N111" s="1" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="O111" s="24" t="n">
         <v>9</v>
@@ -6932,10 +6928,10 @@
     </row>
     <row r="112" customFormat="false" ht="25.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B112" s="31" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C112" s="32" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="D112" s="32" t="n">
         <v>1</v>
@@ -6945,7 +6941,7 @@
       </c>
       <c r="F112" s="23"/>
       <c r="G112" s="22" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="H112" s="22" t="s">
         <v>27</v>
@@ -6968,7 +6964,7 @@
         <v>17.21875</v>
       </c>
       <c r="N112" s="1" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="O112" s="24" t="n">
         <v>9</v>
@@ -6982,10 +6978,10 @@
     </row>
     <row r="113" customFormat="false" ht="25.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B113" s="31" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="C113" s="32" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="D113" s="32" t="n">
         <v>1</v>
@@ -6995,13 +6991,13 @@
       </c>
       <c r="F113" s="23"/>
       <c r="G113" s="22" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="H113" s="22" t="s">
         <v>27</v>
       </c>
       <c r="I113" s="32" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="J113" s="29" t="n">
         <f aca="false">J112+D112</f>
@@ -7020,7 +7016,7 @@
         <v>17.25</v>
       </c>
       <c r="N113" s="1" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="O113" s="24" t="n">
         <v>9</v>
@@ -7034,10 +7030,10 @@
     </row>
     <row r="114" customFormat="false" ht="25.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B114" s="31" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C114" s="32" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="D114" s="32" t="n">
         <v>1</v>
@@ -7047,7 +7043,7 @@
       </c>
       <c r="F114" s="23"/>
       <c r="G114" s="22" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="H114" s="22" t="s">
         <v>27</v>
@@ -7070,7 +7066,7 @@
         <v>17.28125</v>
       </c>
       <c r="N114" s="1" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="O114" s="24" t="n">
         <v>9</v>
@@ -7084,10 +7080,10 @@
     </row>
     <row r="115" customFormat="false" ht="25.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B115" s="31" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="C115" s="32" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="D115" s="32" t="n">
         <v>1</v>
@@ -7097,7 +7093,7 @@
       </c>
       <c r="F115" s="23"/>
       <c r="G115" s="22" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="H115" s="22" t="s">
         <v>27</v>
@@ -7120,7 +7116,7 @@
         <v>17.3125</v>
       </c>
       <c r="N115" s="1" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="O115" s="24" t="n">
         <v>9</v>
@@ -7134,10 +7130,10 @@
     </row>
     <row r="116" customFormat="false" ht="25.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B116" s="31" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C116" s="32" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="D116" s="32" t="n">
         <v>1</v>
@@ -7147,7 +7143,7 @@
       </c>
       <c r="F116" s="23"/>
       <c r="G116" s="22" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="H116" s="22" t="s">
         <v>27</v>
@@ -7170,7 +7166,7 @@
         <v>17.34375</v>
       </c>
       <c r="N116" s="1" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="O116" s="24" t="n">
         <v>9</v>
@@ -7184,10 +7180,10 @@
     </row>
     <row r="117" customFormat="false" ht="25.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B117" s="31" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="C117" s="32" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="D117" s="32" t="n">
         <v>1</v>
@@ -7197,7 +7193,7 @@
       </c>
       <c r="F117" s="23"/>
       <c r="G117" s="22" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="H117" s="22" t="s">
         <v>27</v>
@@ -7220,7 +7216,7 @@
         <v>17.375</v>
       </c>
       <c r="N117" s="1" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="O117" s="24" t="n">
         <v>9</v>
@@ -7234,10 +7230,10 @@
     </row>
     <row r="118" customFormat="false" ht="25.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B118" s="31" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C118" s="32" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="D118" s="32" t="n">
         <v>1</v>
@@ -7247,7 +7243,7 @@
       </c>
       <c r="F118" s="23"/>
       <c r="G118" s="22" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="H118" s="22" t="s">
         <v>27</v>
@@ -7270,7 +7266,7 @@
         <v>17.40625</v>
       </c>
       <c r="N118" s="1" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="O118" s="24" t="n">
         <v>9</v>
@@ -7284,10 +7280,10 @@
     </row>
     <row r="119" customFormat="false" ht="25.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B119" s="31" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="C119" s="32" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="D119" s="32" t="n">
         <v>1</v>
@@ -7297,7 +7293,7 @@
       </c>
       <c r="F119" s="23"/>
       <c r="G119" s="22" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="H119" s="22" t="s">
         <v>27</v>
@@ -7320,7 +7316,7 @@
         <v>17.4375</v>
       </c>
       <c r="N119" s="1" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="O119" s="24" t="n">
         <v>9</v>
@@ -7334,10 +7330,10 @@
     </row>
     <row r="120" customFormat="false" ht="25.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B120" s="31" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C120" s="32" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="D120" s="32" t="n">
         <v>1</v>
@@ -7347,7 +7343,7 @@
       </c>
       <c r="F120" s="23"/>
       <c r="G120" s="22" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="H120" s="22" t="s">
         <v>27</v>
@@ -7370,7 +7366,7 @@
         <v>17.46875</v>
       </c>
       <c r="N120" s="1" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="O120" s="24" t="n">
         <v>9</v>
@@ -7384,10 +7380,10 @@
     </row>
     <row r="121" customFormat="false" ht="25.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B121" s="31" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="C121" s="32" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="D121" s="32" t="n">
         <v>1</v>
@@ -7397,13 +7393,13 @@
       </c>
       <c r="F121" s="23"/>
       <c r="G121" s="22" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="H121" s="22" t="s">
         <v>27</v>
       </c>
       <c r="I121" s="32" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="J121" s="29" t="n">
         <f aca="false">J120+D120</f>
@@ -7422,7 +7418,7 @@
         <v>17.5</v>
       </c>
       <c r="N121" s="1" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="O121" s="24" t="n">
         <v>9</v>
@@ -7436,10 +7432,10 @@
     </row>
     <row r="122" customFormat="false" ht="25.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B122" s="31" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="C122" s="32" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="D122" s="32" t="n">
         <v>1</v>
@@ -7449,7 +7445,7 @@
       </c>
       <c r="F122" s="23"/>
       <c r="G122" s="22" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="H122" s="22" t="s">
         <v>27</v>
@@ -7472,7 +7468,7 @@
         <v>17.53125</v>
       </c>
       <c r="N122" s="1" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="O122" s="24" t="n">
         <v>9</v>
@@ -7486,10 +7482,10 @@
     </row>
     <row r="123" customFormat="false" ht="25.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B123" s="31" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="C123" s="32" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="D123" s="32" t="n">
         <v>1</v>
@@ -7499,7 +7495,7 @@
       </c>
       <c r="F123" s="23"/>
       <c r="G123" s="22" t="s">
-        <v>318</v>
+        <v>260</v>
       </c>
       <c r="H123" s="22" t="s">
         <v>27</v>
@@ -7522,7 +7518,7 @@
         <v>17.5625</v>
       </c>
       <c r="N123" s="1" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="O123" s="24" t="n">
         <v>9</v>
@@ -7549,7 +7545,7 @@
       </c>
       <c r="F124" s="23"/>
       <c r="G124" s="22" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="H124" s="22" t="s">
         <v>27</v>
@@ -7572,7 +7568,7 @@
         <v>17.59375</v>
       </c>
       <c r="N124" s="1" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="O124" s="24" t="n">
         <v>9</v>
@@ -7586,7 +7582,7 @@
     </row>
     <row r="125" customFormat="false" ht="25.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B125" s="31" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="C125" s="32" t="s">
         <v>321</v>
@@ -7599,7 +7595,7 @@
       </c>
       <c r="F125" s="23"/>
       <c r="G125" s="22" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="H125" s="22" t="s">
         <v>27</v>
@@ -7622,7 +7618,7 @@
         <v>17.625</v>
       </c>
       <c r="N125" s="1" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="O125" s="24" t="n">
         <v>9</v>
@@ -7636,7 +7632,7 @@
     </row>
     <row r="126" customFormat="false" ht="25.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B126" s="31" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="C126" s="32" t="s">
         <v>322</v>
@@ -7649,7 +7645,7 @@
       </c>
       <c r="F126" s="23"/>
       <c r="G126" s="22" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="H126" s="22" t="s">
         <v>27</v>
@@ -7672,7 +7668,7 @@
         <v>17.65625</v>
       </c>
       <c r="N126" s="1" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="O126" s="24" t="n">
         <v>9</v>
@@ -7799,7 +7795,7 @@
       </c>
       <c r="F129" s="23"/>
       <c r="G129" s="22" t="s">
-        <v>318</v>
+        <v>260</v>
       </c>
       <c r="H129" s="22" t="s">
         <v>27</v>
@@ -7849,7 +7845,7 @@
       </c>
       <c r="F130" s="23"/>
       <c r="G130" s="22" t="s">
-        <v>318</v>
+        <v>260</v>
       </c>
       <c r="H130" s="22" t="s">
         <v>27</v>
@@ -7899,7 +7895,7 @@
       </c>
       <c r="F131" s="23"/>
       <c r="G131" s="22" t="s">
-        <v>318</v>
+        <v>260</v>
       </c>
       <c r="H131" s="22" t="s">
         <v>27</v>
@@ -7949,7 +7945,7 @@
       </c>
       <c r="F132" s="23"/>
       <c r="G132" s="22" t="s">
-        <v>318</v>
+        <v>260</v>
       </c>
       <c r="H132" s="22"/>
       <c r="I132" s="32"/>
@@ -7970,7 +7966,7 @@
         <v>17.875</v>
       </c>
       <c r="N132" s="1" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="O132" s="24" t="n">
         <v>9</v>
@@ -8053,7 +8049,7 @@
         <v>27</v>
       </c>
       <c r="I134" s="23" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="J134" s="29" t="n">
         <f aca="false">J133+D133</f>
@@ -8078,7 +8074,7 @@
         <v>2</v>
       </c>
       <c r="P134" s="1" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="Q134" s="1" t="n">
         <v>0</v>
@@ -8759,7 +8755,7 @@
         <v>2</v>
       </c>
       <c r="P148" s="1" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="Q148" s="1" t="n">
         <v>0</v>
@@ -8809,7 +8805,7 @@
         <v>2</v>
       </c>
       <c r="P149" s="1" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="Q149" s="1" t="n">
         <v>0</v>
@@ -10095,7 +10091,7 @@
         <v>2</v>
       </c>
       <c r="P188" s="1" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="Q188" s="1" t="n">
         <v>0</v>
@@ -10147,7 +10143,7 @@
         <v>2</v>
       </c>
       <c r="P189" s="1" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="Q189" s="1" t="n">
         <v>0</v>
@@ -10199,7 +10195,7 @@
         <v>2</v>
       </c>
       <c r="P190" s="1" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Q190" s="1" t="n">
         <v>0</v>
@@ -11023,7 +11019,7 @@
         <v>27</v>
       </c>
       <c r="I215" s="28" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="J215" s="4" t="n">
         <f aca="false">J214+D214</f>
@@ -13158,10 +13154,10 @@
   <dimension ref="B6:Q1031"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C33" activeCellId="0" sqref="C33"/>
+      <selection pane="topLeft" activeCell="C33" activeCellId="1" sqref="G97 C33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.0390625" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.0546875" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="40" width="20.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="40" width="16.11"/>
@@ -13184,7 +13180,7 @@
         <v>505</v>
       </c>
       <c r="G6" s="50" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="H6" s="50" t="s">
         <v>506</v>

</xml_diff>

<commit_message>
Add spacecraft time in seconds to match with UTC
</commit_message>
<xml_diff>
--- a/genSpacecraft/DownlinkSpecLTM.xlsx
+++ b/genSpacecraft/DownlinkSpecLTM.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1394" uniqueCount="515">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1401" uniqueCount="518">
   <si>
     <t xml:space="preserve">//</t>
   </si>
@@ -1341,6 +1341,15 @@
   </si>
   <si>
     <t xml:space="preserve">General Info</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SecondsInEpoch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">secsInEpoch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seconds within current Epoch</t>
   </si>
   <si>
     <t xml:space="preserve">#ifdef LEGACY_IHU</t>
@@ -1941,10 +1950,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q263"/>
+  <dimension ref="A1:Q264"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A82" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G97" activeCellId="0" sqref="G97"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A211" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Q221" activeCellId="0" sqref="Q221"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11196,73 +11205,73 @@
       </c>
     </row>
     <row r="221" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A221" s="1" t="s">
+      <c r="B221" s="43" t="s">
         <v>440</v>
       </c>
-      <c r="B221" s="43"/>
-      <c r="C221" s="38"/>
-      <c r="D221" s="38"/>
-      <c r="E221" s="38"/>
+      <c r="C221" s="38" t="s">
+        <v>441</v>
+      </c>
+      <c r="D221" s="38" t="n">
+        <v>32</v>
+      </c>
+      <c r="E221" s="38" t="s">
+        <v>26</v>
+      </c>
       <c r="F221" s="38"/>
-      <c r="G221" s="38"/>
-      <c r="H221" s="38"/>
-      <c r="I221" s="38"/>
-      <c r="J221" s="44"/>
-      <c r="K221" s="38"/>
-      <c r="L221" s="28"/>
-      <c r="M221" s="28"/>
-    </row>
-    <row r="222" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B222" s="43" t="s">
-        <v>441</v>
-      </c>
-      <c r="C222" s="38" t="s">
-        <v>441</v>
-      </c>
-      <c r="D222" s="38" t="n">
-        <v>1</v>
-      </c>
-      <c r="E222" s="38" t="s">
-        <v>26</v>
-      </c>
-      <c r="F222" s="38"/>
-      <c r="G222" s="38" t="s">
+      <c r="G221" s="38" t="s">
+        <v>133</v>
+      </c>
+      <c r="H221" s="38" t="s">
+        <v>437</v>
+      </c>
+      <c r="I221" s="38" t="s">
         <v>442</v>
       </c>
-      <c r="H222" s="38" t="s">
-        <v>27</v>
-      </c>
-      <c r="I222" s="38" t="s">
-        <v>443</v>
-      </c>
-      <c r="J222" s="44" t="n">
+      <c r="J221" s="44" t="n">
         <f aca="false">J220+D220</f>
         <v>32</v>
       </c>
-      <c r="K222" s="38" t="n">
-        <f aca="false">J222/8</f>
+      <c r="K221" s="38" t="n">
+        <f aca="false">J221/8</f>
         <v>4</v>
       </c>
-      <c r="L222" s="28" t="n">
-        <f aca="false">J222/16</f>
+      <c r="L221" s="28" t="n">
+        <f aca="false">J221/16</f>
         <v>2</v>
       </c>
-      <c r="M222" s="28" t="n">
-        <f aca="false">J222/32</f>
+      <c r="M221" s="28" t="n">
+        <f aca="false">J221/32</f>
         <v>1</v>
       </c>
-      <c r="N222" s="1" t="s">
+      <c r="N221" s="1" t="s">
         <v>439</v>
       </c>
-      <c r="O222" s="3" t="n">
+      <c r="O221" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="P222" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="Q222" s="1" t="n">
-        <v>0</v>
-      </c>
+      <c r="P221" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q221" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="222" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A222" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="B222" s="43"/>
+      <c r="C222" s="38"/>
+      <c r="D222" s="38"/>
+      <c r="E222" s="38"/>
+      <c r="F222" s="38"/>
+      <c r="G222" s="38"/>
+      <c r="H222" s="38"/>
+      <c r="I222" s="38"/>
+      <c r="J222" s="44"/>
+      <c r="K222" s="38"/>
+      <c r="L222" s="28"/>
+      <c r="M222" s="28"/>
     </row>
     <row r="223" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B223" s="43" t="s">
@@ -11272,34 +11281,36 @@
         <v>444</v>
       </c>
       <c r="D223" s="38" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E223" s="38" t="s">
         <v>26</v>
       </c>
       <c r="F223" s="38"/>
       <c r="G223" s="38" t="s">
-        <v>133</v>
-      </c>
-      <c r="H223" s="38"/>
+        <v>445</v>
+      </c>
+      <c r="H223" s="38" t="s">
+        <v>27</v>
+      </c>
       <c r="I223" s="38" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="J223" s="44" t="n">
-        <f aca="false">J222+D222</f>
-        <v>33</v>
+        <f aca="false">J221+D221</f>
+        <v>64</v>
       </c>
       <c r="K223" s="38" t="n">
         <f aca="false">J223/8</f>
-        <v>4.125</v>
+        <v>8</v>
       </c>
       <c r="L223" s="28" t="n">
         <f aca="false">J223/16</f>
-        <v>2.0625</v>
+        <v>4</v>
       </c>
       <c r="M223" s="28" t="n">
         <f aca="false">J223/32</f>
-        <v>1.03125</v>
+        <v>2</v>
       </c>
       <c r="N223" s="1" t="s">
         <v>439</v>
@@ -11308,7 +11319,7 @@
         <v>1</v>
       </c>
       <c r="P223" s="1" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="Q223" s="1" t="n">
         <v>0</v>
@@ -11316,13 +11327,13 @@
     </row>
     <row r="224" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B224" s="43" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="C224" s="38" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="D224" s="38" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E224" s="38" t="s">
         <v>26</v>
@@ -11331,27 +11342,25 @@
       <c r="G224" s="38" t="s">
         <v>133</v>
       </c>
-      <c r="H224" s="38" t="s">
-        <v>27</v>
-      </c>
+      <c r="H224" s="38"/>
       <c r="I224" s="38" t="s">
-        <v>443</v>
+        <v>448</v>
       </c>
       <c r="J224" s="44" t="n">
         <f aca="false">J223+D223</f>
-        <v>38</v>
+        <v>65</v>
       </c>
       <c r="K224" s="38" t="n">
         <f aca="false">J224/8</f>
-        <v>4.75</v>
+        <v>8.125</v>
       </c>
       <c r="L224" s="28" t="n">
         <f aca="false">J224/16</f>
-        <v>2.375</v>
+        <v>4.0625</v>
       </c>
       <c r="M224" s="28" t="n">
         <f aca="false">J224/32</f>
-        <v>1.1875</v>
+        <v>2.03125</v>
       </c>
       <c r="N224" s="1" t="s">
         <v>439</v>
@@ -11360,7 +11369,7 @@
         <v>1</v>
       </c>
       <c r="P224" s="1" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="Q224" s="1" t="n">
         <v>0</v>
@@ -11368,13 +11377,13 @@
     </row>
     <row r="225" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B225" s="43" t="s">
-        <v>447</v>
+        <v>449</v>
       </c>
       <c r="C225" s="38" t="s">
-        <v>447</v>
+        <v>449</v>
       </c>
       <c r="D225" s="38" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E225" s="38" t="s">
         <v>26</v>
@@ -11387,23 +11396,23 @@
         <v>27</v>
       </c>
       <c r="I225" s="38" t="s">
-        <v>443</v>
+        <v>446</v>
       </c>
       <c r="J225" s="44" t="n">
         <f aca="false">J224+D224</f>
-        <v>42</v>
+        <v>70</v>
       </c>
       <c r="K225" s="38" t="n">
         <f aca="false">J225/8</f>
-        <v>5.25</v>
+        <v>8.75</v>
       </c>
       <c r="L225" s="28" t="n">
         <f aca="false">J225/16</f>
-        <v>2.625</v>
+        <v>4.375</v>
       </c>
       <c r="M225" s="28" t="n">
         <f aca="false">J225/32</f>
-        <v>1.3125</v>
+        <v>2.1875</v>
       </c>
       <c r="N225" s="1" t="s">
         <v>439</v>
@@ -11412,7 +11421,7 @@
         <v>1</v>
       </c>
       <c r="P225" s="1" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="Q225" s="1" t="n">
         <v>0</v>
@@ -11420,13 +11429,13 @@
     </row>
     <row r="226" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B226" s="43" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="C226" s="38" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="D226" s="38" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E226" s="38" t="s">
         <v>26</v>
@@ -11439,23 +11448,23 @@
         <v>27</v>
       </c>
       <c r="I226" s="38" t="s">
-        <v>443</v>
+        <v>446</v>
       </c>
       <c r="J226" s="44" t="n">
         <f aca="false">J225+D225</f>
-        <v>47</v>
+        <v>74</v>
       </c>
       <c r="K226" s="38" t="n">
         <f aca="false">J226/8</f>
-        <v>5.875</v>
+        <v>9.25</v>
       </c>
       <c r="L226" s="28" t="n">
         <f aca="false">J226/16</f>
-        <v>2.9375</v>
+        <v>4.625</v>
       </c>
       <c r="M226" s="28" t="n">
         <f aca="false">J226/32</f>
-        <v>1.46875</v>
+        <v>2.3125</v>
       </c>
       <c r="N226" s="1" t="s">
         <v>439</v>
@@ -11464,7 +11473,7 @@
         <v>1</v>
       </c>
       <c r="P226" s="1" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="Q226" s="1" t="n">
         <v>0</v>
@@ -11472,10 +11481,10 @@
     </row>
     <row r="227" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B227" s="43" t="s">
-        <v>449</v>
+        <v>451</v>
       </c>
       <c r="C227" s="38" t="s">
-        <v>449</v>
+        <v>451</v>
       </c>
       <c r="D227" s="38" t="n">
         <v>6</v>
@@ -11491,23 +11500,23 @@
         <v>27</v>
       </c>
       <c r="I227" s="38" t="s">
-        <v>443</v>
+        <v>446</v>
       </c>
       <c r="J227" s="44" t="n">
         <f aca="false">J226+D226</f>
-        <v>53</v>
+        <v>79</v>
       </c>
       <c r="K227" s="38" t="n">
         <f aca="false">J227/8</f>
-        <v>6.625</v>
+        <v>9.875</v>
       </c>
       <c r="L227" s="28" t="n">
         <f aca="false">J227/16</f>
-        <v>3.3125</v>
+        <v>4.9375</v>
       </c>
       <c r="M227" s="28" t="n">
         <f aca="false">J227/32</f>
-        <v>1.65625</v>
+        <v>2.46875</v>
       </c>
       <c r="N227" s="1" t="s">
         <v>439</v>
@@ -11516,7 +11525,7 @@
         <v>1</v>
       </c>
       <c r="P227" s="1" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="Q227" s="1" t="n">
         <v>0</v>
@@ -11524,13 +11533,13 @@
     </row>
     <row r="228" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B228" s="43" t="s">
-        <v>450</v>
+        <v>452</v>
       </c>
       <c r="C228" s="38" t="s">
-        <v>450</v>
+        <v>452</v>
       </c>
       <c r="D228" s="38" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E228" s="38" t="s">
         <v>26</v>
@@ -11543,23 +11552,23 @@
         <v>27</v>
       </c>
       <c r="I228" s="38" t="s">
-        <v>443</v>
+        <v>446</v>
       </c>
       <c r="J228" s="44" t="n">
         <f aca="false">J227+D227</f>
-        <v>59</v>
+        <v>85</v>
       </c>
       <c r="K228" s="38" t="n">
         <f aca="false">J228/8</f>
-        <v>7.375</v>
+        <v>10.625</v>
       </c>
       <c r="L228" s="28" t="n">
         <f aca="false">J228/16</f>
-        <v>3.6875</v>
+        <v>5.3125</v>
       </c>
       <c r="M228" s="28" t="n">
         <f aca="false">J228/32</f>
-        <v>1.84375</v>
+        <v>2.65625</v>
       </c>
       <c r="N228" s="1" t="s">
         <v>439</v>
@@ -11568,87 +11577,87 @@
         <v>1</v>
       </c>
       <c r="P228" s="1" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="Q228" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="229" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A229" s="1" t="s">
-        <v>451</v>
-      </c>
-      <c r="B229" s="43"/>
-      <c r="C229" s="38"/>
-      <c r="D229" s="38"/>
-      <c r="E229" s="38"/>
+      <c r="B229" s="43" t="s">
+        <v>453</v>
+      </c>
+      <c r="C229" s="38" t="s">
+        <v>453</v>
+      </c>
+      <c r="D229" s="38" t="n">
+        <v>5</v>
+      </c>
+      <c r="E229" s="38" t="s">
+        <v>26</v>
+      </c>
       <c r="F229" s="38"/>
-      <c r="G229" s="38"/>
-      <c r="H229" s="38"/>
-      <c r="I229" s="38"/>
-      <c r="J229" s="44"/>
-      <c r="K229" s="38"/>
-      <c r="L229" s="28"/>
-      <c r="M229" s="28"/>
+      <c r="G229" s="38" t="s">
+        <v>133</v>
+      </c>
+      <c r="H229" s="38" t="s">
+        <v>27</v>
+      </c>
+      <c r="I229" s="38" t="s">
+        <v>446</v>
+      </c>
+      <c r="J229" s="44" t="n">
+        <f aca="false">J228+D228</f>
+        <v>91</v>
+      </c>
+      <c r="K229" s="38" t="n">
+        <f aca="false">J229/8</f>
+        <v>11.375</v>
+      </c>
+      <c r="L229" s="28" t="n">
+        <f aca="false">J229/16</f>
+        <v>5.6875</v>
+      </c>
+      <c r="M229" s="28" t="n">
+        <f aca="false">J229/32</f>
+        <v>2.84375</v>
+      </c>
+      <c r="N229" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="O229" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="P229" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q229" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="230" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B230" s="43" t="s">
-        <v>452</v>
-      </c>
-      <c r="C230" s="38" t="s">
-        <v>452</v>
-      </c>
-      <c r="D230" s="38" t="n">
-        <v>8</v>
-      </c>
-      <c r="E230" s="38" t="s">
-        <v>26</v>
-      </c>
+      <c r="A230" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="B230" s="43"/>
+      <c r="C230" s="38"/>
+      <c r="D230" s="38"/>
+      <c r="E230" s="38"/>
       <c r="F230" s="38"/>
-      <c r="G230" s="38" t="s">
-        <v>138</v>
-      </c>
-      <c r="H230" s="38" t="s">
-        <v>71</v>
-      </c>
-      <c r="I230" s="38" t="s">
-        <v>443</v>
-      </c>
-      <c r="J230" s="44" t="n">
-        <f aca="false">J228+D228</f>
-        <v>64</v>
-      </c>
-      <c r="K230" s="38" t="n">
-        <f aca="false">J230/8</f>
-        <v>8</v>
-      </c>
-      <c r="L230" s="28" t="n">
-        <f aca="false">J230/16</f>
-        <v>4</v>
-      </c>
-      <c r="M230" s="28" t="n">
-        <f aca="false">J230/32</f>
-        <v>2</v>
-      </c>
-      <c r="N230" s="1" t="s">
-        <v>439</v>
-      </c>
-      <c r="O230" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="P230" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="Q230" s="1" t="n">
-        <v>0</v>
-      </c>
+      <c r="G230" s="38"/>
+      <c r="H230" s="38"/>
+      <c r="I230" s="38"/>
+      <c r="J230" s="44"/>
+      <c r="K230" s="38"/>
+      <c r="L230" s="28"/>
+      <c r="M230" s="28"/>
     </row>
     <row r="231" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B231" s="43" t="s">
-        <v>453</v>
+        <v>455</v>
       </c>
       <c r="C231" s="38" t="s">
-        <v>453</v>
+        <v>455</v>
       </c>
       <c r="D231" s="38" t="n">
         <v>8</v>
@@ -11664,23 +11673,23 @@
         <v>71</v>
       </c>
       <c r="I231" s="38" t="s">
-        <v>443</v>
+        <v>446</v>
       </c>
       <c r="J231" s="44" t="n">
-        <f aca="false">J230+D230</f>
-        <v>72</v>
+        <f aca="false">J229+D229</f>
+        <v>96</v>
       </c>
       <c r="K231" s="38" t="n">
         <f aca="false">J231/8</f>
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="L231" s="28" t="n">
         <f aca="false">J231/16</f>
-        <v>4.5</v>
+        <v>6</v>
       </c>
       <c r="M231" s="28" t="n">
         <f aca="false">J231/32</f>
-        <v>2.25</v>
+        <v>3</v>
       </c>
       <c r="N231" s="1" t="s">
         <v>439</v>
@@ -11697,269 +11706,269 @@
     </row>
     <row r="232" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B232" s="43" t="s">
-        <v>454</v>
+        <v>456</v>
       </c>
       <c r="C232" s="38" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="D232" s="38" t="n">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E232" s="38" t="s">
         <v>26</v>
       </c>
       <c r="F232" s="38"/>
-      <c r="G232" s="38" t="n">
-        <v>0</v>
+      <c r="G232" s="38" t="s">
+        <v>138</v>
       </c>
       <c r="H232" s="38" t="s">
-        <v>27</v>
+        <v>71</v>
       </c>
       <c r="I232" s="38" t="s">
-        <v>443</v>
+        <v>446</v>
       </c>
       <c r="J232" s="44" t="n">
         <f aca="false">J231+D231</f>
-        <v>80</v>
+        <v>104</v>
       </c>
       <c r="K232" s="38" t="n">
         <f aca="false">J232/8</f>
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="L232" s="28" t="n">
         <f aca="false">J232/16</f>
-        <v>5</v>
+        <v>6.5</v>
       </c>
       <c r="M232" s="28" t="n">
         <f aca="false">J232/32</f>
-        <v>2.5</v>
+        <v>3.25</v>
       </c>
       <c r="N232" s="1" t="s">
-        <v>28</v>
+        <v>439</v>
       </c>
       <c r="O232" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P232" s="1" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="Q232" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="233" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A233" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B233" s="43"/>
-      <c r="C233" s="38"/>
-      <c r="D233" s="38"/>
+      <c r="B233" s="43" t="s">
+        <v>457</v>
+      </c>
+      <c r="C233" s="38" t="s">
+        <v>458</v>
+      </c>
+      <c r="D233" s="38" t="n">
+        <v>16</v>
+      </c>
+      <c r="E233" s="38" t="s">
+        <v>26</v>
+      </c>
       <c r="F233" s="38"/>
-      <c r="G233" s="38"/>
-      <c r="H233" s="38"/>
+      <c r="G233" s="38" t="n">
+        <v>0</v>
+      </c>
+      <c r="H233" s="38" t="s">
+        <v>27</v>
+      </c>
       <c r="I233" s="38" t="s">
-        <v>233</v>
+        <v>446</v>
       </c>
       <c r="J233" s="44" t="n">
         <f aca="false">J232+D232</f>
-        <v>96</v>
+        <v>112</v>
       </c>
       <c r="K233" s="38" t="n">
         <f aca="false">J233/8</f>
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="L233" s="28" t="n">
         <f aca="false">J233/16</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M233" s="28" t="n">
         <f aca="false">J233/32</f>
-        <v>3</v>
+        <v>3.5</v>
+      </c>
+      <c r="N233" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O233" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P233" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q233" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="234" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A234" s="42" t="s">
-        <v>456</v>
-      </c>
+      <c r="A234" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B234" s="43"/>
+      <c r="C234" s="38"/>
+      <c r="D234" s="38"/>
       <c r="F234" s="38"/>
       <c r="G234" s="38"/>
       <c r="H234" s="38"/>
-      <c r="I234" s="38"/>
-      <c r="J234" s="44"/>
-      <c r="K234" s="38"/>
-      <c r="L234" s="28"/>
-      <c r="M234" s="28"/>
-    </row>
-    <row r="235" s="14" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A235" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="B235" s="15" t="s">
+      <c r="I234" s="38" t="s">
+        <v>233</v>
+      </c>
+      <c r="J234" s="44" t="n">
+        <f aca="false">J233+D233</f>
+        <v>128</v>
+      </c>
+      <c r="K234" s="38" t="n">
+        <f aca="false">J234/8</f>
+        <v>16</v>
+      </c>
+      <c r="L234" s="28" t="n">
+        <f aca="false">J234/16</f>
         <v>8</v>
       </c>
-      <c r="C235" s="12" t="s">
+      <c r="M234" s="28" t="n">
+        <f aca="false">J234/32</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="235" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A235" s="42" t="s">
+        <v>459</v>
+      </c>
+      <c r="F235" s="38"/>
+      <c r="G235" s="38"/>
+      <c r="H235" s="38"/>
+      <c r="I235" s="38"/>
+      <c r="J235" s="44"/>
+      <c r="K235" s="38"/>
+      <c r="L235" s="28"/>
+      <c r="M235" s="28"/>
+    </row>
+    <row r="236" s="14" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A236" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B236" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C236" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="D235" s="12" t="s">
+      <c r="D236" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="E235" s="12" t="s">
+      <c r="E236" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="F235" s="12" t="s">
+      <c r="F236" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="G235" s="12" t="s">
+      <c r="G236" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="H235" s="12" t="s">
+      <c r="H236" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="I235" s="13" t="s">
+      <c r="I236" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="J235" s="30" t="s">
+      <c r="J236" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="K235" s="14" t="s">
+      <c r="K236" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="L235" s="14" t="s">
+      <c r="L236" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="M235" s="14" t="s">
+      <c r="M236" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="N235" s="19" t="s">
+      <c r="N236" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="O235" s="20" t="s">
+      <c r="O236" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="P235" s="14" t="s">
+      <c r="P236" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="Q235" s="14" t="s">
+      <c r="Q236" s="14" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="236" s="47" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A236" s="1" t="s">
+    <row r="237" s="47" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A237" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B236" s="21"/>
-      <c r="C236" s="45"/>
-      <c r="D236" s="1"/>
-      <c r="E236" s="38"/>
-      <c r="F236" s="46"/>
-      <c r="G236" s="38"/>
-      <c r="H236" s="38"/>
-      <c r="I236" s="38"/>
-      <c r="J236" s="44"/>
-      <c r="K236" s="28"/>
-      <c r="L236" s="28"/>
-      <c r="M236" s="28"/>
-      <c r="O236" s="3"/>
-    </row>
-    <row r="237" s="47" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B237" s="21" t="s">
-        <v>457</v>
-      </c>
-      <c r="C237" s="45" t="s">
-        <v>458</v>
-      </c>
-      <c r="D237" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="E237" s="38" t="s">
-        <v>26</v>
-      </c>
+      <c r="B237" s="21"/>
+      <c r="C237" s="45"/>
+      <c r="D237" s="1"/>
+      <c r="E237" s="38"/>
       <c r="F237" s="46"/>
-      <c r="G237" s="38" t="n">
-        <v>0</v>
-      </c>
-      <c r="H237" s="38" t="s">
-        <v>27</v>
-      </c>
-      <c r="I237" s="38" t="s">
-        <v>443</v>
-      </c>
-      <c r="J237" s="44" t="n">
-        <f aca="false">J233</f>
-        <v>96</v>
-      </c>
-      <c r="K237" s="28" t="n">
-        <f aca="false">J237/8</f>
-        <v>12</v>
-      </c>
-      <c r="L237" s="28" t="n">
-        <f aca="false">J237/16</f>
-        <v>6</v>
-      </c>
-      <c r="M237" s="28" t="n">
-        <f aca="false">J237/32</f>
-        <v>3</v>
-      </c>
-      <c r="N237" s="47" t="s">
-        <v>28</v>
-      </c>
-      <c r="O237" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="P237" s="47" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q237" s="47" t="n">
-        <v>0</v>
-      </c>
+      <c r="G237" s="38"/>
+      <c r="H237" s="38"/>
+      <c r="I237" s="38"/>
+      <c r="J237" s="44"/>
+      <c r="K237" s="28"/>
+      <c r="L237" s="28"/>
+      <c r="M237" s="28"/>
+      <c r="O237" s="3"/>
     </row>
     <row r="238" s="47" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B238" s="21" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="C238" s="45" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="D238" s="1" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E238" s="38" t="s">
         <v>26</v>
       </c>
       <c r="F238" s="46"/>
-      <c r="G238" s="38" t="s">
-        <v>442</v>
+      <c r="G238" s="38" t="n">
+        <v>0</v>
       </c>
       <c r="H238" s="38" t="s">
         <v>27</v>
       </c>
       <c r="I238" s="38" t="s">
-        <v>443</v>
+        <v>446</v>
       </c>
       <c r="J238" s="44" t="n">
-        <f aca="false">J237+D237</f>
-        <v>101</v>
+        <f aca="false">J234</f>
+        <v>128</v>
       </c>
       <c r="K238" s="28" t="n">
         <f aca="false">J238/8</f>
-        <v>12.625</v>
+        <v>16</v>
       </c>
       <c r="L238" s="28" t="n">
         <f aca="false">J238/16</f>
-        <v>6.3125</v>
+        <v>8</v>
       </c>
       <c r="M238" s="28" t="n">
         <f aca="false">J238/32</f>
-        <v>3.15625</v>
-      </c>
-      <c r="N238" s="1" t="s">
-        <v>439</v>
+        <v>4</v>
+      </c>
+      <c r="N238" s="47" t="s">
+        <v>28</v>
       </c>
       <c r="O238" s="3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P238" s="47" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q238" s="47" t="n">
         <v>0</v>
@@ -11967,10 +11976,10 @@
     </row>
     <row r="239" s="47" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B239" s="21" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="C239" s="45" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="D239" s="1" t="n">
         <v>1</v>
@@ -11980,38 +11989,38 @@
       </c>
       <c r="F239" s="46"/>
       <c r="G239" s="38" t="s">
-        <v>442</v>
+        <v>445</v>
       </c>
       <c r="H239" s="38" t="s">
         <v>27</v>
       </c>
       <c r="I239" s="38" t="s">
-        <v>443</v>
+        <v>446</v>
       </c>
       <c r="J239" s="44" t="n">
         <f aca="false">J238+D238</f>
-        <v>102</v>
+        <v>133</v>
       </c>
       <c r="K239" s="28" t="n">
         <f aca="false">J239/8</f>
-        <v>12.75</v>
+        <v>16.625</v>
       </c>
       <c r="L239" s="28" t="n">
         <f aca="false">J239/16</f>
-        <v>6.375</v>
+        <v>8.3125</v>
       </c>
       <c r="M239" s="28" t="n">
         <f aca="false">J239/32</f>
-        <v>3.1875</v>
+        <v>4.15625</v>
       </c>
       <c r="N239" s="1" t="s">
-        <v>463</v>
+        <v>439</v>
       </c>
       <c r="O239" s="3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P239" s="47" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="Q239" s="47" t="n">
         <v>0</v>
@@ -12025,45 +12034,45 @@
         <v>465</v>
       </c>
       <c r="D240" s="1" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E240" s="38" t="s">
         <v>26</v>
       </c>
       <c r="F240" s="46"/>
       <c r="G240" s="38" t="s">
-        <v>133</v>
+        <v>445</v>
       </c>
       <c r="H240" s="38" t="s">
         <v>27</v>
       </c>
       <c r="I240" s="38" t="s">
-        <v>443</v>
+        <v>446</v>
       </c>
       <c r="J240" s="44" t="n">
         <f aca="false">J239+D239</f>
-        <v>103</v>
+        <v>134</v>
       </c>
       <c r="K240" s="28" t="n">
         <f aca="false">J240/8</f>
-        <v>12.875</v>
+        <v>16.75</v>
       </c>
       <c r="L240" s="28" t="n">
         <f aca="false">J240/16</f>
-        <v>6.4375</v>
+        <v>8.375</v>
       </c>
       <c r="M240" s="28" t="n">
         <f aca="false">J240/32</f>
-        <v>3.21875</v>
+        <v>4.1875</v>
       </c>
       <c r="N240" s="1" t="s">
-        <v>463</v>
+        <v>466</v>
       </c>
       <c r="O240" s="3" t="n">
         <v>2</v>
       </c>
       <c r="P240" s="47" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="Q240" s="47" t="n">
         <v>0</v>
@@ -12071,51 +12080,51 @@
     </row>
     <row r="241" s="47" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B241" s="21" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="C241" s="45" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="D241" s="1" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E241" s="38" t="s">
         <v>26</v>
       </c>
       <c r="F241" s="46"/>
       <c r="G241" s="38" t="s">
-        <v>468</v>
+        <v>133</v>
       </c>
       <c r="H241" s="38" t="s">
         <v>27</v>
       </c>
       <c r="I241" s="38" t="s">
-        <v>443</v>
+        <v>446</v>
       </c>
       <c r="J241" s="44" t="n">
         <f aca="false">J240+D240</f>
-        <v>106</v>
+        <v>135</v>
       </c>
       <c r="K241" s="28" t="n">
         <f aca="false">J241/8</f>
-        <v>13.25</v>
+        <v>16.875</v>
       </c>
       <c r="L241" s="28" t="n">
         <f aca="false">J241/16</f>
-        <v>6.625</v>
+        <v>8.4375</v>
       </c>
       <c r="M241" s="28" t="n">
         <f aca="false">J241/32</f>
-        <v>3.3125</v>
+        <v>4.21875</v>
       </c>
       <c r="N241" s="1" t="s">
-        <v>463</v>
+        <v>466</v>
       </c>
       <c r="O241" s="3" t="n">
         <v>2</v>
       </c>
       <c r="P241" s="47" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="Q241" s="47" t="n">
         <v>0</v>
@@ -12136,38 +12145,38 @@
       </c>
       <c r="F242" s="46"/>
       <c r="G242" s="38" t="s">
-        <v>468</v>
+        <v>471</v>
       </c>
       <c r="H242" s="38" t="s">
         <v>27</v>
       </c>
       <c r="I242" s="38" t="s">
-        <v>443</v>
+        <v>446</v>
       </c>
       <c r="J242" s="44" t="n">
         <f aca="false">J241+D241</f>
-        <v>110</v>
+        <v>138</v>
       </c>
       <c r="K242" s="28" t="n">
         <f aca="false">J242/8</f>
-        <v>13.75</v>
+        <v>17.25</v>
       </c>
       <c r="L242" s="28" t="n">
         <f aca="false">J242/16</f>
-        <v>6.875</v>
+        <v>8.625</v>
       </c>
       <c r="M242" s="28" t="n">
         <f aca="false">J242/32</f>
-        <v>3.4375</v>
+        <v>4.3125</v>
       </c>
       <c r="N242" s="1" t="s">
-        <v>463</v>
+        <v>466</v>
       </c>
       <c r="O242" s="3" t="n">
         <v>2</v>
       </c>
       <c r="P242" s="47" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="Q242" s="47" t="n">
         <v>0</v>
@@ -12175,51 +12184,51 @@
     </row>
     <row r="243" s="47" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B243" s="21" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="C243" s="45" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="D243" s="1" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E243" s="38" t="s">
         <v>26</v>
       </c>
       <c r="F243" s="46"/>
       <c r="G243" s="38" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="H243" s="38" t="s">
         <v>27</v>
       </c>
       <c r="I243" s="38" t="s">
-        <v>443</v>
+        <v>446</v>
       </c>
       <c r="J243" s="44" t="n">
         <f aca="false">J242+D242</f>
-        <v>114</v>
+        <v>142</v>
       </c>
       <c r="K243" s="28" t="n">
         <f aca="false">J243/8</f>
-        <v>14.25</v>
+        <v>17.75</v>
       </c>
       <c r="L243" s="28" t="n">
         <f aca="false">J243/16</f>
-        <v>7.125</v>
+        <v>8.875</v>
       </c>
       <c r="M243" s="28" t="n">
         <f aca="false">J243/32</f>
-        <v>3.5625</v>
+        <v>4.4375</v>
       </c>
       <c r="N243" s="1" t="s">
-        <v>463</v>
+        <v>466</v>
       </c>
       <c r="O243" s="3" t="n">
         <v>2</v>
       </c>
       <c r="P243" s="47" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="Q243" s="47" t="n">
         <v>0</v>
@@ -12233,120 +12242,120 @@
         <v>475</v>
       </c>
       <c r="D244" s="1" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E244" s="38" t="s">
         <v>26</v>
       </c>
       <c r="F244" s="46"/>
       <c r="G244" s="38" t="s">
-        <v>133</v>
+        <v>476</v>
       </c>
       <c r="H244" s="38" t="s">
         <v>27</v>
       </c>
       <c r="I244" s="38" t="s">
-        <v>443</v>
+        <v>446</v>
       </c>
       <c r="J244" s="44" t="n">
         <f aca="false">J243+D243</f>
-        <v>119</v>
+        <v>146</v>
       </c>
       <c r="K244" s="28" t="n">
         <f aca="false">J244/8</f>
-        <v>14.875</v>
+        <v>18.25</v>
       </c>
       <c r="L244" s="28" t="n">
         <f aca="false">J244/16</f>
-        <v>7.4375</v>
+        <v>9.125</v>
       </c>
       <c r="M244" s="28" t="n">
         <f aca="false">J244/32</f>
-        <v>3.71875</v>
+        <v>4.5625</v>
       </c>
       <c r="N244" s="1" t="s">
-        <v>463</v>
+        <v>466</v>
       </c>
       <c r="O244" s="3" t="n">
         <v>2</v>
       </c>
       <c r="P244" s="47" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q244" s="47" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="245" s="47" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B245" s="21" t="s">
+        <v>477</v>
+      </c>
+      <c r="C245" s="45" t="s">
+        <v>478</v>
+      </c>
+      <c r="D245" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="E245" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="F245" s="46"/>
+      <c r="G245" s="38" t="s">
+        <v>133</v>
+      </c>
+      <c r="H245" s="38" t="s">
+        <v>27</v>
+      </c>
+      <c r="I245" s="38" t="s">
+        <v>446</v>
+      </c>
+      <c r="J245" s="44" t="n">
+        <f aca="false">J244+D244</f>
+        <v>151</v>
+      </c>
+      <c r="K245" s="28" t="n">
+        <f aca="false">J245/8</f>
+        <v>18.875</v>
+      </c>
+      <c r="L245" s="28" t="n">
+        <f aca="false">J245/16</f>
+        <v>9.4375</v>
+      </c>
+      <c r="M245" s="28" t="n">
+        <f aca="false">J245/32</f>
+        <v>4.71875</v>
+      </c>
+      <c r="N245" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="O245" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="P245" s="47" t="n">
         <v>1</v>
       </c>
-      <c r="Q244" s="47" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="245" s="47" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A245" s="47" t="s">
+      <c r="Q245" s="47" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="246" s="47" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A246" s="47" t="s">
         <v>58</v>
       </c>
-      <c r="B245" s="21"/>
-      <c r="C245" s="45"/>
-      <c r="D245" s="1"/>
-      <c r="E245" s="38"/>
-      <c r="F245" s="46"/>
-      <c r="G245" s="38"/>
-      <c r="H245" s="38"/>
-      <c r="I245" s="38"/>
-      <c r="J245" s="44"/>
-      <c r="K245" s="28"/>
-      <c r="L245" s="28"/>
-      <c r="M245" s="28"/>
-      <c r="N245" s="40"/>
-      <c r="O245" s="3"/>
-    </row>
-    <row r="246" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B246" s="47" t="s">
-        <v>476</v>
-      </c>
-      <c r="C246" s="3" t="s">
-        <v>477</v>
-      </c>
-      <c r="D246" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="E246" s="38" t="s">
-        <v>26</v>
-      </c>
-      <c r="F246" s="38"/>
-      <c r="G246" s="38" t="s">
-        <v>133</v>
-      </c>
-      <c r="H246" s="38" t="s">
-        <v>27</v>
-      </c>
-      <c r="I246" s="38" t="s">
-        <v>443</v>
-      </c>
-      <c r="J246" s="44" t="n">
-        <f aca="false">J244+D244</f>
-        <v>128</v>
-      </c>
-      <c r="K246" s="28" t="n">
-        <f aca="false">J246/8</f>
-        <v>16</v>
-      </c>
-      <c r="L246" s="28" t="n">
-        <f aca="false">J246/16</f>
-        <v>8</v>
-      </c>
-      <c r="M246" s="28" t="n">
-        <f aca="false">J246/32</f>
-        <v>4</v>
-      </c>
-      <c r="N246" s="1" t="s">
-        <v>478</v>
-      </c>
-      <c r="O246" s="3" t="n">
-        <v>3</v>
-      </c>
-      <c r="P246" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q246" s="1" t="n">
-        <v>0</v>
-      </c>
+      <c r="B246" s="21"/>
+      <c r="C246" s="45"/>
+      <c r="D246" s="1"/>
+      <c r="E246" s="38"/>
+      <c r="F246" s="46"/>
+      <c r="G246" s="38"/>
+      <c r="H246" s="38"/>
+      <c r="I246" s="38"/>
+      <c r="J246" s="44"/>
+      <c r="K246" s="28"/>
+      <c r="L246" s="28"/>
+      <c r="M246" s="28"/>
+      <c r="N246" s="40"/>
+      <c r="O246" s="3"/>
     </row>
     <row r="247" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B247" s="47" t="s">
@@ -12369,32 +12378,32 @@
         <v>27</v>
       </c>
       <c r="I247" s="38" t="s">
-        <v>443</v>
+        <v>446</v>
       </c>
       <c r="J247" s="44" t="n">
-        <f aca="false">J246+D246</f>
-        <v>136</v>
+        <f aca="false">J245+D245</f>
+        <v>160</v>
       </c>
       <c r="K247" s="28" t="n">
         <f aca="false">J247/8</f>
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="L247" s="28" t="n">
         <f aca="false">J247/16</f>
-        <v>8.5</v>
+        <v>10</v>
       </c>
       <c r="M247" s="28" t="n">
         <f aca="false">J247/32</f>
-        <v>4.25</v>
+        <v>5</v>
       </c>
       <c r="N247" s="1" t="s">
-        <v>478</v>
+        <v>481</v>
       </c>
       <c r="O247" s="3" t="n">
         <v>3</v>
       </c>
       <c r="P247" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q247" s="1" t="n">
         <v>0</v>
@@ -12402,10 +12411,10 @@
     </row>
     <row r="248" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B248" s="47" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="C248" s="3" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="D248" s="1" t="n">
         <v>8</v>
@@ -12421,32 +12430,32 @@
         <v>27</v>
       </c>
       <c r="I248" s="38" t="s">
-        <v>443</v>
+        <v>446</v>
       </c>
       <c r="J248" s="44" t="n">
         <f aca="false">J247+D247</f>
-        <v>144</v>
+        <v>168</v>
       </c>
       <c r="K248" s="28" t="n">
         <f aca="false">J248/8</f>
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="L248" s="28" t="n">
         <f aca="false">J248/16</f>
-        <v>9</v>
+        <v>10.5</v>
       </c>
       <c r="M248" s="28" t="n">
         <f aca="false">J248/32</f>
-        <v>4.5</v>
+        <v>5.25</v>
       </c>
       <c r="N248" s="1" t="s">
-        <v>478</v>
+        <v>481</v>
       </c>
       <c r="O248" s="3" t="n">
         <v>3</v>
       </c>
       <c r="P248" s="1" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Q248" s="1" t="n">
         <v>0</v>
@@ -12454,10 +12463,10 @@
     </row>
     <row r="249" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B249" s="47" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="C249" s="3" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="D249" s="1" t="n">
         <v>8</v>
@@ -12473,32 +12482,32 @@
         <v>27</v>
       </c>
       <c r="I249" s="38" t="s">
-        <v>443</v>
+        <v>446</v>
       </c>
       <c r="J249" s="44" t="n">
         <f aca="false">J248+D248</f>
-        <v>152</v>
+        <v>176</v>
       </c>
       <c r="K249" s="28" t="n">
         <f aca="false">J249/8</f>
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L249" s="28" t="n">
         <f aca="false">J249/16</f>
-        <v>9.5</v>
+        <v>11</v>
       </c>
       <c r="M249" s="28" t="n">
         <f aca="false">J249/32</f>
-        <v>4.75</v>
+        <v>5.5</v>
       </c>
       <c r="N249" s="1" t="s">
-        <v>478</v>
+        <v>481</v>
       </c>
       <c r="O249" s="3" t="n">
         <v>3</v>
       </c>
       <c r="P249" s="1" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Q249" s="1" t="n">
         <v>0</v>
@@ -12506,10 +12515,10 @@
     </row>
     <row r="250" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B250" s="47" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="C250" s="3" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="D250" s="1" t="n">
         <v>8</v>
@@ -12525,32 +12534,32 @@
         <v>27</v>
       </c>
       <c r="I250" s="38" t="s">
-        <v>443</v>
+        <v>446</v>
       </c>
       <c r="J250" s="44" t="n">
         <f aca="false">J249+D249</f>
-        <v>160</v>
+        <v>184</v>
       </c>
       <c r="K250" s="28" t="n">
         <f aca="false">J250/8</f>
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="L250" s="28" t="n">
         <f aca="false">J250/16</f>
-        <v>10</v>
+        <v>11.5</v>
       </c>
       <c r="M250" s="28" t="n">
         <f aca="false">J250/32</f>
-        <v>5</v>
+        <v>5.75</v>
       </c>
       <c r="N250" s="1" t="s">
-        <v>478</v>
+        <v>481</v>
       </c>
       <c r="O250" s="3" t="n">
         <v>3</v>
       </c>
       <c r="P250" s="1" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="Q250" s="1" t="n">
         <v>0</v>
@@ -12558,10 +12567,10 @@
     </row>
     <row r="251" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B251" s="47" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="C251" s="3" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="D251" s="1" t="n">
         <v>8</v>
@@ -12577,32 +12586,32 @@
         <v>27</v>
       </c>
       <c r="I251" s="38" t="s">
-        <v>443</v>
+        <v>446</v>
       </c>
       <c r="J251" s="44" t="n">
         <f aca="false">J250+D250</f>
-        <v>168</v>
+        <v>192</v>
       </c>
       <c r="K251" s="28" t="n">
         <f aca="false">J251/8</f>
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="L251" s="28" t="n">
         <f aca="false">J251/16</f>
-        <v>10.5</v>
+        <v>12</v>
       </c>
       <c r="M251" s="28" t="n">
         <f aca="false">J251/32</f>
-        <v>5.25</v>
+        <v>6</v>
       </c>
       <c r="N251" s="1" t="s">
-        <v>478</v>
+        <v>481</v>
       </c>
       <c r="O251" s="3" t="n">
         <v>3</v>
       </c>
       <c r="P251" s="1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="Q251" s="1" t="n">
         <v>0</v>
@@ -12610,10 +12619,10 @@
     </row>
     <row r="252" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B252" s="47" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="C252" s="3" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="D252" s="1" t="n">
         <v>8</v>
@@ -12629,32 +12638,32 @@
         <v>27</v>
       </c>
       <c r="I252" s="38" t="s">
-        <v>443</v>
+        <v>446</v>
       </c>
       <c r="J252" s="44" t="n">
         <f aca="false">J251+D251</f>
-        <v>176</v>
+        <v>200</v>
       </c>
       <c r="K252" s="28" t="n">
         <f aca="false">J252/8</f>
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="L252" s="28" t="n">
         <f aca="false">J252/16</f>
-        <v>11</v>
+        <v>12.5</v>
       </c>
       <c r="M252" s="28" t="n">
         <f aca="false">J252/32</f>
-        <v>5.5</v>
+        <v>6.25</v>
       </c>
       <c r="N252" s="1" t="s">
-        <v>478</v>
+        <v>481</v>
       </c>
       <c r="O252" s="3" t="n">
         <v>3</v>
       </c>
       <c r="P252" s="1" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="Q252" s="1" t="n">
         <v>0</v>
@@ -12662,10 +12671,10 @@
     </row>
     <row r="253" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B253" s="47" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="C253" s="3" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="D253" s="1" t="n">
         <v>8</v>
@@ -12681,32 +12690,32 @@
         <v>27</v>
       </c>
       <c r="I253" s="38" t="s">
-        <v>443</v>
+        <v>446</v>
       </c>
       <c r="J253" s="44" t="n">
         <f aca="false">J252+D252</f>
-        <v>184</v>
+        <v>208</v>
       </c>
       <c r="K253" s="28" t="n">
         <f aca="false">J253/8</f>
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="L253" s="28" t="n">
         <f aca="false">J253/16</f>
-        <v>11.5</v>
+        <v>13</v>
       </c>
       <c r="M253" s="28" t="n">
         <f aca="false">J253/32</f>
-        <v>5.75</v>
+        <v>6.5</v>
       </c>
       <c r="N253" s="1" t="s">
-        <v>478</v>
+        <v>481</v>
       </c>
       <c r="O253" s="3" t="n">
         <v>3</v>
       </c>
       <c r="P253" s="1" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="Q253" s="1" t="n">
         <v>0</v>
@@ -12714,10 +12723,10 @@
     </row>
     <row r="254" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B254" s="47" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="C254" s="3" t="s">
-        <v>493</v>
+        <v>495</v>
       </c>
       <c r="D254" s="1" t="n">
         <v>8</v>
@@ -12733,32 +12742,32 @@
         <v>27</v>
       </c>
       <c r="I254" s="38" t="s">
-        <v>443</v>
+        <v>446</v>
       </c>
       <c r="J254" s="44" t="n">
         <f aca="false">J253+D253</f>
-        <v>192</v>
+        <v>216</v>
       </c>
       <c r="K254" s="28" t="n">
         <f aca="false">J254/8</f>
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="L254" s="28" t="n">
         <f aca="false">J254/16</f>
-        <v>12</v>
+        <v>13.5</v>
       </c>
       <c r="M254" s="28" t="n">
         <f aca="false">J254/32</f>
-        <v>6</v>
+        <v>6.75</v>
       </c>
       <c r="N254" s="1" t="s">
-        <v>478</v>
+        <v>481</v>
       </c>
       <c r="O254" s="3" t="n">
         <v>3</v>
       </c>
       <c r="P254" s="1" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="Q254" s="1" t="n">
         <v>0</v>
@@ -12766,10 +12775,10 @@
     </row>
     <row r="255" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B255" s="47" t="s">
-        <v>494</v>
+        <v>496</v>
       </c>
       <c r="C255" s="3" t="s">
-        <v>494</v>
+        <v>496</v>
       </c>
       <c r="D255" s="1" t="n">
         <v>8</v>
@@ -12785,32 +12794,32 @@
         <v>27</v>
       </c>
       <c r="I255" s="38" t="s">
-        <v>443</v>
+        <v>446</v>
       </c>
       <c r="J255" s="44" t="n">
         <f aca="false">J254+D254</f>
-        <v>200</v>
+        <v>224</v>
       </c>
       <c r="K255" s="28" t="n">
         <f aca="false">J255/8</f>
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="L255" s="28" t="n">
         <f aca="false">J255/16</f>
-        <v>12.5</v>
+        <v>14</v>
       </c>
       <c r="M255" s="28" t="n">
         <f aca="false">J255/32</f>
-        <v>6.25</v>
+        <v>7</v>
       </c>
       <c r="N255" s="1" t="s">
-        <v>478</v>
+        <v>481</v>
       </c>
       <c r="O255" s="3" t="n">
         <v>3</v>
       </c>
       <c r="P255" s="1" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="Q255" s="1" t="n">
         <v>0</v>
@@ -12818,10 +12827,10 @@
     </row>
     <row r="256" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B256" s="47" t="s">
-        <v>495</v>
+        <v>497</v>
       </c>
       <c r="C256" s="3" t="s">
-        <v>495</v>
+        <v>497</v>
       </c>
       <c r="D256" s="1" t="n">
         <v>8</v>
@@ -12837,32 +12846,32 @@
         <v>27</v>
       </c>
       <c r="I256" s="38" t="s">
-        <v>443</v>
+        <v>446</v>
       </c>
       <c r="J256" s="44" t="n">
         <f aca="false">J255+D255</f>
-        <v>208</v>
+        <v>232</v>
       </c>
       <c r="K256" s="28" t="n">
         <f aca="false">J256/8</f>
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="L256" s="28" t="n">
         <f aca="false">J256/16</f>
-        <v>13</v>
+        <v>14.5</v>
       </c>
       <c r="M256" s="28" t="n">
         <f aca="false">J256/32</f>
-        <v>6.5</v>
+        <v>7.25</v>
       </c>
       <c r="N256" s="1" t="s">
-        <v>478</v>
+        <v>481</v>
       </c>
       <c r="O256" s="3" t="n">
         <v>3</v>
       </c>
       <c r="P256" s="1" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="Q256" s="1" t="n">
         <v>0</v>
@@ -12870,10 +12879,10 @@
     </row>
     <row r="257" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B257" s="47" t="s">
-        <v>496</v>
+        <v>498</v>
       </c>
       <c r="C257" s="3" t="s">
-        <v>496</v>
+        <v>498</v>
       </c>
       <c r="D257" s="1" t="n">
         <v>8</v>
@@ -12889,32 +12898,32 @@
         <v>27</v>
       </c>
       <c r="I257" s="38" t="s">
-        <v>443</v>
+        <v>446</v>
       </c>
       <c r="J257" s="44" t="n">
         <f aca="false">J256+D256</f>
-        <v>216</v>
+        <v>240</v>
       </c>
       <c r="K257" s="28" t="n">
         <f aca="false">J257/8</f>
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="L257" s="28" t="n">
         <f aca="false">J257/16</f>
-        <v>13.5</v>
+        <v>15</v>
       </c>
       <c r="M257" s="28" t="n">
         <f aca="false">J257/32</f>
-        <v>6.75</v>
+        <v>7.5</v>
       </c>
       <c r="N257" s="1" t="s">
-        <v>478</v>
+        <v>481</v>
       </c>
       <c r="O257" s="3" t="n">
         <v>3</v>
       </c>
       <c r="P257" s="1" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="Q257" s="1" t="n">
         <v>0</v>
@@ -12922,10 +12931,10 @@
     </row>
     <row r="258" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B258" s="47" t="s">
-        <v>497</v>
+        <v>499</v>
       </c>
       <c r="C258" s="3" t="s">
-        <v>497</v>
+        <v>499</v>
       </c>
       <c r="D258" s="1" t="n">
         <v>8</v>
@@ -12941,32 +12950,32 @@
         <v>27</v>
       </c>
       <c r="I258" s="38" t="s">
-        <v>443</v>
+        <v>446</v>
       </c>
       <c r="J258" s="44" t="n">
         <f aca="false">J257+D257</f>
-        <v>224</v>
+        <v>248</v>
       </c>
       <c r="K258" s="28" t="n">
         <f aca="false">J258/8</f>
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="L258" s="28" t="n">
         <f aca="false">J258/16</f>
-        <v>14</v>
+        <v>15.5</v>
       </c>
       <c r="M258" s="28" t="n">
         <f aca="false">J258/32</f>
-        <v>7</v>
+        <v>7.75</v>
       </c>
       <c r="N258" s="1" t="s">
-        <v>478</v>
+        <v>481</v>
       </c>
       <c r="O258" s="3" t="n">
         <v>3</v>
       </c>
       <c r="P258" s="1" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="Q258" s="1" t="n">
         <v>0</v>
@@ -12974,20 +12983,18 @@
     </row>
     <row r="259" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B259" s="47" t="s">
-        <v>498</v>
+        <v>500</v>
       </c>
       <c r="C259" s="3" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="D259" s="1" t="n">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E259" s="38" t="s">
         <v>26</v>
       </c>
-      <c r="F259" s="38" t="s">
-        <v>116</v>
-      </c>
+      <c r="F259" s="38"/>
       <c r="G259" s="38" t="s">
         <v>133</v>
       </c>
@@ -12995,32 +13002,32 @@
         <v>27</v>
       </c>
       <c r="I259" s="38" t="s">
-        <v>443</v>
+        <v>446</v>
       </c>
       <c r="J259" s="44" t="n">
         <f aca="false">J258+D258</f>
-        <v>232</v>
+        <v>256</v>
       </c>
       <c r="K259" s="28" t="n">
         <f aca="false">J259/8</f>
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="L259" s="28" t="n">
         <f aca="false">J259/16</f>
-        <v>14.5</v>
+        <v>16</v>
       </c>
       <c r="M259" s="28" t="n">
         <f aca="false">J259/32</f>
-        <v>7.25</v>
+        <v>8</v>
       </c>
       <c r="N259" s="1" t="s">
-        <v>439</v>
+        <v>481</v>
       </c>
       <c r="O259" s="3" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="P259" s="1" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="Q259" s="1" t="n">
         <v>0</v>
@@ -13028,18 +13035,20 @@
     </row>
     <row r="260" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B260" s="47" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="C260" s="3" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="D260" s="1" t="n">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E260" s="38" t="s">
         <v>26</v>
       </c>
-      <c r="F260" s="38"/>
+      <c r="F260" s="38" t="s">
+        <v>116</v>
+      </c>
       <c r="G260" s="38" t="s">
         <v>133</v>
       </c>
@@ -13047,78 +13056,130 @@
         <v>27</v>
       </c>
       <c r="I260" s="38" t="s">
-        <v>443</v>
+        <v>446</v>
       </c>
       <c r="J260" s="44" t="n">
         <f aca="false">J259+D259</f>
-        <v>248</v>
+        <v>264</v>
       </c>
       <c r="K260" s="28" t="n">
         <f aca="false">J260/8</f>
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="L260" s="28" t="n">
         <f aca="false">J260/16</f>
-        <v>15.5</v>
+        <v>16.5</v>
       </c>
       <c r="M260" s="28" t="n">
         <f aca="false">J260/32</f>
-        <v>7.75</v>
+        <v>8.25</v>
       </c>
       <c r="N260" s="1" t="s">
-        <v>463</v>
+        <v>439</v>
       </c>
       <c r="O260" s="3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P260" s="1" t="n">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="Q260" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="261" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A261" s="1" t="s">
-        <v>59</v>
+      <c r="B261" s="47" t="s">
+        <v>503</v>
+      </c>
+      <c r="C261" s="3" t="s">
+        <v>504</v>
+      </c>
+      <c r="D261" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="E261" s="38" t="s">
+        <v>26</v>
       </c>
       <c r="F261" s="38"/>
-      <c r="G261" s="38"/>
-      <c r="H261" s="38"/>
-      <c r="I261" s="38"/>
+      <c r="G261" s="38" t="s">
+        <v>133</v>
+      </c>
+      <c r="H261" s="38" t="s">
+        <v>27</v>
+      </c>
+      <c r="I261" s="38" t="s">
+        <v>446</v>
+      </c>
       <c r="J261" s="44" t="n">
         <f aca="false">J260+D260</f>
-        <v>256</v>
+        <v>280</v>
       </c>
       <c r="K261" s="28" t="n">
         <f aca="false">J261/8</f>
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="L261" s="28" t="n">
         <f aca="false">J261/16</f>
-        <v>16</v>
+        <v>17.5</v>
       </c>
       <c r="M261" s="28" t="n">
         <f aca="false">J261/32</f>
-        <v>8</v>
+        <v>8.75</v>
+      </c>
+      <c r="N261" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="O261" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="P261" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q261" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="262" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A262" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="F262" s="38"/>
       <c r="G262" s="38"/>
       <c r="H262" s="38"/>
       <c r="I262" s="38"/>
-      <c r="J262" s="44"/>
-      <c r="K262" s="28"/>
-      <c r="L262" s="28"/>
-      <c r="M262" s="28"/>
+      <c r="J262" s="44" t="n">
+        <f aca="false">J261+D261</f>
+        <v>288</v>
+      </c>
+      <c r="K262" s="28" t="n">
+        <f aca="false">J262/8</f>
+        <v>36</v>
+      </c>
+      <c r="L262" s="28" t="n">
+        <f aca="false">J262/16</f>
+        <v>18</v>
+      </c>
+      <c r="M262" s="28" t="n">
+        <f aca="false">J262/32</f>
+        <v>9</v>
+      </c>
     </row>
     <row r="263" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B263" s="47"/>
-      <c r="J263" s="48"/>
-      <c r="K263" s="1"/>
-      <c r="L263" s="1"/>
-      <c r="M263" s="1"/>
+      <c r="F263" s="38"/>
+      <c r="G263" s="38"/>
+      <c r="H263" s="38"/>
+      <c r="I263" s="38"/>
+      <c r="J263" s="44"/>
+      <c r="K263" s="28"/>
+      <c r="L263" s="28"/>
+      <c r="M263" s="28"/>
+    </row>
+    <row r="264" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B264" s="47"/>
+      <c r="J264" s="48"/>
+      <c r="K264" s="1"/>
+      <c r="L264" s="1"/>
+      <c r="M264" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -13134,7 +13195,7 @@
     <hyperlink ref="A201" r:id="rId2" display="Structure:science_t, file:sciDownlink.h"/>
     <hyperlink ref="A210" r:id="rId3" display="Structure:sciWodSpecific_t,file:sciWodSpecificDownlink.h"/>
     <hyperlink ref="A218" r:id="rId4" display="Structure:infrequentDownlink_t,file:infrequentDownlink.h"/>
-    <hyperlink ref="A234" r:id="rId5" display="Structure:legacyErrors_t,file:legacyErrorsDownlink.h"/>
+    <hyperlink ref="A235" r:id="rId5" display="Structure:legacyErrors_t,file:legacyErrorsDownlink.h"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -13154,10 +13215,10 @@
   <dimension ref="B6:Q1031"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C33" activeCellId="1" sqref="G97 C33"/>
+      <selection pane="topLeft" activeCell="C33" activeCellId="0" sqref="C33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.0546875" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.06640625" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="40" width="20.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="40" width="16.11"/>
@@ -13168,22 +13229,22 @@
     <row r="6" s="49" customFormat="true" ht="34.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B6" s="50"/>
       <c r="C6" s="50" t="s">
-        <v>502</v>
+        <v>505</v>
       </c>
       <c r="D6" s="50" t="s">
-        <v>503</v>
+        <v>506</v>
       </c>
       <c r="E6" s="50" t="s">
-        <v>504</v>
+        <v>507</v>
       </c>
       <c r="F6" s="50" t="s">
-        <v>505</v>
+        <v>508</v>
       </c>
       <c r="G6" s="50" t="s">
         <v>280</v>
       </c>
       <c r="H6" s="50" t="s">
-        <v>506</v>
+        <v>509</v>
       </c>
       <c r="I6" s="50"/>
     </row>
@@ -13553,10 +13614,10 @@
     </row>
     <row r="26" s="1" customFormat="true" ht="37.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="32" t="s">
-        <v>507</v>
+        <v>510</v>
       </c>
       <c r="C26" s="32" t="s">
-        <v>508</v>
+        <v>511</v>
       </c>
       <c r="D26" s="27" t="n">
         <v>16</v>
@@ -13605,10 +13666,10 @@
     </row>
     <row r="27" s="1" customFormat="true" ht="37.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="32" t="s">
-        <v>509</v>
+        <v>512</v>
       </c>
       <c r="C27" s="32" t="s">
-        <v>510</v>
+        <v>513</v>
       </c>
       <c r="D27" s="27" t="n">
         <v>32</v>
@@ -13655,16 +13716,16 @@
     </row>
     <row r="30" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="52" t="s">
-        <v>511</v>
+        <v>514</v>
       </c>
       <c r="C30" s="52" t="s">
-        <v>512</v>
+        <v>515</v>
       </c>
       <c r="D30" s="52" t="s">
-        <v>513</v>
+        <v>516</v>
       </c>
       <c r="E30" s="52" t="s">
-        <v>514</v>
+        <v>517</v>
       </c>
       <c r="F30" s="52"/>
     </row>

</xml_diff>

<commit_message>
Move some fields around to make more sense
</commit_message>
<xml_diff>
--- a/genSpacecraft/DownlinkSpecLTM.xlsx
+++ b/genSpacecraft/DownlinkSpecLTM.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -443,6 +443,9 @@
     <t xml:space="preserve">Vbatt Bus voltage</t>
   </si>
   <si>
+    <t xml:space="preserve">Spacecraft Status</t>
+  </si>
+  <si>
     <t xml:space="preserve">PA Current</t>
   </si>
   <si>
@@ -578,9 +581,6 @@
     <t xml:space="preserve">Internal Temperature of IHU</t>
   </si>
   <si>
-    <t xml:space="preserve">Spacecraft Status</t>
-  </si>
-  <si>
     <t xml:space="preserve">Modulator Temp</t>
   </si>
   <si>
@@ -809,7 +809,7 @@
     <t xml:space="preserve">Antenna sensor is ok</t>
   </si>
   <si>
-    <t xml:space="preserve">Min/Max Resets</t>
+    <t xml:space="preserve">Min/Max Reset Count</t>
   </si>
   <si>
     <t xml:space="preserve">TLMresets</t>
@@ -1952,8 +1952,8 @@
   </sheetPr>
   <dimension ref="A1:Q264"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A211" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q221" activeCellId="0" sqref="Q221"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A169" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N188" activeCellId="0" sqref="N188"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3842,13 +3842,13 @@
         <v>4.75</v>
       </c>
       <c r="N47" s="1" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="O47" s="3" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="P47" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q47" s="1" t="n">
         <v>3</v>
@@ -3856,10 +3856,10 @@
     </row>
     <row r="48" customFormat="false" ht="56.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B48" s="31" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C48" s="32" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D48" s="32" t="n">
         <v>8</v>
@@ -3869,13 +3869,13 @@
       </c>
       <c r="F48" s="23"/>
       <c r="G48" s="23" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="H48" s="3" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="I48" s="23" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="J48" s="29" t="n">
         <f aca="false">J47+D47</f>
@@ -3908,10 +3908,10 @@
     </row>
     <row r="49" customFormat="false" ht="25.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="31" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C49" s="32" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D49" s="32" t="n">
         <v>8</v>
@@ -3927,7 +3927,7 @@
         <v>77</v>
       </c>
       <c r="I49" s="23" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="J49" s="29" t="n">
         <f aca="false">J48+D48</f>
@@ -3960,10 +3960,10 @@
     </row>
     <row r="50" customFormat="false" ht="37.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="31" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C50" s="32" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D50" s="32" t="n">
         <v>8</v>
@@ -3979,7 +3979,7 @@
         <v>65</v>
       </c>
       <c r="I50" s="23" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="J50" s="29" t="n">
         <f aca="false">J49+D49</f>
@@ -4012,10 +4012,10 @@
     </row>
     <row r="51" customFormat="false" ht="37.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="31" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C51" s="32" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D51" s="32" t="n">
         <v>8</v>
@@ -4025,13 +4025,13 @@
       </c>
       <c r="F51" s="23"/>
       <c r="G51" s="23" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="H51" s="3" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="I51" s="23" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="J51" s="29" t="n">
         <f aca="false">J50+D50</f>
@@ -4064,10 +4064,10 @@
     </row>
     <row r="52" customFormat="false" ht="37.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="31" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C52" s="32" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D52" s="32" t="n">
         <v>8</v>
@@ -4083,7 +4083,7 @@
         <v>71</v>
       </c>
       <c r="I52" s="23" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="J52" s="29" t="n">
         <f aca="false">J51+D51</f>
@@ -4116,10 +4116,10 @@
     </row>
     <row r="53" customFormat="false" ht="25.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="31" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C53" s="32" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D53" s="32" t="n">
         <v>8</v>
@@ -4135,7 +4135,7 @@
         <v>71</v>
       </c>
       <c r="I53" s="32" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="J53" s="29" t="n">
         <f aca="false">J52+D52</f>
@@ -4171,7 +4171,7 @@
         <v>131</v>
       </c>
       <c r="C54" s="32" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D54" s="32" t="n">
         <v>8</v>
@@ -4187,7 +4187,7 @@
         <v>71</v>
       </c>
       <c r="I54" s="32" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="J54" s="29" t="n">
         <f aca="false">J53+D53</f>
@@ -4220,10 +4220,10 @@
     </row>
     <row r="55" customFormat="false" ht="37.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B55" s="31" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C55" s="32" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D55" s="32" t="n">
         <v>8</v>
@@ -4239,7 +4239,7 @@
         <v>71</v>
       </c>
       <c r="I55" s="32" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="J55" s="29" t="n">
         <f aca="false">J54+D54</f>
@@ -4270,12 +4270,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="37.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B56" s="31" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C56" s="32" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D56" s="32" t="n">
         <v>8</v>
@@ -4291,7 +4291,7 @@
         <v>77</v>
       </c>
       <c r="I56" s="23" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="J56" s="29" t="n">
         <f aca="false">J55+D55</f>
@@ -4316,18 +4316,18 @@
         <v>7</v>
       </c>
       <c r="P56" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q56" s="1" t="n">
         <v>3</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="25.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="31" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C57" s="32" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D57" s="32" t="n">
         <v>8</v>
@@ -4343,7 +4343,7 @@
         <v>77</v>
       </c>
       <c r="I57" s="32" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="J57" s="29" t="n">
         <f aca="false">J56+D56</f>
@@ -4368,18 +4368,18 @@
         <v>7</v>
       </c>
       <c r="P57" s="1" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Q57" s="1" t="n">
         <v>3</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="25.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B58" s="31" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C58" s="32" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D58" s="32" t="n">
         <v>8</v>
@@ -4395,7 +4395,7 @@
         <v>77</v>
       </c>
       <c r="I58" s="32" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="J58" s="29" t="n">
         <f aca="false">J57+D57</f>
@@ -4420,18 +4420,18 @@
         <v>7</v>
       </c>
       <c r="P58" s="1" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Q58" s="1" t="n">
         <v>3</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="37.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B59" s="31" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C59" s="32" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="D59" s="32" t="n">
         <v>8</v>
@@ -4447,7 +4447,7 @@
         <v>77</v>
       </c>
       <c r="I59" s="32" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="J59" s="29" t="n">
         <f aca="false">J58+D58</f>
@@ -4472,7 +4472,7 @@
         <v>7</v>
       </c>
       <c r="P59" s="1" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="Q59" s="1" t="n">
         <v>3</v>
@@ -4480,10 +4480,10 @@
     </row>
     <row r="60" customFormat="false" ht="37.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B60" s="31" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C60" s="32" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D60" s="32" t="n">
         <v>8</v>
@@ -4499,7 +4499,7 @@
         <v>71</v>
       </c>
       <c r="I60" s="23" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="J60" s="29" t="n">
         <f aca="false">J59+D59</f>
@@ -4532,10 +4532,10 @@
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B61" s="31" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C61" s="32" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D61" s="32" t="n">
         <v>8</v>
@@ -4549,7 +4549,7 @@
       </c>
       <c r="H61" s="22"/>
       <c r="I61" s="32" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="J61" s="29" t="n">
         <f aca="false">J60+D60</f>
@@ -4574,7 +4574,7 @@
         <v>7</v>
       </c>
       <c r="P61" s="1" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="Q61" s="1" t="n">
         <v>3</v>
@@ -4582,10 +4582,10 @@
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B62" s="31" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C62" s="32" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D62" s="32" t="n">
         <v>8</v>
@@ -4599,7 +4599,7 @@
       </c>
       <c r="H62" s="22"/>
       <c r="I62" s="32" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="J62" s="29" t="n">
         <f aca="false">J61+D61</f>
@@ -4624,7 +4624,7 @@
         <v>7</v>
       </c>
       <c r="P62" s="1" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="Q62" s="1" t="n">
         <v>4</v>
@@ -4632,10 +4632,10 @@
     </row>
     <row r="63" customFormat="false" ht="37.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B63" s="31" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C63" s="32" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="D63" s="32" t="n">
         <v>8</v>
@@ -4651,7 +4651,7 @@
         <v>77</v>
       </c>
       <c r="I63" s="23" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="J63" s="29" t="n">
         <f aca="false">J62+D62</f>
@@ -4670,7 +4670,7 @@
         <v>8.75</v>
       </c>
       <c r="N63" s="1" t="s">
-        <v>185</v>
+        <v>140</v>
       </c>
       <c r="O63" s="3" t="n">
         <v>2</v>
@@ -4736,7 +4736,7 @@
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B65" s="31" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C65" s="32" t="s">
         <v>189</v>
@@ -4778,7 +4778,7 @@
         <v>7</v>
       </c>
       <c r="P65" s="1" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="Q65" s="1" t="n">
         <v>3</v>
@@ -5756,13 +5756,13 @@
         <v>14</v>
       </c>
       <c r="N87" s="5" t="s">
-        <v>185</v>
+        <v>140</v>
       </c>
       <c r="O87" s="24" t="n">
         <v>2</v>
       </c>
       <c r="P87" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Q87" s="1" t="n">
         <v>0</v>
@@ -5927,13 +5927,13 @@
         <v>14.53125</v>
       </c>
       <c r="N91" s="1" t="s">
-        <v>185</v>
+        <v>140</v>
       </c>
       <c r="O91" s="24" t="n">
         <v>2</v>
       </c>
       <c r="P91" s="1" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="Q91" s="1" t="n">
         <v>0</v>
@@ -5979,13 +5979,13 @@
         <v>14.5625</v>
       </c>
       <c r="N92" s="1" t="s">
-        <v>185</v>
+        <v>140</v>
       </c>
       <c r="O92" s="24" t="n">
         <v>2</v>
       </c>
       <c r="P92" s="1" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="Q92" s="1" t="n">
         <v>0</v>
@@ -6237,13 +6237,13 @@
         <v>14.71875</v>
       </c>
       <c r="N97" s="1" t="s">
-        <v>185</v>
+        <v>140</v>
       </c>
       <c r="O97" s="3" t="n">
         <v>2</v>
       </c>
       <c r="P97" s="1" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="Q97" s="1" t="n">
         <v>0</v>
@@ -6309,13 +6309,13 @@
         <v>14.75</v>
       </c>
       <c r="N99" s="1" t="s">
-        <v>185</v>
+        <v>140</v>
       </c>
       <c r="O99" s="3" t="n">
         <v>2</v>
       </c>
       <c r="P99" s="1" t="n">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="Q99" s="1" t="n">
         <v>0</v>
@@ -6361,7 +6361,7 @@
         <v>15</v>
       </c>
       <c r="N100" s="1" t="s">
-        <v>185</v>
+        <v>140</v>
       </c>
       <c r="O100" s="3" t="n">
         <v>2</v>
@@ -7883,7 +7883,7 @@
         <v>7</v>
       </c>
       <c r="P130" s="1" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="Q130" s="1" t="n">
         <v>0</v>
@@ -8077,7 +8077,7 @@
         <v>18</v>
       </c>
       <c r="N134" s="5" t="s">
-        <v>185</v>
+        <v>140</v>
       </c>
       <c r="O134" s="24" t="n">
         <v>2</v>
@@ -8758,7 +8758,7 @@
         <v>20.8125</v>
       </c>
       <c r="N148" s="1" t="s">
-        <v>185</v>
+        <v>140</v>
       </c>
       <c r="O148" s="3" t="n">
         <v>2</v>
@@ -8808,7 +8808,7 @@
         <v>20.90625</v>
       </c>
       <c r="N149" s="1" t="s">
-        <v>185</v>
+        <v>140</v>
       </c>
       <c r="O149" s="3" t="n">
         <v>2</v>
@@ -9315,8 +9315,8 @@
         <v>382</v>
       </c>
       <c r="F165" s="23"/>
-      <c r="G165" s="39" t="n">
-        <v>1</v>
+      <c r="G165" s="23" t="n">
+        <v>36</v>
       </c>
       <c r="H165" s="3" t="s">
         <v>383</v>
@@ -9367,8 +9367,8 @@
         <v>26</v>
       </c>
       <c r="F166" s="23"/>
-      <c r="G166" s="39" t="n">
-        <v>1</v>
+      <c r="G166" s="23" t="n">
+        <v>36</v>
       </c>
       <c r="H166" s="3" t="s">
         <v>383</v>
@@ -9419,8 +9419,8 @@
         <v>382</v>
       </c>
       <c r="F167" s="23"/>
-      <c r="G167" s="22" t="n">
-        <v>1</v>
+      <c r="G167" s="23" t="n">
+        <v>36</v>
       </c>
       <c r="H167" s="22" t="s">
         <v>27</v>
@@ -9554,8 +9554,8 @@
       </c>
       <c r="E173" s="38"/>
       <c r="F173" s="23"/>
-      <c r="G173" s="39" t="n">
-        <v>1</v>
+      <c r="G173" s="23" t="n">
+        <v>36</v>
       </c>
       <c r="H173" s="3" t="s">
         <v>383</v>
@@ -9606,8 +9606,8 @@
         <v>26</v>
       </c>
       <c r="F174" s="23"/>
-      <c r="G174" s="39" t="n">
-        <v>1</v>
+      <c r="G174" s="23" t="n">
+        <v>36</v>
       </c>
       <c r="H174" s="3" t="s">
         <v>383</v>
@@ -9656,8 +9656,8 @@
       </c>
       <c r="E175" s="38"/>
       <c r="F175" s="23"/>
-      <c r="G175" s="39" t="n">
-        <v>1</v>
+      <c r="G175" s="23" t="n">
+        <v>36</v>
       </c>
       <c r="I175" s="28" t="s">
         <v>403</v>
@@ -9703,8 +9703,8 @@
       </c>
       <c r="E176" s="38"/>
       <c r="F176" s="23"/>
-      <c r="G176" s="39" t="n">
-        <v>1</v>
+      <c r="G176" s="23" t="n">
+        <v>36</v>
       </c>
       <c r="I176" s="28" t="s">
         <v>406</v>
@@ -9752,8 +9752,8 @@
         <v>382</v>
       </c>
       <c r="F177" s="23"/>
-      <c r="G177" s="22" t="n">
-        <v>1</v>
+      <c r="G177" s="23" t="n">
+        <v>36</v>
       </c>
       <c r="H177" s="22" t="s">
         <v>27</v>
@@ -10094,13 +10094,13 @@
         <v>23.75</v>
       </c>
       <c r="N188" s="1" t="s">
-        <v>185</v>
+        <v>140</v>
       </c>
       <c r="O188" s="24" t="n">
         <v>2</v>
       </c>
       <c r="P188" s="1" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="Q188" s="1" t="n">
         <v>0</v>
@@ -10146,13 +10146,13 @@
         <v>23.78125</v>
       </c>
       <c r="N189" s="1" t="s">
-        <v>185</v>
+        <v>140</v>
       </c>
       <c r="O189" s="24" t="n">
         <v>2</v>
       </c>
       <c r="P189" s="1" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="Q189" s="1" t="n">
         <v>0</v>
@@ -10198,13 +10198,13 @@
         <v>23.8125</v>
       </c>
       <c r="N190" s="1" t="s">
-        <v>185</v>
+        <v>140</v>
       </c>
       <c r="O190" s="24" t="n">
         <v>2</v>
       </c>
       <c r="P190" s="1" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="Q190" s="1" t="n">
         <v>0</v>
@@ -13218,7 +13218,7 @@
       <selection pane="topLeft" activeCell="C33" activeCellId="0" sqref="C33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.06640625" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.07421875" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="40" width="20.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="40" width="16.11"/>

</xml_diff>

<commit_message>
Re-arrange FoxTelem panels and fix duplicate pad names
</commit_message>
<xml_diff>
--- a/genSpacecraft/DownlinkSpecLTM.xlsx
+++ b/genSpacecraft/DownlinkSpecLTM.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1401" uniqueCount="518">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1401" uniqueCount="520">
   <si>
     <t xml:space="preserve">//</t>
   </si>
@@ -710,16 +710,16 @@
     <t xml:space="preserve">Host OBC Temp</t>
   </si>
   <si>
-    <t xml:space="preserve">spare19</t>
+    <t xml:space="preserve">commonSpare1</t>
   </si>
   <si>
     <t xml:space="preserve">spare</t>
   </si>
   <si>
-    <t xml:space="preserve">spare20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">spare21</t>
+    <t xml:space="preserve">commonSpare2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">commonSpare3</t>
   </si>
   <si>
     <t xml:space="preserve">Totals:</t>
@@ -746,13 +746,13 @@
     <t xml:space="preserve">TBD</t>
   </si>
   <si>
-    <t xml:space="preserve">spare28</t>
+    <t xml:space="preserve">wodSpare1</t>
   </si>
   <si>
     <t xml:space="preserve">de</t>
   </si>
   <si>
-    <t xml:space="preserve">SpareBit1</t>
+    <t xml:space="preserve">wodSpare2</t>
   </si>
   <si>
     <t xml:space="preserve">Auto Safe Allowed</t>
@@ -773,13 +773,16 @@
     <t xml:space="preserve">Autosafe Mode Active</t>
   </si>
   <si>
-    <t xml:space="preserve">Spare Bit 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">spareBit1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SpareBit3</t>
+    <t xml:space="preserve">com2 Spare Bit 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com2spareBit2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com2 Spare Bit 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com2spareBit3</t>
   </si>
   <si>
     <t xml:space="preserve">Transponder Enabled</t>
@@ -1073,28 +1076,25 @@
     <t xml:space="preserve">Modulator Register 8 - Mode</t>
   </si>
   <si>
-    <t xml:space="preserve">spare29</t>
-  </si>
-  <si>
-    <t xml:space="preserve">spare30</t>
-  </si>
-  <si>
-    <t xml:space="preserve">spare31</t>
-  </si>
-  <si>
-    <t xml:space="preserve">spare32</t>
-  </si>
-  <si>
-    <t xml:space="preserve">spare33</t>
-  </si>
-  <si>
-    <t xml:space="preserve">spare34</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SpareBit4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SpareBit1a</t>
+    <t xml:space="preserve">com2spare4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com2spare5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com2spare6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com2spare7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com2spare8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com2spare9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com2Spare10</t>
   </si>
   <si>
     <t xml:space="preserve">Modulator Valid</t>
@@ -1139,16 +1139,16 @@
     <t xml:space="preserve">ICR Receiving Carrier</t>
   </si>
   <si>
-    <t xml:space="preserve">spare341</t>
-  </si>
-  <si>
-    <t xml:space="preserve">spare35</t>
-  </si>
-  <si>
-    <t xml:space="preserve">spare36</t>
-  </si>
-  <si>
-    <t xml:space="preserve">spare37</t>
+    <t xml:space="preserve">com2spare11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com2spare12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com2spare13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com2spare14</t>
   </si>
   <si>
     <t xml:space="preserve">Total Length</t>
@@ -1298,24 +1298,30 @@
     <t xml:space="preserve">Opaque CAN data from host experiment</t>
   </si>
   <si>
+    <t xml:space="preserve">LongSciSparebits</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Longscisparebits</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Overflow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">overflow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">One or more CAN messages lost</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Structure:science_t, file:sciDownlink.h</t>
+  </si>
+  <si>
     <t xml:space="preserve">Sparebits</t>
   </si>
   <si>
     <t xml:space="preserve">sparebits</t>
   </si>
   <si>
-    <t xml:space="preserve">Overflow</t>
-  </si>
-  <si>
-    <t xml:space="preserve">overflow</t>
-  </si>
-  <si>
-    <t xml:space="preserve">One or more CAN messages lost</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Structure:science_t, file:sciDownlink.h</t>
-  </si>
-  <si>
     <t xml:space="preserve">Structure:sciWodSpecific_t,file:sciWodSpecificDownlink.h</t>
   </si>
   <si>
@@ -1397,7 +1403,7 @@
     <t xml:space="preserve">Fill to 32-bits</t>
   </si>
   <si>
-    <t xml:space="preserve">pad1</t>
+    <t xml:space="preserve">infreqSpare1</t>
   </si>
   <si>
     <t xml:space="preserve">Structure:legacyErrors_t,file:legacyErrorsDownlink.h</t>
@@ -1952,8 +1958,8 @@
   </sheetPr>
   <dimension ref="A1:Q264"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A169" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N188" activeCellId="0" sqref="N188"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B229" activeCellId="0" sqref="B229"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5491,7 +5497,7 @@
       <c r="B80" s="31" t="s">
         <v>229</v>
       </c>
-      <c r="C80" s="32" t="s">
+      <c r="C80" s="31" t="s">
         <v>229</v>
       </c>
       <c r="D80" s="32" t="n">
@@ -5541,7 +5547,7 @@
       <c r="B81" s="31" t="s">
         <v>231</v>
       </c>
-      <c r="C81" s="32" t="s">
+      <c r="C81" s="31" t="s">
         <v>231</v>
       </c>
       <c r="D81" s="32" t="n">
@@ -5591,7 +5597,7 @@
       <c r="B82" s="31" t="s">
         <v>232</v>
       </c>
-      <c r="C82" s="32" t="s">
+      <c r="C82" s="31" t="s">
         <v>232</v>
       </c>
       <c r="D82" s="32" t="n">
@@ -5772,7 +5778,7 @@
       <c r="B88" s="31" t="s">
         <v>241</v>
       </c>
-      <c r="C88" s="32" t="s">
+      <c r="C88" s="31" t="s">
         <v>241</v>
       </c>
       <c r="D88" s="32" t="n">
@@ -5841,7 +5847,7 @@
       <c r="B90" s="31" t="s">
         <v>243</v>
       </c>
-      <c r="C90" s="32" t="s">
+      <c r="C90" s="31" t="s">
         <v>243</v>
       </c>
       <c r="D90" s="32" t="n">
@@ -6048,7 +6054,7 @@
         <v>252</v>
       </c>
       <c r="C94" s="32" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="D94" s="32" t="n">
         <v>1</v>
@@ -6097,10 +6103,10 @@
     </row>
     <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B95" s="31" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="C95" s="32" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="D95" s="32" t="n">
         <v>1</v>
@@ -6147,10 +6153,10 @@
     </row>
     <row r="96" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B96" s="33" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="C96" s="32" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="D96" s="32" t="n">
         <v>1</v>
@@ -6166,7 +6172,7 @@
         <v>27</v>
       </c>
       <c r="I96" s="23" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="J96" s="29" t="n">
         <f aca="false">J95+D95</f>
@@ -6199,10 +6205,10 @@
     </row>
     <row r="97" customFormat="false" ht="25.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B97" s="33" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="C97" s="32" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="D97" s="32" t="n">
         <v>1</v>
@@ -6212,13 +6218,13 @@
       </c>
       <c r="F97" s="23"/>
       <c r="G97" s="22" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="H97" s="22" t="s">
         <v>27</v>
       </c>
       <c r="I97" s="23" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="J97" s="29" t="n">
         <f aca="false">J96+D96</f>
@@ -6271,10 +6277,10 @@
     </row>
     <row r="99" customFormat="false" ht="50.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B99" s="31" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="C99" s="32" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="D99" s="32" t="n">
         <v>8</v>
@@ -6290,7 +6296,7 @@
         <v>27</v>
       </c>
       <c r="I99" s="23" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="J99" s="29" t="n">
         <f aca="false">J97+D97</f>
@@ -6323,10 +6329,10 @@
     </row>
     <row r="100" customFormat="false" ht="75.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B100" s="31" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="C100" s="32" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="D100" s="32" t="n">
         <v>8</v>
@@ -6342,7 +6348,7 @@
         <v>27</v>
       </c>
       <c r="I100" s="23" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="J100" s="29" t="n">
         <f aca="false">J99+D99</f>
@@ -6375,10 +6381,10 @@
     </row>
     <row r="101" customFormat="false" ht="25.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B101" s="31" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="C101" s="32" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="D101" s="32" t="n">
         <v>32</v>
@@ -6396,7 +6402,7 @@
         <v>27</v>
       </c>
       <c r="I101" s="23" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="J101" s="29" t="n">
         <f aca="false">J100+D100</f>
@@ -6429,10 +6435,10 @@
     </row>
     <row r="102" customFormat="false" ht="50.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B102" s="31" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="C102" s="32" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="D102" s="32" t="n">
         <v>8</v>
@@ -6448,7 +6454,7 @@
         <v>27</v>
       </c>
       <c r="I102" s="23" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="J102" s="29" t="n">
         <f aca="false">J101+D101</f>
@@ -6481,10 +6487,10 @@
     </row>
     <row r="103" customFormat="false" ht="50.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B103" s="31" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C103" s="32" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="D103" s="32" t="n">
         <v>8</v>
@@ -6500,7 +6506,7 @@
         <v>27</v>
       </c>
       <c r="I103" s="23" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="J103" s="29" t="n">
         <f aca="false">J102+D102</f>
@@ -6533,10 +6539,10 @@
     </row>
     <row r="104" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B104" s="31" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="C104" s="32" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="D104" s="32" t="n">
         <v>8</v>
@@ -6546,13 +6552,13 @@
       </c>
       <c r="F104" s="23"/>
       <c r="G104" s="23" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="H104" s="22" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="I104" s="23" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="J104" s="29" t="n">
         <f aca="false">J103+D103</f>
@@ -6585,10 +6591,10 @@
     </row>
     <row r="105" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B105" s="31" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="C105" s="32" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="D105" s="32" t="n">
         <v>1</v>
@@ -6598,13 +6604,13 @@
       </c>
       <c r="F105" s="23"/>
       <c r="G105" s="22" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="H105" s="22" t="s">
         <v>27</v>
       </c>
       <c r="I105" s="32" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="J105" s="29" t="n">
         <f aca="false">J104+D104</f>
@@ -6637,10 +6643,10 @@
     </row>
     <row r="106" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B106" s="31" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="C106" s="32" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D106" s="32" t="n">
         <v>1</v>
@@ -6650,7 +6656,7 @@
       </c>
       <c r="F106" s="23"/>
       <c r="G106" s="22" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="H106" s="22" t="s">
         <v>27</v>
@@ -6687,10 +6693,10 @@
     </row>
     <row r="107" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B107" s="31" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C107" s="32" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="D107" s="32" t="n">
         <v>1</v>
@@ -6700,7 +6706,7 @@
       </c>
       <c r="F107" s="23"/>
       <c r="G107" s="22" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="H107" s="22" t="s">
         <v>27</v>
@@ -6737,10 +6743,10 @@
     </row>
     <row r="108" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B108" s="31" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="C108" s="32" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="D108" s="32" t="n">
         <v>1</v>
@@ -6750,7 +6756,7 @@
       </c>
       <c r="F108" s="23"/>
       <c r="G108" s="22" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="H108" s="22" t="s">
         <v>27</v>
@@ -6787,10 +6793,10 @@
     </row>
     <row r="109" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B109" s="31" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="C109" s="32" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="D109" s="32" t="n">
         <v>1</v>
@@ -6800,7 +6806,7 @@
       </c>
       <c r="F109" s="23"/>
       <c r="G109" s="22" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="H109" s="22" t="s">
         <v>27</v>
@@ -6823,7 +6829,7 @@
         <v>17.125</v>
       </c>
       <c r="N109" s="1" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="O109" s="24" t="n">
         <v>9</v>
@@ -6837,10 +6843,10 @@
     </row>
     <row r="110" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B110" s="31" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C110" s="32" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="D110" s="32" t="n">
         <v>1</v>
@@ -6850,7 +6856,7 @@
       </c>
       <c r="F110" s="23"/>
       <c r="G110" s="22" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="H110" s="22" t="s">
         <v>27</v>
@@ -6873,7 +6879,7 @@
         <v>17.15625</v>
       </c>
       <c r="N110" s="1" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="O110" s="24" t="n">
         <v>9</v>
@@ -6887,10 +6893,10 @@
     </row>
     <row r="111" customFormat="false" ht="25.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B111" s="31" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="C111" s="32" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="D111" s="32" t="n">
         <v>1</v>
@@ -6900,7 +6906,7 @@
       </c>
       <c r="F111" s="23"/>
       <c r="G111" s="22" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="H111" s="22" t="s">
         <v>27</v>
@@ -6923,7 +6929,7 @@
         <v>17.1875</v>
       </c>
       <c r="N111" s="1" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="O111" s="24" t="n">
         <v>9</v>
@@ -6937,10 +6943,10 @@
     </row>
     <row r="112" customFormat="false" ht="25.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B112" s="31" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C112" s="32" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="D112" s="32" t="n">
         <v>1</v>
@@ -6950,7 +6956,7 @@
       </c>
       <c r="F112" s="23"/>
       <c r="G112" s="22" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="H112" s="22" t="s">
         <v>27</v>
@@ -6973,7 +6979,7 @@
         <v>17.21875</v>
       </c>
       <c r="N112" s="1" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="O112" s="24" t="n">
         <v>9</v>
@@ -6987,10 +6993,10 @@
     </row>
     <row r="113" customFormat="false" ht="25.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B113" s="31" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="C113" s="32" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="D113" s="32" t="n">
         <v>1</v>
@@ -7000,13 +7006,13 @@
       </c>
       <c r="F113" s="23"/>
       <c r="G113" s="22" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="H113" s="22" t="s">
         <v>27</v>
       </c>
       <c r="I113" s="32" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="J113" s="29" t="n">
         <f aca="false">J112+D112</f>
@@ -7025,7 +7031,7 @@
         <v>17.25</v>
       </c>
       <c r="N113" s="1" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="O113" s="24" t="n">
         <v>9</v>
@@ -7039,10 +7045,10 @@
     </row>
     <row r="114" customFormat="false" ht="25.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B114" s="31" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C114" s="32" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="D114" s="32" t="n">
         <v>1</v>
@@ -7052,7 +7058,7 @@
       </c>
       <c r="F114" s="23"/>
       <c r="G114" s="22" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="H114" s="22" t="s">
         <v>27</v>
@@ -7075,7 +7081,7 @@
         <v>17.28125</v>
       </c>
       <c r="N114" s="1" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="O114" s="24" t="n">
         <v>9</v>
@@ -7089,10 +7095,10 @@
     </row>
     <row r="115" customFormat="false" ht="25.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B115" s="31" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="C115" s="32" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="D115" s="32" t="n">
         <v>1</v>
@@ -7102,7 +7108,7 @@
       </c>
       <c r="F115" s="23"/>
       <c r="G115" s="22" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="H115" s="22" t="s">
         <v>27</v>
@@ -7125,7 +7131,7 @@
         <v>17.3125</v>
       </c>
       <c r="N115" s="1" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="O115" s="24" t="n">
         <v>9</v>
@@ -7139,10 +7145,10 @@
     </row>
     <row r="116" customFormat="false" ht="25.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B116" s="31" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C116" s="32" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="D116" s="32" t="n">
         <v>1</v>
@@ -7152,7 +7158,7 @@
       </c>
       <c r="F116" s="23"/>
       <c r="G116" s="22" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="H116" s="22" t="s">
         <v>27</v>
@@ -7175,7 +7181,7 @@
         <v>17.34375</v>
       </c>
       <c r="N116" s="1" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="O116" s="24" t="n">
         <v>9</v>
@@ -7189,10 +7195,10 @@
     </row>
     <row r="117" customFormat="false" ht="25.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B117" s="31" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="C117" s="32" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="D117" s="32" t="n">
         <v>1</v>
@@ -7202,7 +7208,7 @@
       </c>
       <c r="F117" s="23"/>
       <c r="G117" s="22" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="H117" s="22" t="s">
         <v>27</v>
@@ -7225,7 +7231,7 @@
         <v>17.375</v>
       </c>
       <c r="N117" s="1" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="O117" s="24" t="n">
         <v>9</v>
@@ -7239,10 +7245,10 @@
     </row>
     <row r="118" customFormat="false" ht="25.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B118" s="31" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C118" s="32" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="D118" s="32" t="n">
         <v>1</v>
@@ -7252,7 +7258,7 @@
       </c>
       <c r="F118" s="23"/>
       <c r="G118" s="22" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="H118" s="22" t="s">
         <v>27</v>
@@ -7275,7 +7281,7 @@
         <v>17.40625</v>
       </c>
       <c r="N118" s="1" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="O118" s="24" t="n">
         <v>9</v>
@@ -7289,10 +7295,10 @@
     </row>
     <row r="119" customFormat="false" ht="25.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B119" s="31" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="C119" s="32" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="D119" s="32" t="n">
         <v>1</v>
@@ -7302,7 +7308,7 @@
       </c>
       <c r="F119" s="23"/>
       <c r="G119" s="22" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="H119" s="22" t="s">
         <v>27</v>
@@ -7325,7 +7331,7 @@
         <v>17.4375</v>
       </c>
       <c r="N119" s="1" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="O119" s="24" t="n">
         <v>9</v>
@@ -7339,10 +7345,10 @@
     </row>
     <row r="120" customFormat="false" ht="25.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B120" s="31" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C120" s="32" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="D120" s="32" t="n">
         <v>1</v>
@@ -7352,7 +7358,7 @@
       </c>
       <c r="F120" s="23"/>
       <c r="G120" s="22" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="H120" s="22" t="s">
         <v>27</v>
@@ -7375,7 +7381,7 @@
         <v>17.46875</v>
       </c>
       <c r="N120" s="1" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="O120" s="24" t="n">
         <v>9</v>
@@ -7389,10 +7395,10 @@
     </row>
     <row r="121" customFormat="false" ht="25.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B121" s="31" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="C121" s="32" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="D121" s="32" t="n">
         <v>1</v>
@@ -7402,13 +7408,13 @@
       </c>
       <c r="F121" s="23"/>
       <c r="G121" s="22" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="H121" s="22" t="s">
         <v>27</v>
       </c>
       <c r="I121" s="32" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="J121" s="29" t="n">
         <f aca="false">J120+D120</f>
@@ -7427,7 +7433,7 @@
         <v>17.5</v>
       </c>
       <c r="N121" s="1" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="O121" s="24" t="n">
         <v>9</v>
@@ -7441,10 +7447,10 @@
     </row>
     <row r="122" customFormat="false" ht="25.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B122" s="31" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="C122" s="32" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="D122" s="32" t="n">
         <v>1</v>
@@ -7454,7 +7460,7 @@
       </c>
       <c r="F122" s="23"/>
       <c r="G122" s="22" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="H122" s="22" t="s">
         <v>27</v>
@@ -7477,7 +7483,7 @@
         <v>17.53125</v>
       </c>
       <c r="N122" s="1" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="O122" s="24" t="n">
         <v>9</v>
@@ -7491,10 +7497,10 @@
     </row>
     <row r="123" customFormat="false" ht="25.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B123" s="31" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="C123" s="32" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="D123" s="32" t="n">
         <v>1</v>
@@ -7504,7 +7510,7 @@
       </c>
       <c r="F123" s="23"/>
       <c r="G123" s="22" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="H123" s="22" t="s">
         <v>27</v>
@@ -7527,7 +7533,7 @@
         <v>17.5625</v>
       </c>
       <c r="N123" s="1" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="O123" s="24" t="n">
         <v>9</v>
@@ -7541,10 +7547,10 @@
     </row>
     <row r="124" customFormat="false" ht="25.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B124" s="31" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="C124" s="32" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="D124" s="32" t="n">
         <v>1</v>
@@ -7554,7 +7560,7 @@
       </c>
       <c r="F124" s="23"/>
       <c r="G124" s="22" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="H124" s="22" t="s">
         <v>27</v>
@@ -7577,7 +7583,7 @@
         <v>17.59375</v>
       </c>
       <c r="N124" s="1" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="O124" s="24" t="n">
         <v>9</v>
@@ -7591,10 +7597,10 @@
     </row>
     <row r="125" customFormat="false" ht="25.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B125" s="31" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="C125" s="32" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="D125" s="32" t="n">
         <v>1</v>
@@ -7604,7 +7610,7 @@
       </c>
       <c r="F125" s="23"/>
       <c r="G125" s="22" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="H125" s="22" t="s">
         <v>27</v>
@@ -7627,7 +7633,7 @@
         <v>17.625</v>
       </c>
       <c r="N125" s="1" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="O125" s="24" t="n">
         <v>9</v>
@@ -7641,10 +7647,10 @@
     </row>
     <row r="126" customFormat="false" ht="25.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B126" s="31" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="C126" s="32" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="D126" s="32" t="n">
         <v>1</v>
@@ -7654,7 +7660,7 @@
       </c>
       <c r="F126" s="23"/>
       <c r="G126" s="22" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="H126" s="22" t="s">
         <v>27</v>
@@ -7677,7 +7683,7 @@
         <v>17.65625</v>
       </c>
       <c r="N126" s="1" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="O126" s="24" t="n">
         <v>9</v>
@@ -7691,10 +7697,10 @@
     </row>
     <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B127" s="31" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="C127" s="32" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="D127" s="32" t="n">
         <v>2</v>
@@ -7741,10 +7747,10 @@
     </row>
     <row r="128" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B128" s="31" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C128" s="32" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="D128" s="32" t="n">
         <v>1</v>
@@ -7754,7 +7760,7 @@
       </c>
       <c r="F128" s="23"/>
       <c r="G128" s="22" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="H128" s="22" t="s">
         <v>27</v>
@@ -7791,10 +7797,10 @@
     </row>
     <row r="129" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B129" s="31" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="C129" s="32" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="D129" s="32" t="n">
         <v>1</v>
@@ -7804,7 +7810,7 @@
       </c>
       <c r="F129" s="23"/>
       <c r="G129" s="22" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="H129" s="22" t="s">
         <v>27</v>
@@ -7841,10 +7847,10 @@
     </row>
     <row r="130" customFormat="false" ht="25.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B130" s="31" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="C130" s="32" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="D130" s="32" t="n">
         <v>1</v>
@@ -7854,7 +7860,7 @@
       </c>
       <c r="F130" s="23"/>
       <c r="G130" s="22" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="H130" s="22" t="s">
         <v>27</v>
@@ -7891,10 +7897,10 @@
     </row>
     <row r="131" customFormat="false" ht="25.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B131" s="31" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="C131" s="32" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="D131" s="32" t="n">
         <v>1</v>
@@ -7904,7 +7910,7 @@
       </c>
       <c r="F131" s="23"/>
       <c r="G131" s="22" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="H131" s="22" t="s">
         <v>27</v>
@@ -7941,10 +7947,10 @@
     </row>
     <row r="132" customFormat="false" ht="25.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B132" s="31" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="C132" s="32" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="D132" s="32" t="n">
         <v>1</v>
@@ -7954,7 +7960,7 @@
       </c>
       <c r="F132" s="23"/>
       <c r="G132" s="22" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="H132" s="22"/>
       <c r="I132" s="32"/>
@@ -7975,7 +7981,7 @@
         <v>17.875</v>
       </c>
       <c r="N132" s="1" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="O132" s="24" t="n">
         <v>9</v>
@@ -7989,10 +7995,10 @@
     </row>
     <row r="133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B133" s="31" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="C133" s="32" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="D133" s="32" t="n">
         <v>3</v>
@@ -8039,10 +8045,10 @@
     </row>
     <row r="134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B134" s="31" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="C134" s="32" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="D134" s="32" t="n">
         <v>8</v>
@@ -8091,10 +8097,10 @@
     </row>
     <row r="135" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B135" s="31" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="C135" s="32" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="D135" s="32" t="n">
         <v>8</v>
@@ -8110,7 +8116,7 @@
         <v>27</v>
       </c>
       <c r="I135" s="23" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="J135" s="29" t="n">
         <f aca="false">J134+D134</f>
@@ -8143,10 +8149,10 @@
     </row>
     <row r="136" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B136" s="31" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="C136" s="32" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="D136" s="32" t="n">
         <v>8</v>
@@ -8162,7 +8168,7 @@
         <v>27</v>
       </c>
       <c r="I136" s="23" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="J136" s="29" t="n">
         <f aca="false">J135+D135</f>
@@ -8195,10 +8201,10 @@
     </row>
     <row r="137" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B137" s="31" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="C137" s="32" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="D137" s="32" t="n">
         <v>8</v>
@@ -8214,7 +8220,7 @@
         <v>27</v>
       </c>
       <c r="I137" s="23" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="J137" s="29" t="n">
         <f aca="false">J136+D136</f>
@@ -8247,10 +8253,10 @@
     </row>
     <row r="138" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B138" s="31" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="C138" s="32" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="D138" s="32" t="n">
         <v>8</v>
@@ -8266,7 +8272,7 @@
         <v>27</v>
       </c>
       <c r="I138" s="23" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="J138" s="29" t="n">
         <f aca="false">J137+D137</f>
@@ -8299,10 +8305,10 @@
     </row>
     <row r="139" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B139" s="31" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="C139" s="32" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="D139" s="32" t="n">
         <v>8</v>
@@ -8349,10 +8355,10 @@
     </row>
     <row r="140" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B140" s="31" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="C140" s="32" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="D140" s="32" t="n">
         <v>8</v>
@@ -8399,10 +8405,10 @@
     </row>
     <row r="141" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B141" s="31" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="C141" s="32" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="D141" s="32" t="n">
         <v>8</v>
@@ -8449,10 +8455,10 @@
     </row>
     <row r="142" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B142" s="31" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="C142" s="32" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="D142" s="32" t="n">
         <v>8</v>
@@ -8499,10 +8505,10 @@
     </row>
     <row r="143" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B143" s="31" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="C143" s="32" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="D143" s="32" t="n">
         <v>8</v>
@@ -8549,10 +8555,10 @@
     </row>
     <row r="144" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B144" s="31" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="C144" s="32" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="D144" s="32" t="n">
         <v>8</v>
@@ -8621,9 +8627,9 @@
     </row>
     <row r="146" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B146" s="31" t="s">
-        <v>356</v>
-      </c>
-      <c r="C146" s="32" t="s">
+        <v>357</v>
+      </c>
+      <c r="C146" s="31" t="s">
         <v>357</v>
       </c>
       <c r="D146" s="32" t="n">
@@ -8948,7 +8954,7 @@
       <c r="B153" s="31" t="s">
         <v>372</v>
       </c>
-      <c r="C153" s="32" t="s">
+      <c r="C153" s="31" t="s">
         <v>372</v>
       </c>
       <c r="D153" s="32" t="n">
@@ -8998,7 +9004,7 @@
       <c r="B154" s="31" t="s">
         <v>373</v>
       </c>
-      <c r="C154" s="32" t="s">
+      <c r="C154" s="31" t="s">
         <v>373</v>
       </c>
       <c r="D154" s="32" t="n">
@@ -9048,7 +9054,7 @@
       <c r="B155" s="31" t="s">
         <v>374</v>
       </c>
-      <c r="C155" s="32" t="s">
+      <c r="C155" s="31" t="s">
         <v>374</v>
       </c>
       <c r="D155" s="32" t="n">
@@ -9098,7 +9104,7 @@
       <c r="B156" s="31" t="s">
         <v>375</v>
       </c>
-      <c r="C156" s="32" t="s">
+      <c r="C156" s="31" t="s">
         <v>375</v>
       </c>
       <c r="D156" s="32" t="n">
@@ -10663,10 +10669,10 @@
     </row>
     <row r="204" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B204" s="31" t="s">
-        <v>425</v>
+        <v>431</v>
       </c>
       <c r="C204" s="22" t="s">
-        <v>426</v>
+        <v>432</v>
       </c>
       <c r="D204" s="22" t="n">
         <v>7</v>
@@ -10789,7 +10795,7 @@
     </row>
     <row r="210" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A210" s="42" t="s">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c r="B210" s="11"/>
       <c r="C210" s="41"/>
@@ -10871,7 +10877,7 @@
         <v>1</v>
       </c>
       <c r="H212" s="39" t="s">
-        <v>432</v>
+        <v>434</v>
       </c>
       <c r="I212" s="28" t="s">
         <v>414</v>
@@ -10907,7 +10913,7 @@
     </row>
     <row r="213" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B213" s="31" t="s">
-        <v>433</v>
+        <v>435</v>
       </c>
       <c r="C213" s="32" t="s">
         <v>417</v>
@@ -10919,7 +10925,7 @@
         <v>26</v>
       </c>
       <c r="F213" s="23" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="G213" s="39" t="n">
         <v>1</v>
@@ -10978,7 +10984,7 @@
         <v>27</v>
       </c>
       <c r="I214" s="28" t="s">
-        <v>435</v>
+        <v>437</v>
       </c>
       <c r="J214" s="4" t="n">
         <f aca="false">J213+D213</f>
@@ -11097,7 +11103,7 @@
     </row>
     <row r="218" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A218" s="42" t="s">
-        <v>436</v>
+        <v>438</v>
       </c>
     </row>
     <row r="219" s="14" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11171,10 +11177,10 @@
         <v>133</v>
       </c>
       <c r="H220" s="38" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="I220" s="38" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="J220" s="44" t="n">
         <v>0</v>
@@ -11192,7 +11198,7 @@
         <v>0</v>
       </c>
       <c r="N220" s="1" t="s">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="O220" s="3" t="n">
         <v>1</v>
@@ -11206,10 +11212,10 @@
     </row>
     <row r="221" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B221" s="43" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
       <c r="C221" s="38" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="D221" s="38" t="n">
         <v>32</v>
@@ -11222,10 +11228,10 @@
         <v>133</v>
       </c>
       <c r="H221" s="38" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="I221" s="38" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="J221" s="44" t="n">
         <f aca="false">J220+D220</f>
@@ -11244,7 +11250,7 @@
         <v>1</v>
       </c>
       <c r="N221" s="1" t="s">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="O221" s="3" t="n">
         <v>1</v>
@@ -11258,7 +11264,7 @@
     </row>
     <row r="222" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A222" s="1" t="s">
-        <v>443</v>
+        <v>445</v>
       </c>
       <c r="B222" s="43"/>
       <c r="C222" s="38"/>
@@ -11275,10 +11281,10 @@
     </row>
     <row r="223" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B223" s="43" t="s">
-        <v>444</v>
+        <v>446</v>
       </c>
       <c r="C223" s="38" t="s">
-        <v>444</v>
+        <v>446</v>
       </c>
       <c r="D223" s="38" t="n">
         <v>1</v>
@@ -11288,13 +11294,13 @@
       </c>
       <c r="F223" s="38"/>
       <c r="G223" s="38" t="s">
-        <v>445</v>
+        <v>447</v>
       </c>
       <c r="H223" s="38" t="s">
         <v>27</v>
       </c>
       <c r="I223" s="38" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="J223" s="44" t="n">
         <f aca="false">J221+D221</f>
@@ -11313,7 +11319,7 @@
         <v>2</v>
       </c>
       <c r="N223" s="1" t="s">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="O223" s="3" t="n">
         <v>1</v>
@@ -11327,10 +11333,10 @@
     </row>
     <row r="224" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B224" s="43" t="s">
-        <v>447</v>
+        <v>449</v>
       </c>
       <c r="C224" s="38" t="s">
-        <v>447</v>
+        <v>449</v>
       </c>
       <c r="D224" s="38" t="n">
         <v>5</v>
@@ -11344,7 +11350,7 @@
       </c>
       <c r="H224" s="38"/>
       <c r="I224" s="38" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="J224" s="44" t="n">
         <f aca="false">J223+D223</f>
@@ -11363,7 +11369,7 @@
         <v>2.03125</v>
       </c>
       <c r="N224" s="1" t="s">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="O224" s="3" t="n">
         <v>1</v>
@@ -11377,10 +11383,10 @@
     </row>
     <row r="225" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B225" s="43" t="s">
-        <v>449</v>
+        <v>451</v>
       </c>
       <c r="C225" s="38" t="s">
-        <v>449</v>
+        <v>451</v>
       </c>
       <c r="D225" s="38" t="n">
         <v>4</v>
@@ -11396,7 +11402,7 @@
         <v>27</v>
       </c>
       <c r="I225" s="38" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="J225" s="44" t="n">
         <f aca="false">J224+D224</f>
@@ -11415,7 +11421,7 @@
         <v>2.1875</v>
       </c>
       <c r="N225" s="1" t="s">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="O225" s="3" t="n">
         <v>1</v>
@@ -11429,10 +11435,10 @@
     </row>
     <row r="226" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B226" s="43" t="s">
-        <v>450</v>
+        <v>452</v>
       </c>
       <c r="C226" s="38" t="s">
-        <v>450</v>
+        <v>452</v>
       </c>
       <c r="D226" s="38" t="n">
         <v>5</v>
@@ -11448,7 +11454,7 @@
         <v>27</v>
       </c>
       <c r="I226" s="38" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="J226" s="44" t="n">
         <f aca="false">J225+D225</f>
@@ -11467,7 +11473,7 @@
         <v>2.3125</v>
       </c>
       <c r="N226" s="1" t="s">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="O226" s="3" t="n">
         <v>1</v>
@@ -11481,10 +11487,10 @@
     </row>
     <row r="227" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B227" s="43" t="s">
-        <v>451</v>
+        <v>453</v>
       </c>
       <c r="C227" s="38" t="s">
-        <v>451</v>
+        <v>453</v>
       </c>
       <c r="D227" s="38" t="n">
         <v>6</v>
@@ -11500,7 +11506,7 @@
         <v>27</v>
       </c>
       <c r="I227" s="38" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="J227" s="44" t="n">
         <f aca="false">J226+D226</f>
@@ -11519,7 +11525,7 @@
         <v>2.46875</v>
       </c>
       <c r="N227" s="1" t="s">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="O227" s="3" t="n">
         <v>1</v>
@@ -11533,10 +11539,10 @@
     </row>
     <row r="228" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B228" s="43" t="s">
-        <v>452</v>
+        <v>454</v>
       </c>
       <c r="C228" s="38" t="s">
-        <v>452</v>
+        <v>454</v>
       </c>
       <c r="D228" s="38" t="n">
         <v>6</v>
@@ -11552,7 +11558,7 @@
         <v>27</v>
       </c>
       <c r="I228" s="38" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="J228" s="44" t="n">
         <f aca="false">J227+D227</f>
@@ -11571,7 +11577,7 @@
         <v>2.65625</v>
       </c>
       <c r="N228" s="1" t="s">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="O228" s="3" t="n">
         <v>1</v>
@@ -11585,10 +11591,10 @@
     </row>
     <row r="229" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B229" s="43" t="s">
-        <v>453</v>
+        <v>455</v>
       </c>
       <c r="C229" s="38" t="s">
-        <v>453</v>
+        <v>455</v>
       </c>
       <c r="D229" s="38" t="n">
         <v>5</v>
@@ -11604,7 +11610,7 @@
         <v>27</v>
       </c>
       <c r="I229" s="38" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="J229" s="44" t="n">
         <f aca="false">J228+D228</f>
@@ -11623,7 +11629,7 @@
         <v>2.84375</v>
       </c>
       <c r="N229" s="1" t="s">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="O229" s="3" t="n">
         <v>1</v>
@@ -11637,7 +11643,7 @@
     </row>
     <row r="230" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A230" s="1" t="s">
-        <v>454</v>
+        <v>456</v>
       </c>
       <c r="B230" s="43"/>
       <c r="C230" s="38"/>
@@ -11654,10 +11660,10 @@
     </row>
     <row r="231" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B231" s="43" t="s">
-        <v>455</v>
+        <v>457</v>
       </c>
       <c r="C231" s="38" t="s">
-        <v>455</v>
+        <v>457</v>
       </c>
       <c r="D231" s="38" t="n">
         <v>8</v>
@@ -11673,7 +11679,7 @@
         <v>71</v>
       </c>
       <c r="I231" s="38" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="J231" s="44" t="n">
         <f aca="false">J229+D229</f>
@@ -11692,7 +11698,7 @@
         <v>3</v>
       </c>
       <c r="N231" s="1" t="s">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="O231" s="3" t="n">
         <v>1</v>
@@ -11706,10 +11712,10 @@
     </row>
     <row r="232" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B232" s="43" t="s">
-        <v>456</v>
+        <v>458</v>
       </c>
       <c r="C232" s="38" t="s">
-        <v>456</v>
+        <v>458</v>
       </c>
       <c r="D232" s="38" t="n">
         <v>8</v>
@@ -11725,7 +11731,7 @@
         <v>71</v>
       </c>
       <c r="I232" s="38" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="J232" s="44" t="n">
         <f aca="false">J231+D231</f>
@@ -11744,7 +11750,7 @@
         <v>3.25</v>
       </c>
       <c r="N232" s="1" t="s">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="O232" s="3" t="n">
         <v>1</v>
@@ -11758,10 +11764,10 @@
     </row>
     <row r="233" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B233" s="43" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
       <c r="C233" s="38" t="s">
-        <v>458</v>
+        <v>460</v>
       </c>
       <c r="D233" s="38" t="n">
         <v>16</v>
@@ -11777,7 +11783,7 @@
         <v>27</v>
       </c>
       <c r="I233" s="38" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="J233" s="44" t="n">
         <f aca="false">J232+D232</f>
@@ -11840,7 +11846,7 @@
     </row>
     <row r="235" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A235" s="42" t="s">
-        <v>459</v>
+        <v>461</v>
       </c>
       <c r="F235" s="38"/>
       <c r="G235" s="38"/>
@@ -11924,10 +11930,10 @@
     </row>
     <row r="238" s="47" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B238" s="21" t="s">
-        <v>460</v>
+        <v>462</v>
       </c>
       <c r="C238" s="45" t="s">
-        <v>461</v>
+        <v>463</v>
       </c>
       <c r="D238" s="1" t="n">
         <v>5</v>
@@ -11943,7 +11949,7 @@
         <v>27</v>
       </c>
       <c r="I238" s="38" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="J238" s="44" t="n">
         <f aca="false">J234</f>
@@ -11976,10 +11982,10 @@
     </row>
     <row r="239" s="47" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B239" s="21" t="s">
-        <v>462</v>
+        <v>464</v>
       </c>
       <c r="C239" s="45" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="D239" s="1" t="n">
         <v>1</v>
@@ -11989,13 +11995,13 @@
       </c>
       <c r="F239" s="46"/>
       <c r="G239" s="38" t="s">
-        <v>445</v>
+        <v>447</v>
       </c>
       <c r="H239" s="38" t="s">
         <v>27</v>
       </c>
       <c r="I239" s="38" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="J239" s="44" t="n">
         <f aca="false">J238+D238</f>
@@ -12014,7 +12020,7 @@
         <v>4.15625</v>
       </c>
       <c r="N239" s="1" t="s">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="O239" s="3" t="n">
         <v>1</v>
@@ -12028,10 +12034,10 @@
     </row>
     <row r="240" s="47" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B240" s="21" t="s">
-        <v>464</v>
+        <v>466</v>
       </c>
       <c r="C240" s="45" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="D240" s="1" t="n">
         <v>1</v>
@@ -12041,13 +12047,13 @@
       </c>
       <c r="F240" s="46"/>
       <c r="G240" s="38" t="s">
-        <v>445</v>
+        <v>447</v>
       </c>
       <c r="H240" s="38" t="s">
         <v>27</v>
       </c>
       <c r="I240" s="38" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="J240" s="44" t="n">
         <f aca="false">J239+D239</f>
@@ -12066,7 +12072,7 @@
         <v>4.1875</v>
       </c>
       <c r="N240" s="1" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="O240" s="3" t="n">
         <v>2</v>
@@ -12080,10 +12086,10 @@
     </row>
     <row r="241" s="47" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B241" s="21" t="s">
-        <v>467</v>
+        <v>469</v>
       </c>
       <c r="C241" s="45" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="D241" s="1" t="n">
         <v>3</v>
@@ -12099,7 +12105,7 @@
         <v>27</v>
       </c>
       <c r="I241" s="38" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="J241" s="44" t="n">
         <f aca="false">J240+D240</f>
@@ -12118,7 +12124,7 @@
         <v>4.21875</v>
       </c>
       <c r="N241" s="1" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="O241" s="3" t="n">
         <v>2</v>
@@ -12132,10 +12138,10 @@
     </row>
     <row r="242" s="47" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B242" s="21" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="C242" s="45" t="s">
-        <v>470</v>
+        <v>472</v>
       </c>
       <c r="D242" s="1" t="n">
         <v>4</v>
@@ -12145,13 +12151,13 @@
       </c>
       <c r="F242" s="46"/>
       <c r="G242" s="38" t="s">
-        <v>471</v>
+        <v>473</v>
       </c>
       <c r="H242" s="38" t="s">
         <v>27</v>
       </c>
       <c r="I242" s="38" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="J242" s="44" t="n">
         <f aca="false">J241+D241</f>
@@ -12170,7 +12176,7 @@
         <v>4.3125</v>
       </c>
       <c r="N242" s="1" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="O242" s="3" t="n">
         <v>2</v>
@@ -12184,10 +12190,10 @@
     </row>
     <row r="243" s="47" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B243" s="21" t="s">
-        <v>472</v>
+        <v>474</v>
       </c>
       <c r="C243" s="45" t="s">
-        <v>473</v>
+        <v>475</v>
       </c>
       <c r="D243" s="1" t="n">
         <v>4</v>
@@ -12197,13 +12203,13 @@
       </c>
       <c r="F243" s="46"/>
       <c r="G243" s="38" t="s">
-        <v>471</v>
+        <v>473</v>
       </c>
       <c r="H243" s="38" t="s">
         <v>27</v>
       </c>
       <c r="I243" s="38" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="J243" s="44" t="n">
         <f aca="false">J242+D242</f>
@@ -12222,7 +12228,7 @@
         <v>4.4375</v>
       </c>
       <c r="N243" s="1" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="O243" s="3" t="n">
         <v>2</v>
@@ -12236,10 +12242,10 @@
     </row>
     <row r="244" s="47" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B244" s="21" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="C244" s="45" t="s">
-        <v>475</v>
+        <v>477</v>
       </c>
       <c r="D244" s="1" t="n">
         <v>5</v>
@@ -12249,13 +12255,13 @@
       </c>
       <c r="F244" s="46"/>
       <c r="G244" s="38" t="s">
-        <v>476</v>
+        <v>478</v>
       </c>
       <c r="H244" s="38" t="s">
         <v>27</v>
       </c>
       <c r="I244" s="38" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="J244" s="44" t="n">
         <f aca="false">J243+D243</f>
@@ -12274,7 +12280,7 @@
         <v>4.5625</v>
       </c>
       <c r="N244" s="1" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="O244" s="3" t="n">
         <v>2</v>
@@ -12288,10 +12294,10 @@
     </row>
     <row r="245" s="47" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B245" s="21" t="s">
-        <v>477</v>
+        <v>479</v>
       </c>
       <c r="C245" s="45" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="D245" s="1" t="n">
         <v>9</v>
@@ -12307,7 +12313,7 @@
         <v>27</v>
       </c>
       <c r="I245" s="38" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="J245" s="44" t="n">
         <f aca="false">J244+D244</f>
@@ -12326,7 +12332,7 @@
         <v>4.71875</v>
       </c>
       <c r="N245" s="1" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="O245" s="3" t="n">
         <v>2</v>
@@ -12359,10 +12365,10 @@
     </row>
     <row r="247" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B247" s="47" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="C247" s="3" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="D247" s="1" t="n">
         <v>8</v>
@@ -12378,7 +12384,7 @@
         <v>27</v>
       </c>
       <c r="I247" s="38" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="J247" s="44" t="n">
         <f aca="false">J245+D245</f>
@@ -12397,7 +12403,7 @@
         <v>5</v>
       </c>
       <c r="N247" s="1" t="s">
-        <v>481</v>
+        <v>483</v>
       </c>
       <c r="O247" s="3" t="n">
         <v>3</v>
@@ -12411,10 +12417,10 @@
     </row>
     <row r="248" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B248" s="47" t="s">
-        <v>482</v>
+        <v>484</v>
       </c>
       <c r="C248" s="3" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="D248" s="1" t="n">
         <v>8</v>
@@ -12430,7 +12436,7 @@
         <v>27</v>
       </c>
       <c r="I248" s="38" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="J248" s="44" t="n">
         <f aca="false">J247+D247</f>
@@ -12449,7 +12455,7 @@
         <v>5.25</v>
       </c>
       <c r="N248" s="1" t="s">
-        <v>481</v>
+        <v>483</v>
       </c>
       <c r="O248" s="3" t="n">
         <v>3</v>
@@ -12463,10 +12469,10 @@
     </row>
     <row r="249" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B249" s="47" t="s">
-        <v>484</v>
+        <v>486</v>
       </c>
       <c r="C249" s="3" t="s">
-        <v>485</v>
+        <v>487</v>
       </c>
       <c r="D249" s="1" t="n">
         <v>8</v>
@@ -12482,7 +12488,7 @@
         <v>27</v>
       </c>
       <c r="I249" s="38" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="J249" s="44" t="n">
         <f aca="false">J248+D248</f>
@@ -12501,7 +12507,7 @@
         <v>5.5</v>
       </c>
       <c r="N249" s="1" t="s">
-        <v>481</v>
+        <v>483</v>
       </c>
       <c r="O249" s="3" t="n">
         <v>3</v>
@@ -12515,10 +12521,10 @@
     </row>
     <row r="250" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B250" s="47" t="s">
-        <v>486</v>
+        <v>488</v>
       </c>
       <c r="C250" s="3" t="s">
-        <v>487</v>
+        <v>489</v>
       </c>
       <c r="D250" s="1" t="n">
         <v>8</v>
@@ -12534,7 +12540,7 @@
         <v>27</v>
       </c>
       <c r="I250" s="38" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="J250" s="44" t="n">
         <f aca="false">J249+D249</f>
@@ -12553,7 +12559,7 @@
         <v>5.75</v>
       </c>
       <c r="N250" s="1" t="s">
-        <v>481</v>
+        <v>483</v>
       </c>
       <c r="O250" s="3" t="n">
         <v>3</v>
@@ -12567,10 +12573,10 @@
     </row>
     <row r="251" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B251" s="47" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="C251" s="3" t="s">
-        <v>489</v>
+        <v>491</v>
       </c>
       <c r="D251" s="1" t="n">
         <v>8</v>
@@ -12586,7 +12592,7 @@
         <v>27</v>
       </c>
       <c r="I251" s="38" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="J251" s="44" t="n">
         <f aca="false">J250+D250</f>
@@ -12605,7 +12611,7 @@
         <v>6</v>
       </c>
       <c r="N251" s="1" t="s">
-        <v>481</v>
+        <v>483</v>
       </c>
       <c r="O251" s="3" t="n">
         <v>3</v>
@@ -12619,10 +12625,10 @@
     </row>
     <row r="252" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B252" s="47" t="s">
-        <v>490</v>
+        <v>492</v>
       </c>
       <c r="C252" s="3" t="s">
-        <v>491</v>
+        <v>493</v>
       </c>
       <c r="D252" s="1" t="n">
         <v>8</v>
@@ -12638,7 +12644,7 @@
         <v>27</v>
       </c>
       <c r="I252" s="38" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="J252" s="44" t="n">
         <f aca="false">J251+D251</f>
@@ -12657,7 +12663,7 @@
         <v>6.25</v>
       </c>
       <c r="N252" s="1" t="s">
-        <v>481</v>
+        <v>483</v>
       </c>
       <c r="O252" s="3" t="n">
         <v>3</v>
@@ -12671,10 +12677,10 @@
     </row>
     <row r="253" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B253" s="47" t="s">
-        <v>492</v>
+        <v>494</v>
       </c>
       <c r="C253" s="3" t="s">
-        <v>493</v>
+        <v>495</v>
       </c>
       <c r="D253" s="1" t="n">
         <v>8</v>
@@ -12690,7 +12696,7 @@
         <v>27</v>
       </c>
       <c r="I253" s="38" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="J253" s="44" t="n">
         <f aca="false">J252+D252</f>
@@ -12709,7 +12715,7 @@
         <v>6.5</v>
       </c>
       <c r="N253" s="1" t="s">
-        <v>481</v>
+        <v>483</v>
       </c>
       <c r="O253" s="3" t="n">
         <v>3</v>
@@ -12723,10 +12729,10 @@
     </row>
     <row r="254" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B254" s="47" t="s">
-        <v>494</v>
+        <v>496</v>
       </c>
       <c r="C254" s="3" t="s">
-        <v>495</v>
+        <v>497</v>
       </c>
       <c r="D254" s="1" t="n">
         <v>8</v>
@@ -12742,7 +12748,7 @@
         <v>27</v>
       </c>
       <c r="I254" s="38" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="J254" s="44" t="n">
         <f aca="false">J253+D253</f>
@@ -12761,7 +12767,7 @@
         <v>6.75</v>
       </c>
       <c r="N254" s="1" t="s">
-        <v>481</v>
+        <v>483</v>
       </c>
       <c r="O254" s="3" t="n">
         <v>3</v>
@@ -12775,10 +12781,10 @@
     </row>
     <row r="255" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B255" s="47" t="s">
-        <v>496</v>
+        <v>498</v>
       </c>
       <c r="C255" s="3" t="s">
-        <v>496</v>
+        <v>498</v>
       </c>
       <c r="D255" s="1" t="n">
         <v>8</v>
@@ -12794,7 +12800,7 @@
         <v>27</v>
       </c>
       <c r="I255" s="38" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="J255" s="44" t="n">
         <f aca="false">J254+D254</f>
@@ -12813,7 +12819,7 @@
         <v>7</v>
       </c>
       <c r="N255" s="1" t="s">
-        <v>481</v>
+        <v>483</v>
       </c>
       <c r="O255" s="3" t="n">
         <v>3</v>
@@ -12827,10 +12833,10 @@
     </row>
     <row r="256" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B256" s="47" t="s">
-        <v>497</v>
+        <v>499</v>
       </c>
       <c r="C256" s="3" t="s">
-        <v>497</v>
+        <v>499</v>
       </c>
       <c r="D256" s="1" t="n">
         <v>8</v>
@@ -12846,7 +12852,7 @@
         <v>27</v>
       </c>
       <c r="I256" s="38" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="J256" s="44" t="n">
         <f aca="false">J255+D255</f>
@@ -12865,7 +12871,7 @@
         <v>7.25</v>
       </c>
       <c r="N256" s="1" t="s">
-        <v>481</v>
+        <v>483</v>
       </c>
       <c r="O256" s="3" t="n">
         <v>3</v>
@@ -12879,10 +12885,10 @@
     </row>
     <row r="257" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B257" s="47" t="s">
-        <v>498</v>
+        <v>500</v>
       </c>
       <c r="C257" s="3" t="s">
-        <v>498</v>
+        <v>500</v>
       </c>
       <c r="D257" s="1" t="n">
         <v>8</v>
@@ -12898,7 +12904,7 @@
         <v>27</v>
       </c>
       <c r="I257" s="38" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="J257" s="44" t="n">
         <f aca="false">J256+D256</f>
@@ -12917,7 +12923,7 @@
         <v>7.5</v>
       </c>
       <c r="N257" s="1" t="s">
-        <v>481</v>
+        <v>483</v>
       </c>
       <c r="O257" s="3" t="n">
         <v>3</v>
@@ -12931,10 +12937,10 @@
     </row>
     <row r="258" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B258" s="47" t="s">
-        <v>499</v>
+        <v>501</v>
       </c>
       <c r="C258" s="3" t="s">
-        <v>499</v>
+        <v>501</v>
       </c>
       <c r="D258" s="1" t="n">
         <v>8</v>
@@ -12950,7 +12956,7 @@
         <v>27</v>
       </c>
       <c r="I258" s="38" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="J258" s="44" t="n">
         <f aca="false">J257+D257</f>
@@ -12969,7 +12975,7 @@
         <v>7.75</v>
       </c>
       <c r="N258" s="1" t="s">
-        <v>481</v>
+        <v>483</v>
       </c>
       <c r="O258" s="3" t="n">
         <v>3</v>
@@ -12983,10 +12989,10 @@
     </row>
     <row r="259" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B259" s="47" t="s">
-        <v>500</v>
+        <v>502</v>
       </c>
       <c r="C259" s="3" t="s">
-        <v>500</v>
+        <v>502</v>
       </c>
       <c r="D259" s="1" t="n">
         <v>8</v>
@@ -13002,7 +13008,7 @@
         <v>27</v>
       </c>
       <c r="I259" s="38" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="J259" s="44" t="n">
         <f aca="false">J258+D258</f>
@@ -13021,7 +13027,7 @@
         <v>8</v>
       </c>
       <c r="N259" s="1" t="s">
-        <v>481</v>
+        <v>483</v>
       </c>
       <c r="O259" s="3" t="n">
         <v>3</v>
@@ -13035,10 +13041,10 @@
     </row>
     <row r="260" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B260" s="47" t="s">
-        <v>501</v>
+        <v>503</v>
       </c>
       <c r="C260" s="3" t="s">
-        <v>502</v>
+        <v>504</v>
       </c>
       <c r="D260" s="1" t="n">
         <v>16</v>
@@ -13056,7 +13062,7 @@
         <v>27</v>
       </c>
       <c r="I260" s="38" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="J260" s="44" t="n">
         <f aca="false">J259+D259</f>
@@ -13075,7 +13081,7 @@
         <v>8.25</v>
       </c>
       <c r="N260" s="1" t="s">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="O260" s="3" t="n">
         <v>1</v>
@@ -13089,10 +13095,10 @@
     </row>
     <row r="261" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B261" s="47" t="s">
-        <v>503</v>
+        <v>505</v>
       </c>
       <c r="C261" s="3" t="s">
-        <v>504</v>
+        <v>506</v>
       </c>
       <c r="D261" s="1" t="n">
         <v>8</v>
@@ -13108,7 +13114,7 @@
         <v>27</v>
       </c>
       <c r="I261" s="38" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="J261" s="44" t="n">
         <f aca="false">J260+D260</f>
@@ -13127,7 +13133,7 @@
         <v>8.75</v>
       </c>
       <c r="N261" s="1" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="O261" s="3" t="n">
         <v>2</v>
@@ -13218,7 +13224,7 @@
       <selection pane="topLeft" activeCell="C33" activeCellId="0" sqref="C33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.07421875" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.09375" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="40" width="20.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="40" width="16.11"/>
@@ -13229,22 +13235,22 @@
     <row r="6" s="49" customFormat="true" ht="34.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B6" s="50"/>
       <c r="C6" s="50" t="s">
-        <v>505</v>
+        <v>507</v>
       </c>
       <c r="D6" s="50" t="s">
-        <v>506</v>
+        <v>508</v>
       </c>
       <c r="E6" s="50" t="s">
-        <v>507</v>
+        <v>509</v>
       </c>
       <c r="F6" s="50" t="s">
-        <v>508</v>
+        <v>510</v>
       </c>
       <c r="G6" s="50" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="H6" s="50" t="s">
-        <v>509</v>
+        <v>511</v>
       </c>
       <c r="I6" s="50"/>
     </row>
@@ -13614,10 +13620,10 @@
     </row>
     <row r="26" s="1" customFormat="true" ht="37.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="32" t="s">
-        <v>510</v>
+        <v>512</v>
       </c>
       <c r="C26" s="32" t="s">
-        <v>511</v>
+        <v>513</v>
       </c>
       <c r="D26" s="27" t="n">
         <v>16</v>
@@ -13666,10 +13672,10 @@
     </row>
     <row r="27" s="1" customFormat="true" ht="37.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="32" t="s">
-        <v>512</v>
+        <v>514</v>
       </c>
       <c r="C27" s="32" t="s">
-        <v>513</v>
+        <v>515</v>
       </c>
       <c r="D27" s="27" t="n">
         <v>32</v>
@@ -13716,16 +13722,16 @@
     </row>
     <row r="30" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="52" t="s">
-        <v>514</v>
+        <v>516</v>
       </c>
       <c r="C30" s="52" t="s">
-        <v>515</v>
+        <v>517</v>
       </c>
       <c r="D30" s="52" t="s">
-        <v>516</v>
+        <v>518</v>
       </c>
       <c r="E30" s="52" t="s">
-        <v>517</v>
+        <v>519</v>
       </c>
       <c r="F30" s="52"/>
     </row>

</xml_diff>

<commit_message>
Fix (again) the pad bit names
Now I'm using the spreadsheet line number as part of the pad name to avoid
duplicates
</commit_message>
<xml_diff>
--- a/genSpacecraft/DownlinkSpecLTM.xlsx
+++ b/genSpacecraft/DownlinkSpecLTM.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1401" uniqueCount="520">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1401" uniqueCount="522">
   <si>
     <t xml:space="preserve">//</t>
   </si>
@@ -191,7 +191,7 @@
     <t xml:space="preserve">Pad10</t>
   </si>
   <si>
-    <t xml:space="preserve">pad10</t>
+    <t xml:space="preserve">pad20</t>
   </si>
   <si>
     <t xml:space="preserve">Pad</t>
@@ -1157,7 +1157,7 @@
     <t xml:space="preserve">Structure: realtimeSpecific_t, file:realtimeDownlink.h</t>
   </si>
   <si>
-    <t xml:space="preserve">Pad5</t>
+    <t xml:space="preserve">Pad161</t>
   </si>
   <si>
     <t xml:space="preserve">Structure: maxSpecific_t, file: maxDownlink.h</t>
@@ -1202,7 +1202,7 @@
     <t xml:space="preserve">Filler</t>
   </si>
   <si>
-    <t xml:space="preserve">pad0</t>
+    <t xml:space="preserve">pad168</t>
   </si>
   <si>
     <t xml:space="preserve">Make same length as WOD</t>
@@ -1253,7 +1253,7 @@
     <t xml:space="preserve">CRC Error for the min payload</t>
   </si>
   <si>
-    <t xml:space="preserve">Pad4</t>
+    <t xml:space="preserve">Pad178</t>
   </si>
   <si>
     <t xml:space="preserve">Structure:wodSpecific_t,file:wodSpecificDownlink.h</t>
@@ -1286,6 +1286,9 @@
     <t xml:space="preserve">CRC Error for the WOD Payload</t>
   </si>
   <si>
+    <t xml:space="preserve">pad191</t>
+  </si>
+  <si>
     <t xml:space="preserve">Structure:scienceLong_t, file:sciLongDownlink.h</t>
   </si>
   <si>
@@ -1335,6 +1338,9 @@
   </si>
   <si>
     <t xml:space="preserve">CRC Error for VU Radiataion Payload</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pad215</t>
   </si>
   <si>
     <t xml:space="preserve">Structure:infrequentDownlink_t,file:infrequentDownlink.h</t>
@@ -1958,8 +1964,8 @@
   </sheetPr>
   <dimension ref="A1:Q264"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B229" activeCellId="0" sqref="B229"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A12" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10221,7 +10227,7 @@
         <v>55</v>
       </c>
       <c r="C191" s="22" t="s">
-        <v>56</v>
+        <v>421</v>
       </c>
       <c r="D191" s="22" t="n">
         <v>5</v>
@@ -10310,7 +10316,7 @@
     </row>
     <row r="194" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="40" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="B194" s="11"/>
       <c r="C194" s="41"/>
@@ -10376,10 +10382,10 @@
     </row>
     <row r="196" customFormat="false" ht="37.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B196" s="31" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="C196" s="22" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="D196" s="22" t="n">
         <v>5248</v>
@@ -10397,7 +10403,7 @@
         <v>27</v>
       </c>
       <c r="I196" s="23" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="J196" s="4" t="n">
         <v>0</v>
@@ -10429,10 +10435,10 @@
     </row>
     <row r="197" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B197" s="31" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="C197" s="22" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="D197" s="22" t="n">
         <v>7</v>
@@ -10469,10 +10475,10 @@
     </row>
     <row r="198" customFormat="false" ht="25.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B198" s="31" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="C198" s="22" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="D198" s="22" t="n">
         <v>1</v>
@@ -10486,7 +10492,7 @@
       </c>
       <c r="H198" s="22"/>
       <c r="I198" s="23" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="J198" s="4" t="n">
         <f aca="false">J197+D197</f>
@@ -10550,7 +10556,7 @@
     </row>
     <row r="201" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="42" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="B201" s="11"/>
       <c r="C201" s="41"/>
@@ -10616,10 +10622,10 @@
     </row>
     <row r="203" customFormat="false" ht="37.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B203" s="31" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="C203" s="22" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="D203" s="22" t="n">
         <v>664</v>
@@ -10637,7 +10643,7 @@
         <v>27</v>
       </c>
       <c r="I203" s="23" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="J203" s="4" t="n">
         <v>0</v>
@@ -10669,10 +10675,10 @@
     </row>
     <row r="204" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B204" s="31" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="C204" s="22" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="D204" s="22" t="n">
         <v>7</v>
@@ -10721,10 +10727,10 @@
     </row>
     <row r="205" customFormat="false" ht="25.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B205" s="31" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="C205" s="22" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="D205" s="22" t="n">
         <v>1</v>
@@ -10738,7 +10744,7 @@
       </c>
       <c r="H205" s="22"/>
       <c r="I205" s="23" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="J205" s="4" t="n">
         <f aca="false">J204+D204</f>
@@ -10795,7 +10801,7 @@
     </row>
     <row r="210" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A210" s="42" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="B210" s="11"/>
       <c r="C210" s="41"/>
@@ -10877,7 +10883,7 @@
         <v>1</v>
       </c>
       <c r="H212" s="39" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="I212" s="28" t="s">
         <v>414</v>
@@ -10913,7 +10919,7 @@
     </row>
     <row r="213" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B213" s="31" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="C213" s="32" t="s">
         <v>417</v>
@@ -10925,7 +10931,7 @@
         <v>26</v>
       </c>
       <c r="F213" s="23" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="G213" s="39" t="n">
         <v>1</v>
@@ -10984,7 +10990,7 @@
         <v>27</v>
       </c>
       <c r="I214" s="28" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="J214" s="4" t="n">
         <f aca="false">J213+D213</f>
@@ -11020,7 +11026,7 @@
         <v>28</v>
       </c>
       <c r="C215" s="32" t="s">
-        <v>393</v>
+        <v>439</v>
       </c>
       <c r="D215" s="27" t="n">
         <v>8</v>
@@ -11103,7 +11109,7 @@
     </row>
     <row r="218" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A218" s="42" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
     </row>
     <row r="219" s="14" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11177,10 +11183,10 @@
         <v>133</v>
       </c>
       <c r="H220" s="38" t="s">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="I220" s="38" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
       <c r="J220" s="44" t="n">
         <v>0</v>
@@ -11198,7 +11204,7 @@
         <v>0</v>
       </c>
       <c r="N220" s="1" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="O220" s="3" t="n">
         <v>1</v>
@@ -11212,10 +11218,10 @@
     </row>
     <row r="221" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B221" s="43" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="C221" s="38" t="s">
-        <v>443</v>
+        <v>445</v>
       </c>
       <c r="D221" s="38" t="n">
         <v>32</v>
@@ -11228,10 +11234,10 @@
         <v>133</v>
       </c>
       <c r="H221" s="38" t="s">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="I221" s="38" t="s">
-        <v>444</v>
+        <v>446</v>
       </c>
       <c r="J221" s="44" t="n">
         <f aca="false">J220+D220</f>
@@ -11250,7 +11256,7 @@
         <v>1</v>
       </c>
       <c r="N221" s="1" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="O221" s="3" t="n">
         <v>1</v>
@@ -11264,7 +11270,7 @@
     </row>
     <row r="222" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A222" s="1" t="s">
-        <v>445</v>
+        <v>447</v>
       </c>
       <c r="B222" s="43"/>
       <c r="C222" s="38"/>
@@ -11281,10 +11287,10 @@
     </row>
     <row r="223" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B223" s="43" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="C223" s="38" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="D223" s="38" t="n">
         <v>1</v>
@@ -11294,13 +11300,13 @@
       </c>
       <c r="F223" s="38"/>
       <c r="G223" s="38" t="s">
-        <v>447</v>
+        <v>449</v>
       </c>
       <c r="H223" s="38" t="s">
         <v>27</v>
       </c>
       <c r="I223" s="38" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="J223" s="44" t="n">
         <f aca="false">J221+D221</f>
@@ -11319,7 +11325,7 @@
         <v>2</v>
       </c>
       <c r="N223" s="1" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="O223" s="3" t="n">
         <v>1</v>
@@ -11333,10 +11339,10 @@
     </row>
     <row r="224" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B224" s="43" t="s">
-        <v>449</v>
+        <v>451</v>
       </c>
       <c r="C224" s="38" t="s">
-        <v>449</v>
+        <v>451</v>
       </c>
       <c r="D224" s="38" t="n">
         <v>5</v>
@@ -11350,7 +11356,7 @@
       </c>
       <c r="H224" s="38"/>
       <c r="I224" s="38" t="s">
-        <v>450</v>
+        <v>452</v>
       </c>
       <c r="J224" s="44" t="n">
         <f aca="false">J223+D223</f>
@@ -11369,7 +11375,7 @@
         <v>2.03125</v>
       </c>
       <c r="N224" s="1" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="O224" s="3" t="n">
         <v>1</v>
@@ -11383,10 +11389,10 @@
     </row>
     <row r="225" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B225" s="43" t="s">
-        <v>451</v>
+        <v>453</v>
       </c>
       <c r="C225" s="38" t="s">
-        <v>451</v>
+        <v>453</v>
       </c>
       <c r="D225" s="38" t="n">
         <v>4</v>
@@ -11402,7 +11408,7 @@
         <v>27</v>
       </c>
       <c r="I225" s="38" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="J225" s="44" t="n">
         <f aca="false">J224+D224</f>
@@ -11421,7 +11427,7 @@
         <v>2.1875</v>
       </c>
       <c r="N225" s="1" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="O225" s="3" t="n">
         <v>1</v>
@@ -11435,10 +11441,10 @@
     </row>
     <row r="226" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B226" s="43" t="s">
-        <v>452</v>
+        <v>454</v>
       </c>
       <c r="C226" s="38" t="s">
-        <v>452</v>
+        <v>454</v>
       </c>
       <c r="D226" s="38" t="n">
         <v>5</v>
@@ -11454,7 +11460,7 @@
         <v>27</v>
       </c>
       <c r="I226" s="38" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="J226" s="44" t="n">
         <f aca="false">J225+D225</f>
@@ -11473,7 +11479,7 @@
         <v>2.3125</v>
       </c>
       <c r="N226" s="1" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="O226" s="3" t="n">
         <v>1</v>
@@ -11487,10 +11493,10 @@
     </row>
     <row r="227" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B227" s="43" t="s">
-        <v>453</v>
+        <v>455</v>
       </c>
       <c r="C227" s="38" t="s">
-        <v>453</v>
+        <v>455</v>
       </c>
       <c r="D227" s="38" t="n">
         <v>6</v>
@@ -11506,7 +11512,7 @@
         <v>27</v>
       </c>
       <c r="I227" s="38" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="J227" s="44" t="n">
         <f aca="false">J226+D226</f>
@@ -11525,7 +11531,7 @@
         <v>2.46875</v>
       </c>
       <c r="N227" s="1" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="O227" s="3" t="n">
         <v>1</v>
@@ -11539,10 +11545,10 @@
     </row>
     <row r="228" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B228" s="43" t="s">
-        <v>454</v>
+        <v>456</v>
       </c>
       <c r="C228" s="38" t="s">
-        <v>454</v>
+        <v>456</v>
       </c>
       <c r="D228" s="38" t="n">
         <v>6</v>
@@ -11558,7 +11564,7 @@
         <v>27</v>
       </c>
       <c r="I228" s="38" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="J228" s="44" t="n">
         <f aca="false">J227+D227</f>
@@ -11577,7 +11583,7 @@
         <v>2.65625</v>
       </c>
       <c r="N228" s="1" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="O228" s="3" t="n">
         <v>1</v>
@@ -11591,10 +11597,10 @@
     </row>
     <row r="229" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B229" s="43" t="s">
-        <v>455</v>
+        <v>457</v>
       </c>
       <c r="C229" s="38" t="s">
-        <v>455</v>
+        <v>457</v>
       </c>
       <c r="D229" s="38" t="n">
         <v>5</v>
@@ -11610,7 +11616,7 @@
         <v>27</v>
       </c>
       <c r="I229" s="38" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="J229" s="44" t="n">
         <f aca="false">J228+D228</f>
@@ -11629,7 +11635,7 @@
         <v>2.84375</v>
       </c>
       <c r="N229" s="1" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="O229" s="3" t="n">
         <v>1</v>
@@ -11643,7 +11649,7 @@
     </row>
     <row r="230" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A230" s="1" t="s">
-        <v>456</v>
+        <v>458</v>
       </c>
       <c r="B230" s="43"/>
       <c r="C230" s="38"/>
@@ -11660,10 +11666,10 @@
     </row>
     <row r="231" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B231" s="43" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
       <c r="C231" s="38" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
       <c r="D231" s="38" t="n">
         <v>8</v>
@@ -11679,7 +11685,7 @@
         <v>71</v>
       </c>
       <c r="I231" s="38" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="J231" s="44" t="n">
         <f aca="false">J229+D229</f>
@@ -11698,7 +11704,7 @@
         <v>3</v>
       </c>
       <c r="N231" s="1" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="O231" s="3" t="n">
         <v>1</v>
@@ -11712,10 +11718,10 @@
     </row>
     <row r="232" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B232" s="43" t="s">
-        <v>458</v>
+        <v>460</v>
       </c>
       <c r="C232" s="38" t="s">
-        <v>458</v>
+        <v>460</v>
       </c>
       <c r="D232" s="38" t="n">
         <v>8</v>
@@ -11731,7 +11737,7 @@
         <v>71</v>
       </c>
       <c r="I232" s="38" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="J232" s="44" t="n">
         <f aca="false">J231+D231</f>
@@ -11750,7 +11756,7 @@
         <v>3.25</v>
       </c>
       <c r="N232" s="1" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="O232" s="3" t="n">
         <v>1</v>
@@ -11764,10 +11770,10 @@
     </row>
     <row r="233" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B233" s="43" t="s">
-        <v>459</v>
+        <v>461</v>
       </c>
       <c r="C233" s="38" t="s">
-        <v>460</v>
+        <v>462</v>
       </c>
       <c r="D233" s="38" t="n">
         <v>16</v>
@@ -11783,7 +11789,7 @@
         <v>27</v>
       </c>
       <c r="I233" s="38" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="J233" s="44" t="n">
         <f aca="false">J232+D232</f>
@@ -11846,7 +11852,7 @@
     </row>
     <row r="235" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A235" s="42" t="s">
-        <v>461</v>
+        <v>463</v>
       </c>
       <c r="F235" s="38"/>
       <c r="G235" s="38"/>
@@ -11930,10 +11936,10 @@
     </row>
     <row r="238" s="47" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B238" s="21" t="s">
-        <v>462</v>
+        <v>464</v>
       </c>
       <c r="C238" s="45" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="D238" s="1" t="n">
         <v>5</v>
@@ -11949,7 +11955,7 @@
         <v>27</v>
       </c>
       <c r="I238" s="38" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="J238" s="44" t="n">
         <f aca="false">J234</f>
@@ -11982,10 +11988,10 @@
     </row>
     <row r="239" s="47" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B239" s="21" t="s">
-        <v>464</v>
+        <v>466</v>
       </c>
       <c r="C239" s="45" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="D239" s="1" t="n">
         <v>1</v>
@@ -11995,13 +12001,13 @@
       </c>
       <c r="F239" s="46"/>
       <c r="G239" s="38" t="s">
-        <v>447</v>
+        <v>449</v>
       </c>
       <c r="H239" s="38" t="s">
         <v>27</v>
       </c>
       <c r="I239" s="38" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="J239" s="44" t="n">
         <f aca="false">J238+D238</f>
@@ -12020,7 +12026,7 @@
         <v>4.15625</v>
       </c>
       <c r="N239" s="1" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="O239" s="3" t="n">
         <v>1</v>
@@ -12034,10 +12040,10 @@
     </row>
     <row r="240" s="47" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B240" s="21" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="C240" s="45" t="s">
-        <v>467</v>
+        <v>469</v>
       </c>
       <c r="D240" s="1" t="n">
         <v>1</v>
@@ -12047,13 +12053,13 @@
       </c>
       <c r="F240" s="46"/>
       <c r="G240" s="38" t="s">
-        <v>447</v>
+        <v>449</v>
       </c>
       <c r="H240" s="38" t="s">
         <v>27</v>
       </c>
       <c r="I240" s="38" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="J240" s="44" t="n">
         <f aca="false">J239+D239</f>
@@ -12072,7 +12078,7 @@
         <v>4.1875</v>
       </c>
       <c r="N240" s="1" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="O240" s="3" t="n">
         <v>2</v>
@@ -12086,10 +12092,10 @@
     </row>
     <row r="241" s="47" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B241" s="21" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="C241" s="45" t="s">
-        <v>470</v>
+        <v>472</v>
       </c>
       <c r="D241" s="1" t="n">
         <v>3</v>
@@ -12105,7 +12111,7 @@
         <v>27</v>
       </c>
       <c r="I241" s="38" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="J241" s="44" t="n">
         <f aca="false">J240+D240</f>
@@ -12124,7 +12130,7 @@
         <v>4.21875</v>
       </c>
       <c r="N241" s="1" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="O241" s="3" t="n">
         <v>2</v>
@@ -12138,10 +12144,10 @@
     </row>
     <row r="242" s="47" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B242" s="21" t="s">
-        <v>471</v>
+        <v>473</v>
       </c>
       <c r="C242" s="45" t="s">
-        <v>472</v>
+        <v>474</v>
       </c>
       <c r="D242" s="1" t="n">
         <v>4</v>
@@ -12151,13 +12157,13 @@
       </c>
       <c r="F242" s="46"/>
       <c r="G242" s="38" t="s">
-        <v>473</v>
+        <v>475</v>
       </c>
       <c r="H242" s="38" t="s">
         <v>27</v>
       </c>
       <c r="I242" s="38" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="J242" s="44" t="n">
         <f aca="false">J241+D241</f>
@@ -12176,7 +12182,7 @@
         <v>4.3125</v>
       </c>
       <c r="N242" s="1" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="O242" s="3" t="n">
         <v>2</v>
@@ -12190,10 +12196,10 @@
     </row>
     <row r="243" s="47" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B243" s="21" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="C243" s="45" t="s">
-        <v>475</v>
+        <v>477</v>
       </c>
       <c r="D243" s="1" t="n">
         <v>4</v>
@@ -12203,13 +12209,13 @@
       </c>
       <c r="F243" s="46"/>
       <c r="G243" s="38" t="s">
-        <v>473</v>
+        <v>475</v>
       </c>
       <c r="H243" s="38" t="s">
         <v>27</v>
       </c>
       <c r="I243" s="38" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="J243" s="44" t="n">
         <f aca="false">J242+D242</f>
@@ -12228,7 +12234,7 @@
         <v>4.4375</v>
       </c>
       <c r="N243" s="1" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="O243" s="3" t="n">
         <v>2</v>
@@ -12242,10 +12248,10 @@
     </row>
     <row r="244" s="47" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B244" s="21" t="s">
-        <v>476</v>
+        <v>478</v>
       </c>
       <c r="C244" s="45" t="s">
-        <v>477</v>
+        <v>479</v>
       </c>
       <c r="D244" s="1" t="n">
         <v>5</v>
@@ -12255,13 +12261,13 @@
       </c>
       <c r="F244" s="46"/>
       <c r="G244" s="38" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="H244" s="38" t="s">
         <v>27</v>
       </c>
       <c r="I244" s="38" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="J244" s="44" t="n">
         <f aca="false">J243+D243</f>
@@ -12280,7 +12286,7 @@
         <v>4.5625</v>
       </c>
       <c r="N244" s="1" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="O244" s="3" t="n">
         <v>2</v>
@@ -12294,10 +12300,10 @@
     </row>
     <row r="245" s="47" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B245" s="21" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="C245" s="45" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="D245" s="1" t="n">
         <v>9</v>
@@ -12313,7 +12319,7 @@
         <v>27</v>
       </c>
       <c r="I245" s="38" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="J245" s="44" t="n">
         <f aca="false">J244+D244</f>
@@ -12332,7 +12338,7 @@
         <v>4.71875</v>
       </c>
       <c r="N245" s="1" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="O245" s="3" t="n">
         <v>2</v>
@@ -12365,10 +12371,10 @@
     </row>
     <row r="247" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B247" s="47" t="s">
-        <v>481</v>
+        <v>483</v>
       </c>
       <c r="C247" s="3" t="s">
-        <v>482</v>
+        <v>484</v>
       </c>
       <c r="D247" s="1" t="n">
         <v>8</v>
@@ -12384,7 +12390,7 @@
         <v>27</v>
       </c>
       <c r="I247" s="38" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="J247" s="44" t="n">
         <f aca="false">J245+D245</f>
@@ -12403,7 +12409,7 @@
         <v>5</v>
       </c>
       <c r="N247" s="1" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="O247" s="3" t="n">
         <v>3</v>
@@ -12417,10 +12423,10 @@
     </row>
     <row r="248" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B248" s="47" t="s">
-        <v>484</v>
+        <v>486</v>
       </c>
       <c r="C248" s="3" t="s">
-        <v>485</v>
+        <v>487</v>
       </c>
       <c r="D248" s="1" t="n">
         <v>8</v>
@@ -12436,7 +12442,7 @@
         <v>27</v>
       </c>
       <c r="I248" s="38" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="J248" s="44" t="n">
         <f aca="false">J247+D247</f>
@@ -12455,7 +12461,7 @@
         <v>5.25</v>
       </c>
       <c r="N248" s="1" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="O248" s="3" t="n">
         <v>3</v>
@@ -12469,10 +12475,10 @@
     </row>
     <row r="249" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B249" s="47" t="s">
-        <v>486</v>
+        <v>488</v>
       </c>
       <c r="C249" s="3" t="s">
-        <v>487</v>
+        <v>489</v>
       </c>
       <c r="D249" s="1" t="n">
         <v>8</v>
@@ -12488,7 +12494,7 @@
         <v>27</v>
       </c>
       <c r="I249" s="38" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="J249" s="44" t="n">
         <f aca="false">J248+D248</f>
@@ -12507,7 +12513,7 @@
         <v>5.5</v>
       </c>
       <c r="N249" s="1" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="O249" s="3" t="n">
         <v>3</v>
@@ -12521,10 +12527,10 @@
     </row>
     <row r="250" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B250" s="47" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="C250" s="3" t="s">
-        <v>489</v>
+        <v>491</v>
       </c>
       <c r="D250" s="1" t="n">
         <v>8</v>
@@ -12540,7 +12546,7 @@
         <v>27</v>
       </c>
       <c r="I250" s="38" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="J250" s="44" t="n">
         <f aca="false">J249+D249</f>
@@ -12559,7 +12565,7 @@
         <v>5.75</v>
       </c>
       <c r="N250" s="1" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="O250" s="3" t="n">
         <v>3</v>
@@ -12573,10 +12579,10 @@
     </row>
     <row r="251" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B251" s="47" t="s">
-        <v>490</v>
+        <v>492</v>
       </c>
       <c r="C251" s="3" t="s">
-        <v>491</v>
+        <v>493</v>
       </c>
       <c r="D251" s="1" t="n">
         <v>8</v>
@@ -12592,7 +12598,7 @@
         <v>27</v>
       </c>
       <c r="I251" s="38" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="J251" s="44" t="n">
         <f aca="false">J250+D250</f>
@@ -12611,7 +12617,7 @@
         <v>6</v>
       </c>
       <c r="N251" s="1" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="O251" s="3" t="n">
         <v>3</v>
@@ -12625,10 +12631,10 @@
     </row>
     <row r="252" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B252" s="47" t="s">
-        <v>492</v>
+        <v>494</v>
       </c>
       <c r="C252" s="3" t="s">
-        <v>493</v>
+        <v>495</v>
       </c>
       <c r="D252" s="1" t="n">
         <v>8</v>
@@ -12644,7 +12650,7 @@
         <v>27</v>
       </c>
       <c r="I252" s="38" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="J252" s="44" t="n">
         <f aca="false">J251+D251</f>
@@ -12663,7 +12669,7 @@
         <v>6.25</v>
       </c>
       <c r="N252" s="1" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="O252" s="3" t="n">
         <v>3</v>
@@ -12677,10 +12683,10 @@
     </row>
     <row r="253" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B253" s="47" t="s">
-        <v>494</v>
+        <v>496</v>
       </c>
       <c r="C253" s="3" t="s">
-        <v>495</v>
+        <v>497</v>
       </c>
       <c r="D253" s="1" t="n">
         <v>8</v>
@@ -12696,7 +12702,7 @@
         <v>27</v>
       </c>
       <c r="I253" s="38" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="J253" s="44" t="n">
         <f aca="false">J252+D252</f>
@@ -12715,7 +12721,7 @@
         <v>6.5</v>
       </c>
       <c r="N253" s="1" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="O253" s="3" t="n">
         <v>3</v>
@@ -12729,10 +12735,10 @@
     </row>
     <row r="254" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B254" s="47" t="s">
-        <v>496</v>
+        <v>498</v>
       </c>
       <c r="C254" s="3" t="s">
-        <v>497</v>
+        <v>499</v>
       </c>
       <c r="D254" s="1" t="n">
         <v>8</v>
@@ -12748,7 +12754,7 @@
         <v>27</v>
       </c>
       <c r="I254" s="38" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="J254" s="44" t="n">
         <f aca="false">J253+D253</f>
@@ -12767,7 +12773,7 @@
         <v>6.75</v>
       </c>
       <c r="N254" s="1" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="O254" s="3" t="n">
         <v>3</v>
@@ -12781,10 +12787,10 @@
     </row>
     <row r="255" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B255" s="47" t="s">
-        <v>498</v>
+        <v>500</v>
       </c>
       <c r="C255" s="3" t="s">
-        <v>498</v>
+        <v>500</v>
       </c>
       <c r="D255" s="1" t="n">
         <v>8</v>
@@ -12800,7 +12806,7 @@
         <v>27</v>
       </c>
       <c r="I255" s="38" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="J255" s="44" t="n">
         <f aca="false">J254+D254</f>
@@ -12819,7 +12825,7 @@
         <v>7</v>
       </c>
       <c r="N255" s="1" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="O255" s="3" t="n">
         <v>3</v>
@@ -12833,10 +12839,10 @@
     </row>
     <row r="256" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B256" s="47" t="s">
-        <v>499</v>
+        <v>501</v>
       </c>
       <c r="C256" s="3" t="s">
-        <v>499</v>
+        <v>501</v>
       </c>
       <c r="D256" s="1" t="n">
         <v>8</v>
@@ -12852,7 +12858,7 @@
         <v>27</v>
       </c>
       <c r="I256" s="38" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="J256" s="44" t="n">
         <f aca="false">J255+D255</f>
@@ -12871,7 +12877,7 @@
         <v>7.25</v>
       </c>
       <c r="N256" s="1" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="O256" s="3" t="n">
         <v>3</v>
@@ -12885,10 +12891,10 @@
     </row>
     <row r="257" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B257" s="47" t="s">
-        <v>500</v>
+        <v>502</v>
       </c>
       <c r="C257" s="3" t="s">
-        <v>500</v>
+        <v>502</v>
       </c>
       <c r="D257" s="1" t="n">
         <v>8</v>
@@ -12904,7 +12910,7 @@
         <v>27</v>
       </c>
       <c r="I257" s="38" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="J257" s="44" t="n">
         <f aca="false">J256+D256</f>
@@ -12923,7 +12929,7 @@
         <v>7.5</v>
       </c>
       <c r="N257" s="1" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="O257" s="3" t="n">
         <v>3</v>
@@ -12937,10 +12943,10 @@
     </row>
     <row r="258" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B258" s="47" t="s">
-        <v>501</v>
+        <v>503</v>
       </c>
       <c r="C258" s="3" t="s">
-        <v>501</v>
+        <v>503</v>
       </c>
       <c r="D258" s="1" t="n">
         <v>8</v>
@@ -12956,7 +12962,7 @@
         <v>27</v>
       </c>
       <c r="I258" s="38" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="J258" s="44" t="n">
         <f aca="false">J257+D257</f>
@@ -12975,7 +12981,7 @@
         <v>7.75</v>
       </c>
       <c r="N258" s="1" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="O258" s="3" t="n">
         <v>3</v>
@@ -12989,10 +12995,10 @@
     </row>
     <row r="259" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B259" s="47" t="s">
-        <v>502</v>
+        <v>504</v>
       </c>
       <c r="C259" s="3" t="s">
-        <v>502</v>
+        <v>504</v>
       </c>
       <c r="D259" s="1" t="n">
         <v>8</v>
@@ -13008,7 +13014,7 @@
         <v>27</v>
       </c>
       <c r="I259" s="38" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="J259" s="44" t="n">
         <f aca="false">J258+D258</f>
@@ -13027,7 +13033,7 @@
         <v>8</v>
       </c>
       <c r="N259" s="1" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="O259" s="3" t="n">
         <v>3</v>
@@ -13041,10 +13047,10 @@
     </row>
     <row r="260" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B260" s="47" t="s">
-        <v>503</v>
+        <v>505</v>
       </c>
       <c r="C260" s="3" t="s">
-        <v>504</v>
+        <v>506</v>
       </c>
       <c r="D260" s="1" t="n">
         <v>16</v>
@@ -13062,7 +13068,7 @@
         <v>27</v>
       </c>
       <c r="I260" s="38" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="J260" s="44" t="n">
         <f aca="false">J259+D259</f>
@@ -13081,7 +13087,7 @@
         <v>8.25</v>
       </c>
       <c r="N260" s="1" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="O260" s="3" t="n">
         <v>1</v>
@@ -13095,10 +13101,10 @@
     </row>
     <row r="261" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B261" s="47" t="s">
-        <v>505</v>
+        <v>507</v>
       </c>
       <c r="C261" s="3" t="s">
-        <v>506</v>
+        <v>508</v>
       </c>
       <c r="D261" s="1" t="n">
         <v>8</v>
@@ -13114,7 +13120,7 @@
         <v>27</v>
       </c>
       <c r="I261" s="38" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="J261" s="44" t="n">
         <f aca="false">J260+D260</f>
@@ -13133,7 +13139,7 @@
         <v>8.75</v>
       </c>
       <c r="N261" s="1" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="O261" s="3" t="n">
         <v>2</v>
@@ -13224,7 +13230,7 @@
       <selection pane="topLeft" activeCell="C33" activeCellId="0" sqref="C33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.09375" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.1015625" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="40" width="20.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="40" width="16.11"/>
@@ -13235,22 +13241,22 @@
     <row r="6" s="49" customFormat="true" ht="34.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B6" s="50"/>
       <c r="C6" s="50" t="s">
-        <v>507</v>
+        <v>509</v>
       </c>
       <c r="D6" s="50" t="s">
-        <v>508</v>
+        <v>510</v>
       </c>
       <c r="E6" s="50" t="s">
-        <v>509</v>
+        <v>511</v>
       </c>
       <c r="F6" s="50" t="s">
-        <v>510</v>
+        <v>512</v>
       </c>
       <c r="G6" s="50" t="s">
         <v>281</v>
       </c>
       <c r="H6" s="50" t="s">
-        <v>511</v>
+        <v>513</v>
       </c>
       <c r="I6" s="50"/>
     </row>
@@ -13620,10 +13626,10 @@
     </row>
     <row r="26" s="1" customFormat="true" ht="37.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="32" t="s">
-        <v>512</v>
+        <v>514</v>
       </c>
       <c r="C26" s="32" t="s">
-        <v>513</v>
+        <v>515</v>
       </c>
       <c r="D26" s="27" t="n">
         <v>16</v>
@@ -13672,10 +13678,10 @@
     </row>
     <row r="27" s="1" customFormat="true" ht="37.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="32" t="s">
-        <v>514</v>
+        <v>516</v>
       </c>
       <c r="C27" s="32" t="s">
-        <v>515</v>
+        <v>517</v>
       </c>
       <c r="D27" s="27" t="n">
         <v>32</v>
@@ -13722,16 +13728,16 @@
     </row>
     <row r="30" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="52" t="s">
-        <v>516</v>
+        <v>518</v>
       </c>
       <c r="C30" s="52" t="s">
-        <v>517</v>
+        <v>519</v>
       </c>
       <c r="D30" s="52" t="s">
-        <v>518</v>
+        <v>520</v>
       </c>
       <c r="E30" s="52" t="s">
-        <v>519</v>
+        <v>521</v>
       </c>
       <c r="F30" s="52"/>
     </row>

</xml_diff>

<commit_message>
Fix labels on timestamps
</commit_message>
<xml_diff>
--- a/genSpacecraft/DownlinkSpecLTM.xlsx
+++ b/genSpacecraft/DownlinkSpecLTM.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1406" uniqueCount="530">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1406" uniqueCount="529">
   <si>
     <t xml:space="preserve">//</t>
   </si>
@@ -1238,7 +1238,7 @@
     <t xml:space="preserve">Min Last Change Epoch</t>
   </si>
   <si>
-    <t xml:space="preserve">Last Reset Time</t>
+    <t xml:space="preserve">MinMax Reset Time</t>
   </si>
   <si>
     <t xml:space="preserve">minmaxResetEpoch</t>
@@ -1283,7 +1283,7 @@
     <t xml:space="preserve">Time Whole Orbit Data was collected</t>
   </si>
   <si>
-    <t xml:space="preserve">Reset</t>
+    <t xml:space="preserve">Data Capture Time</t>
   </si>
   <si>
     <t xml:space="preserve">WODTimestampReset</t>
@@ -1350,9 +1350,6 @@
   </si>
   <si>
     <t xml:space="preserve">sec</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reset Count</t>
   </si>
   <si>
     <t xml:space="preserve">uint16_t</t>
@@ -1988,8 +1985,8 @@
   </sheetPr>
   <dimension ref="A1:Q264"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D166" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P186" activeCellId="0" sqref="P186"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A156" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B175" activeCellId="0" sqref="B175"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10946,7 +10943,7 @@
     </row>
     <row r="213" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B213" s="31" t="s">
-        <v>443</v>
+        <v>420</v>
       </c>
       <c r="C213" s="32" t="s">
         <v>421</v>
@@ -10958,7 +10955,7 @@
         <v>26</v>
       </c>
       <c r="F213" s="23" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="G213" s="23" t="s">
         <v>422</v>
@@ -11000,7 +10997,7 @@
     </row>
     <row r="214" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B214" s="31" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C214" s="32" t="s">
         <v>425</v>
@@ -11017,7 +11014,7 @@
         <v>27</v>
       </c>
       <c r="I214" s="28" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="J214" s="4" t="n">
         <f aca="false">J213+D213</f>
@@ -11053,7 +11050,7 @@
         <v>28</v>
       </c>
       <c r="C215" s="32" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="D215" s="27" t="n">
         <v>8</v>
@@ -11136,7 +11133,7 @@
     </row>
     <row r="218" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A218" s="43" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="219" s="14" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11210,10 +11207,10 @@
         <v>133</v>
       </c>
       <c r="H220" s="38" t="s">
+        <v>448</v>
+      </c>
+      <c r="I220" s="38" t="s">
         <v>449</v>
-      </c>
-      <c r="I220" s="38" t="s">
-        <v>450</v>
       </c>
       <c r="J220" s="45" t="n">
         <v>0</v>
@@ -11231,7 +11228,7 @@
         <v>0</v>
       </c>
       <c r="N220" s="1" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="O220" s="3" t="n">
         <v>1</v>
@@ -11245,10 +11242,10 @@
     </row>
     <row r="221" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B221" s="44" t="s">
+        <v>451</v>
+      </c>
+      <c r="C221" s="38" t="s">
         <v>452</v>
-      </c>
-      <c r="C221" s="38" t="s">
-        <v>453</v>
       </c>
       <c r="D221" s="38" t="n">
         <v>32</v>
@@ -11261,10 +11258,10 @@
         <v>133</v>
       </c>
       <c r="H221" s="38" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="I221" s="38" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="J221" s="45" t="n">
         <f aca="false">J220+D220</f>
@@ -11283,7 +11280,7 @@
         <v>1</v>
       </c>
       <c r="N221" s="1" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="O221" s="3" t="n">
         <v>1</v>
@@ -11297,7 +11294,7 @@
     </row>
     <row r="222" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A222" s="1" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B222" s="44"/>
       <c r="C222" s="38"/>
@@ -11314,10 +11311,10 @@
     </row>
     <row r="223" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B223" s="44" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="C223" s="38" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D223" s="38" t="n">
         <v>1</v>
@@ -11327,13 +11324,13 @@
       </c>
       <c r="F223" s="38"/>
       <c r="G223" s="38" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="H223" s="38" t="s">
         <v>27</v>
       </c>
       <c r="I223" s="38" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="J223" s="45" t="n">
         <f aca="false">J221+D221</f>
@@ -11352,7 +11349,7 @@
         <v>2</v>
       </c>
       <c r="N223" s="1" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="O223" s="3" t="n">
         <v>1</v>
@@ -11366,10 +11363,10 @@
     </row>
     <row r="224" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B224" s="44" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="C224" s="38" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="D224" s="38" t="n">
         <v>5</v>
@@ -11383,7 +11380,7 @@
       </c>
       <c r="H224" s="38"/>
       <c r="I224" s="38" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="J224" s="45" t="n">
         <f aca="false">J223+D223</f>
@@ -11402,7 +11399,7 @@
         <v>2.03125</v>
       </c>
       <c r="N224" s="1" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="O224" s="3" t="n">
         <v>1</v>
@@ -11416,10 +11413,10 @@
     </row>
     <row r="225" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B225" s="44" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="C225" s="38" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="D225" s="38" t="n">
         <v>4</v>
@@ -11435,7 +11432,7 @@
         <v>27</v>
       </c>
       <c r="I225" s="38" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="J225" s="45" t="n">
         <f aca="false">J224+D224</f>
@@ -11454,7 +11451,7 @@
         <v>2.1875</v>
       </c>
       <c r="N225" s="1" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="O225" s="3" t="n">
         <v>1</v>
@@ -11468,10 +11465,10 @@
     </row>
     <row r="226" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B226" s="44" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="C226" s="38" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="D226" s="38" t="n">
         <v>5</v>
@@ -11487,7 +11484,7 @@
         <v>27</v>
       </c>
       <c r="I226" s="38" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="J226" s="45" t="n">
         <f aca="false">J225+D225</f>
@@ -11506,7 +11503,7 @@
         <v>2.3125</v>
       </c>
       <c r="N226" s="1" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="O226" s="3" t="n">
         <v>1</v>
@@ -11520,10 +11517,10 @@
     </row>
     <row r="227" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B227" s="44" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C227" s="38" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="D227" s="38" t="n">
         <v>6</v>
@@ -11539,7 +11536,7 @@
         <v>27</v>
       </c>
       <c r="I227" s="38" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="J227" s="45" t="n">
         <f aca="false">J226+D226</f>
@@ -11558,7 +11555,7 @@
         <v>2.46875</v>
       </c>
       <c r="N227" s="1" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="O227" s="3" t="n">
         <v>1</v>
@@ -11572,10 +11569,10 @@
     </row>
     <row r="228" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B228" s="44" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="C228" s="38" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="D228" s="38" t="n">
         <v>6</v>
@@ -11591,7 +11588,7 @@
         <v>27</v>
       </c>
       <c r="I228" s="38" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="J228" s="45" t="n">
         <f aca="false">J227+D227</f>
@@ -11610,7 +11607,7 @@
         <v>2.65625</v>
       </c>
       <c r="N228" s="1" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="O228" s="3" t="n">
         <v>1</v>
@@ -11624,10 +11621,10 @@
     </row>
     <row r="229" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B229" s="44" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="C229" s="38" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="D229" s="38" t="n">
         <v>5</v>
@@ -11643,7 +11640,7 @@
         <v>27</v>
       </c>
       <c r="I229" s="38" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="J229" s="45" t="n">
         <f aca="false">J228+D228</f>
@@ -11662,7 +11659,7 @@
         <v>2.84375</v>
       </c>
       <c r="N229" s="1" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="O229" s="3" t="n">
         <v>1</v>
@@ -11676,7 +11673,7 @@
     </row>
     <row r="230" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A230" s="1" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B230" s="44"/>
       <c r="C230" s="38"/>
@@ -11693,10 +11690,10 @@
     </row>
     <row r="231" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B231" s="44" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="C231" s="38" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="D231" s="38" t="n">
         <v>8</v>
@@ -11712,7 +11709,7 @@
         <v>71</v>
       </c>
       <c r="I231" s="38" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="J231" s="45" t="n">
         <f aca="false">J229+D229</f>
@@ -11731,7 +11728,7 @@
         <v>3</v>
       </c>
       <c r="N231" s="1" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="O231" s="3" t="n">
         <v>1</v>
@@ -11745,10 +11742,10 @@
     </row>
     <row r="232" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B232" s="44" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="C232" s="38" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="D232" s="38" t="n">
         <v>8</v>
@@ -11764,7 +11761,7 @@
         <v>71</v>
       </c>
       <c r="I232" s="38" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="J232" s="45" t="n">
         <f aca="false">J231+D231</f>
@@ -11783,7 +11780,7 @@
         <v>3.25</v>
       </c>
       <c r="N232" s="1" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="O232" s="3" t="n">
         <v>1</v>
@@ -11797,10 +11794,10 @@
     </row>
     <row r="233" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B233" s="44" t="s">
+        <v>468</v>
+      </c>
+      <c r="C233" s="38" t="s">
         <v>469</v>
-      </c>
-      <c r="C233" s="38" t="s">
-        <v>470</v>
       </c>
       <c r="D233" s="38" t="n">
         <v>16</v>
@@ -11816,7 +11813,7 @@
         <v>27</v>
       </c>
       <c r="I233" s="38" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="J233" s="45" t="n">
         <f aca="false">J232+D232</f>
@@ -11879,7 +11876,7 @@
     </row>
     <row r="235" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A235" s="43" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="F235" s="38"/>
       <c r="G235" s="38"/>
@@ -11963,10 +11960,10 @@
     </row>
     <row r="238" s="48" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B238" s="21" t="s">
+        <v>471</v>
+      </c>
+      <c r="C238" s="46" t="s">
         <v>472</v>
-      </c>
-      <c r="C238" s="46" t="s">
-        <v>473</v>
       </c>
       <c r="D238" s="1" t="n">
         <v>5</v>
@@ -11982,7 +11979,7 @@
         <v>27</v>
       </c>
       <c r="I238" s="38" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="J238" s="45" t="n">
         <f aca="false">J234</f>
@@ -12015,10 +12012,10 @@
     </row>
     <row r="239" s="48" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B239" s="21" t="s">
+        <v>473</v>
+      </c>
+      <c r="C239" s="46" t="s">
         <v>474</v>
-      </c>
-      <c r="C239" s="46" t="s">
-        <v>475</v>
       </c>
       <c r="D239" s="1" t="n">
         <v>1</v>
@@ -12028,13 +12025,13 @@
       </c>
       <c r="F239" s="47"/>
       <c r="G239" s="38" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="H239" s="38" t="s">
         <v>27</v>
       </c>
       <c r="I239" s="38" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="J239" s="45" t="n">
         <f aca="false">J238+D238</f>
@@ -12053,7 +12050,7 @@
         <v>4.15625</v>
       </c>
       <c r="N239" s="1" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="O239" s="3" t="n">
         <v>1</v>
@@ -12067,10 +12064,10 @@
     </row>
     <row r="240" s="48" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B240" s="21" t="s">
+        <v>475</v>
+      </c>
+      <c r="C240" s="46" t="s">
         <v>476</v>
-      </c>
-      <c r="C240" s="46" t="s">
-        <v>477</v>
       </c>
       <c r="D240" s="1" t="n">
         <v>1</v>
@@ -12080,13 +12077,13 @@
       </c>
       <c r="F240" s="47"/>
       <c r="G240" s="38" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="H240" s="38" t="s">
         <v>27</v>
       </c>
       <c r="I240" s="38" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="J240" s="45" t="n">
         <f aca="false">J239+D239</f>
@@ -12105,7 +12102,7 @@
         <v>4.1875</v>
       </c>
       <c r="N240" s="1" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="O240" s="3" t="n">
         <v>2</v>
@@ -12119,10 +12116,10 @@
     </row>
     <row r="241" s="48" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B241" s="21" t="s">
+        <v>478</v>
+      </c>
+      <c r="C241" s="46" t="s">
         <v>479</v>
-      </c>
-      <c r="C241" s="46" t="s">
-        <v>480</v>
       </c>
       <c r="D241" s="1" t="n">
         <v>3</v>
@@ -12138,7 +12135,7 @@
         <v>27</v>
       </c>
       <c r="I241" s="38" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="J241" s="45" t="n">
         <f aca="false">J240+D240</f>
@@ -12157,7 +12154,7 @@
         <v>4.21875</v>
       </c>
       <c r="N241" s="1" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="O241" s="3" t="n">
         <v>2</v>
@@ -12171,10 +12168,10 @@
     </row>
     <row r="242" s="48" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B242" s="21" t="s">
+        <v>480</v>
+      </c>
+      <c r="C242" s="46" t="s">
         <v>481</v>
-      </c>
-      <c r="C242" s="46" t="s">
-        <v>482</v>
       </c>
       <c r="D242" s="1" t="n">
         <v>4</v>
@@ -12184,13 +12181,13 @@
       </c>
       <c r="F242" s="47"/>
       <c r="G242" s="38" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="H242" s="38" t="s">
         <v>27</v>
       </c>
       <c r="I242" s="38" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="J242" s="45" t="n">
         <f aca="false">J241+D241</f>
@@ -12209,7 +12206,7 @@
         <v>4.3125</v>
       </c>
       <c r="N242" s="1" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="O242" s="3" t="n">
         <v>2</v>
@@ -12223,10 +12220,10 @@
     </row>
     <row r="243" s="48" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B243" s="21" t="s">
+        <v>483</v>
+      </c>
+      <c r="C243" s="46" t="s">
         <v>484</v>
-      </c>
-      <c r="C243" s="46" t="s">
-        <v>485</v>
       </c>
       <c r="D243" s="1" t="n">
         <v>4</v>
@@ -12236,13 +12233,13 @@
       </c>
       <c r="F243" s="47"/>
       <c r="G243" s="38" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="H243" s="38" t="s">
         <v>27</v>
       </c>
       <c r="I243" s="38" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="J243" s="45" t="n">
         <f aca="false">J242+D242</f>
@@ -12261,7 +12258,7 @@
         <v>4.4375</v>
       </c>
       <c r="N243" s="1" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="O243" s="3" t="n">
         <v>2</v>
@@ -12275,10 +12272,10 @@
     </row>
     <row r="244" s="48" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B244" s="21" t="s">
+        <v>485</v>
+      </c>
+      <c r="C244" s="46" t="s">
         <v>486</v>
-      </c>
-      <c r="C244" s="46" t="s">
-        <v>487</v>
       </c>
       <c r="D244" s="1" t="n">
         <v>5</v>
@@ -12288,13 +12285,13 @@
       </c>
       <c r="F244" s="47"/>
       <c r="G244" s="38" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="H244" s="38" t="s">
         <v>27</v>
       </c>
       <c r="I244" s="38" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="J244" s="45" t="n">
         <f aca="false">J243+D243</f>
@@ -12313,7 +12310,7 @@
         <v>4.5625</v>
       </c>
       <c r="N244" s="1" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="O244" s="3" t="n">
         <v>2</v>
@@ -12327,10 +12324,10 @@
     </row>
     <row r="245" s="48" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B245" s="21" t="s">
+        <v>488</v>
+      </c>
+      <c r="C245" s="46" t="s">
         <v>489</v>
-      </c>
-      <c r="C245" s="46" t="s">
-        <v>490</v>
       </c>
       <c r="D245" s="1" t="n">
         <v>9</v>
@@ -12346,7 +12343,7 @@
         <v>27</v>
       </c>
       <c r="I245" s="38" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="J245" s="45" t="n">
         <f aca="false">J244+D244</f>
@@ -12365,7 +12362,7 @@
         <v>4.71875</v>
       </c>
       <c r="N245" s="1" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="O245" s="3" t="n">
         <v>2</v>
@@ -12398,10 +12395,10 @@
     </row>
     <row r="247" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B247" s="48" t="s">
+        <v>490</v>
+      </c>
+      <c r="C247" s="3" t="s">
         <v>491</v>
-      </c>
-      <c r="C247" s="3" t="s">
-        <v>492</v>
       </c>
       <c r="D247" s="1" t="n">
         <v>8</v>
@@ -12417,7 +12414,7 @@
         <v>27</v>
       </c>
       <c r="I247" s="38" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="J247" s="45" t="n">
         <f aca="false">J245+D245</f>
@@ -12436,7 +12433,7 @@
         <v>5</v>
       </c>
       <c r="N247" s="1" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="O247" s="3" t="n">
         <v>3</v>
@@ -12450,10 +12447,10 @@
     </row>
     <row r="248" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B248" s="48" t="s">
+        <v>493</v>
+      </c>
+      <c r="C248" s="3" t="s">
         <v>494</v>
-      </c>
-      <c r="C248" s="3" t="s">
-        <v>495</v>
       </c>
       <c r="D248" s="1" t="n">
         <v>8</v>
@@ -12469,7 +12466,7 @@
         <v>27</v>
       </c>
       <c r="I248" s="38" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="J248" s="45" t="n">
         <f aca="false">J247+D247</f>
@@ -12488,7 +12485,7 @@
         <v>5.25</v>
       </c>
       <c r="N248" s="1" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="O248" s="3" t="n">
         <v>3</v>
@@ -12502,10 +12499,10 @@
     </row>
     <row r="249" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B249" s="48" t="s">
+        <v>495</v>
+      </c>
+      <c r="C249" s="3" t="s">
         <v>496</v>
-      </c>
-      <c r="C249" s="3" t="s">
-        <v>497</v>
       </c>
       <c r="D249" s="1" t="n">
         <v>8</v>
@@ -12521,7 +12518,7 @@
         <v>27</v>
       </c>
       <c r="I249" s="38" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="J249" s="45" t="n">
         <f aca="false">J248+D248</f>
@@ -12540,7 +12537,7 @@
         <v>5.5</v>
       </c>
       <c r="N249" s="1" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="O249" s="3" t="n">
         <v>3</v>
@@ -12554,10 +12551,10 @@
     </row>
     <row r="250" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B250" s="48" t="s">
+        <v>497</v>
+      </c>
+      <c r="C250" s="3" t="s">
         <v>498</v>
-      </c>
-      <c r="C250" s="3" t="s">
-        <v>499</v>
       </c>
       <c r="D250" s="1" t="n">
         <v>8</v>
@@ -12573,7 +12570,7 @@
         <v>27</v>
       </c>
       <c r="I250" s="38" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="J250" s="45" t="n">
         <f aca="false">J249+D249</f>
@@ -12592,7 +12589,7 @@
         <v>5.75</v>
       </c>
       <c r="N250" s="1" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="O250" s="3" t="n">
         <v>3</v>
@@ -12606,10 +12603,10 @@
     </row>
     <row r="251" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B251" s="48" t="s">
+        <v>499</v>
+      </c>
+      <c r="C251" s="3" t="s">
         <v>500</v>
-      </c>
-      <c r="C251" s="3" t="s">
-        <v>501</v>
       </c>
       <c r="D251" s="1" t="n">
         <v>8</v>
@@ -12625,7 +12622,7 @@
         <v>27</v>
       </c>
       <c r="I251" s="38" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="J251" s="45" t="n">
         <f aca="false">J250+D250</f>
@@ -12644,7 +12641,7 @@
         <v>6</v>
       </c>
       <c r="N251" s="1" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="O251" s="3" t="n">
         <v>3</v>
@@ -12658,10 +12655,10 @@
     </row>
     <row r="252" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B252" s="48" t="s">
+        <v>501</v>
+      </c>
+      <c r="C252" s="3" t="s">
         <v>502</v>
-      </c>
-      <c r="C252" s="3" t="s">
-        <v>503</v>
       </c>
       <c r="D252" s="1" t="n">
         <v>8</v>
@@ -12677,7 +12674,7 @@
         <v>27</v>
       </c>
       <c r="I252" s="38" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="J252" s="45" t="n">
         <f aca="false">J251+D251</f>
@@ -12696,7 +12693,7 @@
         <v>6.25</v>
       </c>
       <c r="N252" s="1" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="O252" s="3" t="n">
         <v>3</v>
@@ -12710,10 +12707,10 @@
     </row>
     <row r="253" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B253" s="48" t="s">
+        <v>503</v>
+      </c>
+      <c r="C253" s="3" t="s">
         <v>504</v>
-      </c>
-      <c r="C253" s="3" t="s">
-        <v>505</v>
       </c>
       <c r="D253" s="1" t="n">
         <v>8</v>
@@ -12729,7 +12726,7 @@
         <v>27</v>
       </c>
       <c r="I253" s="38" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="J253" s="45" t="n">
         <f aca="false">J252+D252</f>
@@ -12748,7 +12745,7 @@
         <v>6.5</v>
       </c>
       <c r="N253" s="1" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="O253" s="3" t="n">
         <v>3</v>
@@ -12762,10 +12759,10 @@
     </row>
     <row r="254" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B254" s="48" t="s">
+        <v>505</v>
+      </c>
+      <c r="C254" s="3" t="s">
         <v>506</v>
-      </c>
-      <c r="C254" s="3" t="s">
-        <v>507</v>
       </c>
       <c r="D254" s="1" t="n">
         <v>8</v>
@@ -12781,7 +12778,7 @@
         <v>27</v>
       </c>
       <c r="I254" s="38" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="J254" s="45" t="n">
         <f aca="false">J253+D253</f>
@@ -12800,7 +12797,7 @@
         <v>6.75</v>
       </c>
       <c r="N254" s="1" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="O254" s="3" t="n">
         <v>3</v>
@@ -12814,10 +12811,10 @@
     </row>
     <row r="255" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B255" s="48" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="C255" s="3" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="D255" s="1" t="n">
         <v>8</v>
@@ -12833,7 +12830,7 @@
         <v>27</v>
       </c>
       <c r="I255" s="38" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="J255" s="45" t="n">
         <f aca="false">J254+D254</f>
@@ -12852,7 +12849,7 @@
         <v>7</v>
       </c>
       <c r="N255" s="1" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="O255" s="3" t="n">
         <v>3</v>
@@ -12866,10 +12863,10 @@
     </row>
     <row r="256" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B256" s="48" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="C256" s="3" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="D256" s="1" t="n">
         <v>8</v>
@@ -12885,7 +12882,7 @@
         <v>27</v>
       </c>
       <c r="I256" s="38" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="J256" s="45" t="n">
         <f aca="false">J255+D255</f>
@@ -12904,7 +12901,7 @@
         <v>7.25</v>
       </c>
       <c r="N256" s="1" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="O256" s="3" t="n">
         <v>3</v>
@@ -12918,10 +12915,10 @@
     </row>
     <row r="257" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B257" s="48" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C257" s="3" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="D257" s="1" t="n">
         <v>8</v>
@@ -12937,7 +12934,7 @@
         <v>27</v>
       </c>
       <c r="I257" s="38" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="J257" s="45" t="n">
         <f aca="false">J256+D256</f>
@@ -12956,7 +12953,7 @@
         <v>7.5</v>
       </c>
       <c r="N257" s="1" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="O257" s="3" t="n">
         <v>3</v>
@@ -12970,10 +12967,10 @@
     </row>
     <row r="258" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B258" s="48" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="C258" s="3" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D258" s="1" t="n">
         <v>8</v>
@@ -12989,7 +12986,7 @@
         <v>27</v>
       </c>
       <c r="I258" s="38" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="J258" s="45" t="n">
         <f aca="false">J257+D257</f>
@@ -13008,7 +13005,7 @@
         <v>7.75</v>
       </c>
       <c r="N258" s="1" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="O258" s="3" t="n">
         <v>3</v>
@@ -13022,10 +13019,10 @@
     </row>
     <row r="259" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B259" s="48" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="C259" s="3" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="D259" s="1" t="n">
         <v>8</v>
@@ -13041,7 +13038,7 @@
         <v>27</v>
       </c>
       <c r="I259" s="38" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="J259" s="45" t="n">
         <f aca="false">J258+D258</f>
@@ -13060,7 +13057,7 @@
         <v>8</v>
       </c>
       <c r="N259" s="1" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="O259" s="3" t="n">
         <v>3</v>
@@ -13074,10 +13071,10 @@
     </row>
     <row r="260" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B260" s="48" t="s">
+        <v>512</v>
+      </c>
+      <c r="C260" s="3" t="s">
         <v>513</v>
-      </c>
-      <c r="C260" s="3" t="s">
-        <v>514</v>
       </c>
       <c r="D260" s="1" t="n">
         <v>16</v>
@@ -13095,7 +13092,7 @@
         <v>27</v>
       </c>
       <c r="I260" s="38" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="J260" s="45" t="n">
         <f aca="false">J259+D259</f>
@@ -13114,7 +13111,7 @@
         <v>8.25</v>
       </c>
       <c r="N260" s="1" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="O260" s="3" t="n">
         <v>1</v>
@@ -13128,10 +13125,10 @@
     </row>
     <row r="261" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B261" s="48" t="s">
+        <v>514</v>
+      </c>
+      <c r="C261" s="3" t="s">
         <v>515</v>
-      </c>
-      <c r="C261" s="3" t="s">
-        <v>516</v>
       </c>
       <c r="D261" s="1" t="n">
         <v>8</v>
@@ -13147,7 +13144,7 @@
         <v>27</v>
       </c>
       <c r="I261" s="38" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="J261" s="45" t="n">
         <f aca="false">J260+D260</f>
@@ -13166,7 +13163,7 @@
         <v>8.75</v>
       </c>
       <c r="N261" s="1" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="O261" s="3" t="n">
         <v>2</v>
@@ -13269,22 +13266,22 @@
     <row r="6" s="51" customFormat="true" ht="34.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B6" s="52"/>
       <c r="C6" s="52" t="s">
+        <v>516</v>
+      </c>
+      <c r="D6" s="52" t="s">
         <v>517</v>
       </c>
-      <c r="D6" s="52" t="s">
+      <c r="E6" s="52" t="s">
         <v>518</v>
       </c>
-      <c r="E6" s="52" t="s">
+      <c r="F6" s="52" t="s">
         <v>519</v>
-      </c>
-      <c r="F6" s="52" t="s">
-        <v>520</v>
       </c>
       <c r="G6" s="52" t="s">
         <v>282</v>
       </c>
       <c r="H6" s="52" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="I6" s="52"/>
     </row>
@@ -13654,10 +13651,10 @@
     </row>
     <row r="26" s="1" customFormat="true" ht="37.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="32" t="s">
+        <v>521</v>
+      </c>
+      <c r="C26" s="32" t="s">
         <v>522</v>
-      </c>
-      <c r="C26" s="32" t="s">
-        <v>523</v>
       </c>
       <c r="D26" s="27" t="n">
         <v>16</v>
@@ -13706,10 +13703,10 @@
     </row>
     <row r="27" s="1" customFormat="true" ht="37.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="32" t="s">
+        <v>523</v>
+      </c>
+      <c r="C27" s="32" t="s">
         <v>524</v>
-      </c>
-      <c r="C27" s="32" t="s">
-        <v>525</v>
       </c>
       <c r="D27" s="27" t="n">
         <v>32</v>
@@ -13756,16 +13753,16 @@
     </row>
     <row r="30" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="50" t="s">
+        <v>525</v>
+      </c>
+      <c r="C30" s="50" t="s">
         <v>526</v>
       </c>
-      <c r="C30" s="50" t="s">
+      <c r="D30" s="50" t="s">
         <v>527</v>
       </c>
-      <c r="D30" s="50" t="s">
+      <c r="E30" s="50" t="s">
         <v>528</v>
-      </c>
-      <c r="E30" s="50" t="s">
-        <v>529</v>
       </c>
       <c r="F30" s="50"/>
     </row>

</xml_diff>

<commit_message>
The last of the power (fwd and rflt) and RSSI changes based on Eric measurements
</commit_message>
<xml_diff>
--- a/genSpacecraft/DownlinkSpecLTM.xlsx
+++ b/genSpacecraft/DownlinkSpecLTM.xlsx
@@ -215,7 +215,7 @@
     <t xml:space="preserve">ReflectedPwr</t>
   </si>
   <si>
-    <t xml:space="preserve">icr_8bit_volts|tx_ref_pwr|dBm_to_mW</t>
+    <t xml:space="preserve">icr_8bit_volts|txv2_ref_pwr</t>
   </si>
   <si>
     <t xml:space="preserve">mW</t>
@@ -476,7 +476,7 @@
     <t xml:space="preserve">FwdPower</t>
   </si>
   <si>
-    <t xml:space="preserve">icr_8bit_volts|tx_pwr1|dBm_to_mW</t>
+    <t xml:space="preserve">icr_8bit_volts|txv2_fwd_pwr|dBm_to_mW</t>
   </si>
   <si>
     <t xml:space="preserve">Receiver card temperature</t>
@@ -488,7 +488,7 @@
     <t xml:space="preserve">rssi</t>
   </si>
   <si>
-    <t xml:space="preserve">icr_8bit_volts|icr_rssi </t>
+    <t xml:space="preserve">icr_8bit_volts|icrv2_rssi </t>
   </si>
   <si>
     <t xml:space="preserve">dBm</t>
@@ -1985,8 +1985,8 @@
   </sheetPr>
   <dimension ref="A1:Q264"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A156" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B175" activeCellId="0" sqref="B175"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G50" activeCellId="0" sqref="G50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4043,7 +4043,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="37.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="31" t="s">
         <v>153</v>
       </c>

</xml_diff>

<commit_message>
A few tweaks with names and labels
</commit_message>
<xml_diff>
--- a/genSpacecraft/DownlinkSpecLTM.xlsx
+++ b/genSpacecraft/DownlinkSpecLTM.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1450" uniqueCount="545">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1452" uniqueCount="545">
   <si>
     <t xml:space="preserve">//</t>
   </si>
@@ -227,7 +227,7 @@
     <t xml:space="preserve">AMSAT Radio</t>
   </si>
   <si>
-    <t xml:space="preserve">3V Prot</t>
+    <t xml:space="preserve">3.3V Prot</t>
   </si>
   <si>
     <t xml:space="preserve">ICR3VProt</t>
@@ -674,7 +674,7 @@
     <t xml:space="preserve">Interior Temp</t>
   </si>
   <si>
-    <t xml:space="preserve">Bck Btm Left Temp</t>
+    <t xml:space="preserve">BckBtmLft Temp</t>
   </si>
   <si>
     <t xml:space="preserve">hostI2cTemp1</t>
@@ -683,25 +683,25 @@
     <t xml:space="preserve">Other MESat Telemetry</t>
   </si>
   <si>
-    <t xml:space="preserve">Front Center Temp</t>
+    <t xml:space="preserve">Front Ctr Temp</t>
   </si>
   <si>
     <t xml:space="preserve">hostI2cTemp2</t>
   </si>
   <si>
-    <t xml:space="preserve">Bck Top Left Temp</t>
+    <t xml:space="preserve">BckTopLft Temp</t>
   </si>
   <si>
     <t xml:space="preserve">hostI2cTemp3</t>
   </si>
   <si>
-    <t xml:space="preserve">Frnt Btm Left Temp</t>
+    <t xml:space="preserve">FrontBtmLft Temp</t>
   </si>
   <si>
     <t xml:space="preserve">hostI2cTemp4</t>
   </si>
   <si>
-    <t xml:space="preserve">Bck Top Right Temp</t>
+    <t xml:space="preserve">BckTopRgt Temp</t>
   </si>
   <si>
     <t xml:space="preserve">hostI2cTemp5</t>
@@ -2033,8 +2033,8 @@
   </sheetPr>
   <dimension ref="A1:Q1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A26" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H46" activeCellId="0" sqref="H46"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A60" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B77" activeCellId="0" sqref="B77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4640,7 +4640,9 @@
       <c r="G61" s="22" t="s">
         <v>133</v>
       </c>
-      <c r="H61" s="22"/>
+      <c r="H61" s="22" t="s">
+        <v>71</v>
+      </c>
       <c r="I61" s="32" t="s">
         <v>181</v>
       </c>
@@ -4690,7 +4692,9 @@
       <c r="G62" s="22" t="s">
         <v>133</v>
       </c>
-      <c r="H62" s="22"/>
+      <c r="H62" s="22" t="s">
+        <v>71</v>
+      </c>
       <c r="I62" s="32" t="s">
         <v>183</v>
       </c>

</xml_diff>

<commit_message>
A few final updates for MESAT1
</commit_message>
<xml_diff>
--- a/genSpacecraft/DownlinkSpecLTM.xlsx
+++ b/genSpacecraft/DownlinkSpecLTM.xlsx
@@ -1019,7 +1019,7 @@
     <t xml:space="preserve">hostBits20</t>
   </si>
   <si>
-    <t xml:space="preserve">spareField0</t>
+    <t xml:space="preserve">Batt Heartbeat</t>
   </si>
   <si>
     <t xml:space="preserve">hostBits21</t>
@@ -2042,8 +2042,8 @@
   </sheetPr>
   <dimension ref="A1:Q1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F49" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G67" activeCellId="0" sqref="G67"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F102" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P126" activeCellId="0" sqref="P126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7780,7 +7780,7 @@
       </c>
       <c r="F126" s="23"/>
       <c r="G126" s="22" t="s">
-        <v>296</v>
+        <v>267</v>
       </c>
       <c r="H126" s="22" t="s">
         <v>27</v>
@@ -7803,13 +7803,13 @@
         <v>17.65625</v>
       </c>
       <c r="N126" s="1" t="s">
-        <v>28</v>
+        <v>118</v>
       </c>
       <c r="O126" s="24" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="P126" s="1" t="n">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="Q126" s="1" t="n">
         <v>0</v>
@@ -7853,13 +7853,13 @@
         <v>17.6875</v>
       </c>
       <c r="N127" s="1" t="s">
-        <v>28</v>
+        <v>221</v>
       </c>
       <c r="O127" s="24" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="P127" s="1" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="Q127" s="1" t="n">
         <v>0</v>
@@ -8190,9 +8190,18 @@
         <f aca="false">J133+D133</f>
         <v>573</v>
       </c>
-      <c r="K134" s="28"/>
-      <c r="L134" s="28"/>
-      <c r="M134" s="28"/>
+      <c r="K134" s="28" t="n">
+        <f aca="false">J134/8</f>
+        <v>71.625</v>
+      </c>
+      <c r="L134" s="28" t="n">
+        <f aca="false">J134/16</f>
+        <v>35.8125</v>
+      </c>
+      <c r="M134" s="28" t="n">
+        <f aca="false">J134/32</f>
+        <v>17.90625</v>
+      </c>
       <c r="N134" s="1" t="s">
         <v>118</v>
       </c>
@@ -8231,17 +8240,26 @@
         <f aca="false">J134+D134</f>
         <v>574</v>
       </c>
-      <c r="K135" s="28"/>
-      <c r="L135" s="28"/>
-      <c r="M135" s="28"/>
+      <c r="K135" s="28" t="n">
+        <f aca="false">J135/8</f>
+        <v>71.75</v>
+      </c>
+      <c r="L135" s="28" t="n">
+        <f aca="false">J135/16</f>
+        <v>35.875</v>
+      </c>
+      <c r="M135" s="28" t="n">
+        <f aca="false">J135/32</f>
+        <v>17.9375</v>
+      </c>
       <c r="N135" s="1" t="s">
-        <v>28</v>
+        <v>135</v>
       </c>
       <c r="O135" s="24" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="P135" s="1" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="Q135" s="1" t="n">
         <v>0</v>
@@ -8272,17 +8290,26 @@
         <f aca="false">J135+D135</f>
         <v>575</v>
       </c>
-      <c r="K136" s="28"/>
-      <c r="L136" s="28"/>
-      <c r="M136" s="28"/>
+      <c r="K136" s="28" t="n">
+        <f aca="false">J136/8</f>
+        <v>71.875</v>
+      </c>
+      <c r="L136" s="28" t="n">
+        <f aca="false">J136/16</f>
+        <v>35.9375</v>
+      </c>
+      <c r="M136" s="28" t="n">
+        <f aca="false">J136/32</f>
+        <v>17.96875</v>
+      </c>
       <c r="N136" s="1" t="s">
-        <v>28</v>
+        <v>293</v>
       </c>
       <c r="O136" s="24" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="P136" s="1" t="n">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="Q136" s="1" t="n">
         <v>0</v>

</xml_diff>